<commit_message>
corregí los errores que envió Paola
</commit_message>
<xml_diff>
--- a/Versión Página web. Calendario Academico UR 2021. V. 17-11-2020 CAMBIOS.xlsx
+++ b/Versión Página web. Calendario Academico UR 2021. V. 17-11-2020 CAMBIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_33946041C23A0D7F2B53E0C4FFB685BA09870FAE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{640389F9-EF47-451F-9A39-377143ACBA6C}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_33946041C23A0D7F2B53E0C4FFB685BA09870FAE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{640389F9-EF47-451F-9A39-377143ACBA6C}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 " sheetId="4" state="hidden" r:id="rId1"/>
@@ -3958,29 +3958,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4012,57 +4000,6 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4072,31 +4009,253 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4105,10 +4264,10 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4153,217 +4312,58 @@
     <xf numFmtId="164" fontId="7" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4680,63 +4680,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="243" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="243"/>
+      <c r="I1" s="243"/>
     </row>
     <row r="2" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="198"/>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
+      <c r="A2" s="321"/>
+      <c r="B2" s="321"/>
+      <c r="C2" s="321"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
+      <c r="F2" s="321"/>
+      <c r="G2" s="321"/>
+      <c r="H2" s="321"/>
+      <c r="I2" s="321"/>
     </row>
     <row r="3" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="243" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
-      <c r="I3" s="197"/>
+      <c r="B3" s="243"/>
+      <c r="C3" s="243"/>
+      <c r="D3" s="243"/>
+      <c r="E3" s="243"/>
+      <c r="F3" s="243"/>
+      <c r="G3" s="243"/>
+      <c r="H3" s="243"/>
+      <c r="I3" s="243"/>
     </row>
     <row r="4" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="199" t="s">
+      <c r="A4" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="201" t="s">
+      <c r="B4" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="203"/>
-      <c r="E4" s="204" t="s">
+      <c r="C4" s="198"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="205"/>
-      <c r="G4" s="206" t="s">
+      <c r="F4" s="201"/>
+      <c r="G4" s="202" t="s">
         <v>163</v>
       </c>
-      <c r="H4" s="207"/>
-      <c r="I4" s="208"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="204"/>
     </row>
     <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="200"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="48" t="s">
         <v>113</v>
       </c>
@@ -4822,63 +4822,63 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="209" t="s">
+      <c r="A9" s="194" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="209"/>
-      <c r="C9" s="209"/>
-      <c r="D9" s="209"/>
-      <c r="E9" s="209"/>
-      <c r="F9" s="209"/>
-      <c r="G9" s="209"/>
-      <c r="H9" s="209"/>
-      <c r="I9" s="209"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="194"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="220"/>
-      <c r="B10" s="220"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="220"/>
-      <c r="I10" s="220"/>
+      <c r="A10" s="310"/>
+      <c r="B10" s="310"/>
+      <c r="C10" s="310"/>
+      <c r="D10" s="310"/>
+      <c r="E10" s="310"/>
+      <c r="F10" s="310"/>
+      <c r="G10" s="310"/>
+      <c r="H10" s="310"/>
+      <c r="I10" s="310"/>
     </row>
     <row r="11" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="197"/>
-      <c r="C11" s="197"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
+      <c r="B11" s="243"/>
+      <c r="C11" s="243"/>
+      <c r="D11" s="243"/>
+      <c r="E11" s="243"/>
+      <c r="F11" s="243"/>
+      <c r="G11" s="243"/>
+      <c r="H11" s="243"/>
+      <c r="I11" s="243"/>
     </row>
     <row r="12" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="199" t="s">
+      <c r="A12" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="201" t="s">
+      <c r="B12" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="202"/>
-      <c r="D12" s="203"/>
-      <c r="E12" s="204" t="s">
+      <c r="C12" s="198"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="205"/>
-      <c r="G12" s="206" t="s">
+      <c r="F12" s="201"/>
+      <c r="G12" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="207"/>
-      <c r="I12" s="208"/>
+      <c r="H12" s="203"/>
+      <c r="I12" s="204"/>
     </row>
     <row r="13" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="200"/>
+      <c r="A13" s="196"/>
       <c r="B13" s="48" t="s">
         <v>113</v>
       </c>
@@ -4978,33 +4978,33 @@
       <c r="A18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="191">
+      <c r="B18" s="212">
         <v>43794</v>
       </c>
-      <c r="C18" s="192"/>
-      <c r="D18" s="193"/>
-      <c r="E18" s="191">
+      <c r="C18" s="213"/>
+      <c r="D18" s="214"/>
+      <c r="E18" s="212">
         <v>43924</v>
       </c>
-      <c r="F18" s="193"/>
-      <c r="G18" s="210">
+      <c r="F18" s="214"/>
+      <c r="G18" s="191">
         <v>43974</v>
       </c>
-      <c r="H18" s="211"/>
-      <c r="I18" s="212"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="192"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="209" t="s">
+      <c r="A19" s="194" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="209"/>
-      <c r="C19" s="209"/>
-      <c r="D19" s="209"/>
-      <c r="E19" s="209"/>
-      <c r="F19" s="209"/>
-      <c r="G19" s="209"/>
-      <c r="H19" s="209"/>
-      <c r="I19" s="209"/>
+      <c r="B19" s="194"/>
+      <c r="C19" s="194"/>
+      <c r="D19" s="194"/>
+      <c r="E19" s="194"/>
+      <c r="F19" s="194"/>
+      <c r="G19" s="194"/>
+      <c r="H19" s="194"/>
+      <c r="I19" s="194"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
@@ -5018,63 +5018,63 @@
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="197" t="s">
+      <c r="A21" s="243" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="197"/>
-      <c r="C21" s="197"/>
-      <c r="D21" s="197"/>
-      <c r="E21" s="197"/>
-      <c r="F21" s="197"/>
-      <c r="G21" s="197"/>
-      <c r="H21" s="197"/>
-      <c r="I21" s="197"/>
+      <c r="B21" s="243"/>
+      <c r="C21" s="243"/>
+      <c r="D21" s="243"/>
+      <c r="E21" s="243"/>
+      <c r="F21" s="243"/>
+      <c r="G21" s="243"/>
+      <c r="H21" s="243"/>
+      <c r="I21" s="243"/>
     </row>
     <row r="22" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="213" t="s">
+      <c r="A22" s="322" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="201" t="s">
+      <c r="B22" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="202"/>
-      <c r="D22" s="203"/>
-      <c r="E22" s="216" t="s">
+      <c r="C22" s="198"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="325" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="217"/>
-      <c r="G22" s="206" t="s">
+      <c r="F22" s="326"/>
+      <c r="G22" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="207"/>
-      <c r="I22" s="208"/>
+      <c r="H22" s="203"/>
+      <c r="I22" s="204"/>
     </row>
     <row r="23" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="214"/>
-      <c r="B23" s="218" t="s">
+      <c r="A23" s="323"/>
+      <c r="B23" s="238" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="202" t="s">
+      <c r="C23" s="198" t="s">
         <v>184</v>
       </c>
-      <c r="D23" s="203"/>
+      <c r="D23" s="199"/>
       <c r="E23" s="119" t="s">
         <v>148</v>
       </c>
       <c r="F23" s="118" t="s">
         <v>112</v>
       </c>
-      <c r="G23" s="229" t="s">
+      <c r="G23" s="318" t="s">
         <v>185</v>
       </c>
-      <c r="H23" s="206" t="s">
+      <c r="H23" s="202" t="s">
         <v>184</v>
       </c>
-      <c r="I23" s="208"/>
+      <c r="I23" s="204"/>
     </row>
     <row r="24" spans="1:9" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="215"/>
-      <c r="B24" s="219"/>
+      <c r="A24" s="324"/>
+      <c r="B24" s="239"/>
       <c r="C24" s="117">
         <v>0.05</v>
       </c>
@@ -5087,7 +5087,7 @@
       <c r="F24" s="115" t="s">
         <v>182</v>
       </c>
-      <c r="G24" s="230"/>
+      <c r="G24" s="319"/>
       <c r="H24" s="114">
         <v>0.05</v>
       </c>
@@ -5249,30 +5249,30 @@
       <c r="A31" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="191">
+      <c r="B31" s="212">
         <v>43857</v>
       </c>
-      <c r="C31" s="192"/>
-      <c r="D31" s="193"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="214"/>
       <c r="E31" s="112"/>
       <c r="F31" s="112"/>
-      <c r="G31" s="194">
+      <c r="G31" s="293">
         <v>44046</v>
       </c>
-      <c r="H31" s="195"/>
-      <c r="I31" s="196"/>
+      <c r="H31" s="320"/>
+      <c r="I31" s="294"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="191"/>
-      <c r="C32" s="192"/>
-      <c r="D32" s="193"/>
-      <c r="E32" s="194">
+      <c r="B32" s="212"/>
+      <c r="C32" s="213"/>
+      <c r="D32" s="214"/>
+      <c r="E32" s="293">
         <v>43626</v>
       </c>
-      <c r="F32" s="196"/>
+      <c r="F32" s="294"/>
       <c r="G32" s="52"/>
       <c r="H32" s="108"/>
       <c r="I32" s="51"/>
@@ -5281,77 +5281,77 @@
       <c r="A33" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="191">
+      <c r="B33" s="212">
         <v>43781</v>
       </c>
-      <c r="C33" s="192"/>
-      <c r="D33" s="193"/>
-      <c r="E33" s="194"/>
-      <c r="F33" s="196"/>
-      <c r="G33" s="191">
+      <c r="C33" s="213"/>
+      <c r="D33" s="214"/>
+      <c r="E33" s="293"/>
+      <c r="F33" s="294"/>
+      <c r="G33" s="212">
         <v>43964</v>
       </c>
-      <c r="H33" s="192"/>
-      <c r="I33" s="193"/>
+      <c r="H33" s="213"/>
+      <c r="I33" s="214"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="225" t="s">
+      <c r="A34" s="208" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="225"/>
-      <c r="C34" s="225"/>
-      <c r="D34" s="225"/>
-      <c r="E34" s="225"/>
-      <c r="F34" s="225"/>
-      <c r="G34" s="225"/>
-      <c r="H34" s="225"/>
-      <c r="I34" s="225"/>
+      <c r="B34" s="208"/>
+      <c r="C34" s="208"/>
+      <c r="D34" s="208"/>
+      <c r="E34" s="208"/>
+      <c r="F34" s="208"/>
+      <c r="G34" s="208"/>
+      <c r="H34" s="208"/>
+      <c r="I34" s="208"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="210"/>
-      <c r="B35" s="211"/>
-      <c r="C35" s="211"/>
-      <c r="D35" s="211"/>
-      <c r="E35" s="211"/>
-      <c r="F35" s="211"/>
-      <c r="G35" s="211"/>
-      <c r="H35" s="211"/>
-      <c r="I35" s="212"/>
+      <c r="A35" s="191"/>
+      <c r="B35" s="193"/>
+      <c r="C35" s="193"/>
+      <c r="D35" s="193"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="192"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="226" t="s">
+      <c r="A36" s="205" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="227"/>
-      <c r="C36" s="227"/>
-      <c r="D36" s="227"/>
-      <c r="E36" s="227"/>
-      <c r="F36" s="227"/>
-      <c r="G36" s="227"/>
-      <c r="H36" s="227"/>
-      <c r="I36" s="228"/>
+      <c r="B36" s="206"/>
+      <c r="C36" s="206"/>
+      <c r="D36" s="206"/>
+      <c r="E36" s="206"/>
+      <c r="F36" s="206"/>
+      <c r="G36" s="206"/>
+      <c r="H36" s="206"/>
+      <c r="I36" s="207"/>
     </row>
     <row r="37" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="199" t="s">
+      <c r="A37" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="201" t="s">
+      <c r="B37" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="202"/>
-      <c r="D37" s="203"/>
-      <c r="E37" s="204" t="s">
+      <c r="C37" s="198"/>
+      <c r="D37" s="199"/>
+      <c r="E37" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="205"/>
-      <c r="G37" s="206" t="s">
+      <c r="F37" s="201"/>
+      <c r="G37" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H37" s="207"/>
-      <c r="I37" s="208"/>
+      <c r="H37" s="203"/>
+      <c r="I37" s="204"/>
     </row>
     <row r="38" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="200"/>
+      <c r="A38" s="196"/>
       <c r="B38" s="48" t="s">
         <v>113</v>
       </c>
@@ -5402,18 +5402,18 @@
       <c r="A40" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="191">
+      <c r="B40" s="212">
         <v>43846</v>
       </c>
-      <c r="C40" s="192"/>
-      <c r="D40" s="193"/>
-      <c r="E40" s="223"/>
-      <c r="F40" s="224"/>
-      <c r="G40" s="191">
+      <c r="C40" s="213"/>
+      <c r="D40" s="214"/>
+      <c r="E40" s="313"/>
+      <c r="F40" s="315"/>
+      <c r="G40" s="212">
         <v>44035</v>
       </c>
-      <c r="H40" s="192"/>
-      <c r="I40" s="193"/>
+      <c r="H40" s="213"/>
+      <c r="I40" s="214"/>
     </row>
     <row r="41" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A41" s="81" t="s">
@@ -5451,8 +5451,8 @@
       <c r="D42" s="14">
         <v>43816</v>
       </c>
-      <c r="E42" s="191"/>
-      <c r="F42" s="193"/>
+      <c r="E42" s="212"/>
+      <c r="F42" s="214"/>
       <c r="G42" s="15">
         <v>44000</v>
       </c>
@@ -5511,22 +5511,22 @@
       <c r="A45" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="191">
+      <c r="B45" s="212">
         <v>43837</v>
       </c>
-      <c r="C45" s="192"/>
-      <c r="D45" s="193"/>
+      <c r="C45" s="213"/>
+      <c r="D45" s="214"/>
       <c r="E45" s="14">
         <v>43616</v>
       </c>
       <c r="F45" s="14">
         <v>43619</v>
       </c>
-      <c r="G45" s="210">
+      <c r="G45" s="191">
         <v>44018</v>
       </c>
-      <c r="H45" s="211"/>
-      <c r="I45" s="212"/>
+      <c r="H45" s="193"/>
+      <c r="I45" s="192"/>
     </row>
     <row r="46" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A46" s="81" t="s">
@@ -5574,9 +5574,9 @@
       <c r="A48" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="191"/>
-      <c r="C48" s="192"/>
-      <c r="D48" s="193"/>
+      <c r="B48" s="212"/>
+      <c r="C48" s="213"/>
+      <c r="D48" s="214"/>
       <c r="E48" s="107"/>
       <c r="F48" s="106"/>
       <c r="G48" s="15">
@@ -5588,17 +5588,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="209" t="s">
+      <c r="A49" s="194" t="s">
         <v>172</v>
       </c>
-      <c r="B49" s="209"/>
-      <c r="C49" s="209"/>
-      <c r="D49" s="209"/>
-      <c r="E49" s="209"/>
-      <c r="F49" s="209"/>
-      <c r="G49" s="209"/>
-      <c r="H49" s="209"/>
-      <c r="I49" s="209"/>
+      <c r="B49" s="194"/>
+      <c r="C49" s="194"/>
+      <c r="D49" s="194"/>
+      <c r="E49" s="194"/>
+      <c r="F49" s="194"/>
+      <c r="G49" s="194"/>
+      <c r="H49" s="194"/>
+      <c r="I49" s="194"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="105"/>
@@ -5612,39 +5612,39 @@
       <c r="I50" s="105"/>
     </row>
     <row r="51" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="226" t="s">
+      <c r="A51" s="205" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="227"/>
-      <c r="C51" s="227"/>
-      <c r="D51" s="227"/>
-      <c r="E51" s="227"/>
-      <c r="F51" s="227"/>
-      <c r="G51" s="227"/>
-      <c r="H51" s="227"/>
-      <c r="I51" s="228"/>
+      <c r="B51" s="206"/>
+      <c r="C51" s="206"/>
+      <c r="D51" s="206"/>
+      <c r="E51" s="206"/>
+      <c r="F51" s="206"/>
+      <c r="G51" s="206"/>
+      <c r="H51" s="206"/>
+      <c r="I51" s="207"/>
     </row>
     <row r="52" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="199" t="s">
+      <c r="A52" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="201" t="s">
+      <c r="B52" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="202"/>
-      <c r="D52" s="203"/>
-      <c r="E52" s="204" t="s">
+      <c r="C52" s="198"/>
+      <c r="D52" s="199"/>
+      <c r="E52" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="205"/>
-      <c r="G52" s="206" t="s">
+      <c r="F52" s="201"/>
+      <c r="G52" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="207"/>
-      <c r="I52" s="208"/>
+      <c r="H52" s="203"/>
+      <c r="I52" s="204"/>
     </row>
     <row r="53" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="231"/>
+      <c r="A53" s="257"/>
       <c r="B53" s="25" t="s">
         <v>113</v>
       </c>
@@ -5670,67 +5670,67 @@
       <c r="A54" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="221">
+      <c r="B54" s="316">
         <v>43817</v>
       </c>
-      <c r="C54" s="221"/>
-      <c r="D54" s="221"/>
-      <c r="E54" s="221"/>
-      <c r="F54" s="221"/>
-      <c r="G54" s="222">
+      <c r="C54" s="316"/>
+      <c r="D54" s="316"/>
+      <c r="E54" s="316"/>
+      <c r="F54" s="316"/>
+      <c r="G54" s="317">
         <v>44005</v>
       </c>
-      <c r="H54" s="222"/>
-      <c r="I54" s="222"/>
+      <c r="H54" s="317"/>
+      <c r="I54" s="317"/>
     </row>
     <row r="55" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B55" s="232">
+      <c r="B55" s="209">
         <v>43840</v>
       </c>
-      <c r="C55" s="232"/>
-      <c r="D55" s="232"/>
-      <c r="E55" s="232"/>
-      <c r="F55" s="232"/>
-      <c r="G55" s="233">
+      <c r="C55" s="209"/>
+      <c r="D55" s="209"/>
+      <c r="E55" s="209"/>
+      <c r="F55" s="209"/>
+      <c r="G55" s="247">
         <v>44018</v>
       </c>
-      <c r="H55" s="233"/>
-      <c r="I55" s="233"/>
+      <c r="H55" s="247"/>
+      <c r="I55" s="247"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="232">
+      <c r="B56" s="209">
         <v>43844</v>
       </c>
-      <c r="C56" s="232"/>
-      <c r="D56" s="232"/>
-      <c r="E56" s="232"/>
-      <c r="F56" s="232"/>
-      <c r="G56" s="233">
+      <c r="C56" s="209"/>
+      <c r="D56" s="209"/>
+      <c r="E56" s="209"/>
+      <c r="F56" s="209"/>
+      <c r="G56" s="247">
         <v>44029</v>
       </c>
-      <c r="H56" s="233"/>
-      <c r="I56" s="233"/>
+      <c r="H56" s="247"/>
+      <c r="I56" s="247"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="232"/>
-      <c r="C57" s="232"/>
-      <c r="D57" s="232"/>
-      <c r="E57" s="232">
+      <c r="B57" s="209"/>
+      <c r="C57" s="209"/>
+      <c r="D57" s="209"/>
+      <c r="E57" s="209">
         <v>43984</v>
       </c>
-      <c r="F57" s="232"/>
-      <c r="G57" s="233"/>
-      <c r="H57" s="233"/>
-      <c r="I57" s="233"/>
+      <c r="F57" s="209"/>
+      <c r="G57" s="247"/>
+      <c r="H57" s="247"/>
+      <c r="I57" s="247"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="81" t="s">
@@ -5743,8 +5743,8 @@
       <c r="D58" s="15">
         <v>43858</v>
       </c>
-      <c r="E58" s="232"/>
-      <c r="F58" s="232"/>
+      <c r="E58" s="209"/>
+      <c r="F58" s="209"/>
       <c r="G58" s="15">
         <v>44035</v>
       </c>
@@ -5754,17 +5754,17 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="225" t="s">
+      <c r="A59" s="208" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="225"/>
-      <c r="C59" s="225"/>
-      <c r="D59" s="225"/>
-      <c r="E59" s="225"/>
-      <c r="F59" s="225"/>
-      <c r="G59" s="225"/>
-      <c r="H59" s="225"/>
-      <c r="I59" s="225"/>
+      <c r="B59" s="208"/>
+      <c r="C59" s="208"/>
+      <c r="D59" s="208"/>
+      <c r="E59" s="208"/>
+      <c r="F59" s="208"/>
+      <c r="G59" s="208"/>
+      <c r="H59" s="208"/>
+      <c r="I59" s="208"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="53"/>
@@ -5778,39 +5778,39 @@
       <c r="I60" s="53"/>
     </row>
     <row r="61" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="197" t="s">
+      <c r="A61" s="243" t="s">
         <v>30</v>
       </c>
-      <c r="B61" s="197"/>
-      <c r="C61" s="197"/>
-      <c r="D61" s="197"/>
-      <c r="E61" s="197"/>
-      <c r="F61" s="197"/>
-      <c r="G61" s="197"/>
-      <c r="H61" s="197"/>
-      <c r="I61" s="197"/>
+      <c r="B61" s="243"/>
+      <c r="C61" s="243"/>
+      <c r="D61" s="243"/>
+      <c r="E61" s="243"/>
+      <c r="F61" s="243"/>
+      <c r="G61" s="243"/>
+      <c r="H61" s="243"/>
+      <c r="I61" s="243"/>
     </row>
     <row r="62" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="199" t="s">
+      <c r="A62" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="201" t="s">
+      <c r="B62" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C62" s="202"/>
-      <c r="D62" s="203"/>
-      <c r="E62" s="204" t="s">
+      <c r="C62" s="198"/>
+      <c r="D62" s="199"/>
+      <c r="E62" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F62" s="205"/>
-      <c r="G62" s="206" t="s">
+      <c r="F62" s="201"/>
+      <c r="G62" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H62" s="207"/>
-      <c r="I62" s="208"/>
+      <c r="H62" s="203"/>
+      <c r="I62" s="204"/>
     </row>
     <row r="63" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="200"/>
+      <c r="A63" s="196"/>
       <c r="B63" s="48" t="s">
         <v>113</v>
       </c>
@@ -5836,145 +5836,145 @@
       <c r="A64" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="223">
+      <c r="B64" s="313">
         <v>43818</v>
       </c>
-      <c r="C64" s="234"/>
-      <c r="D64" s="224"/>
-      <c r="E64" s="223"/>
-      <c r="F64" s="224"/>
-      <c r="G64" s="210">
+      <c r="C64" s="314"/>
+      <c r="D64" s="315"/>
+      <c r="E64" s="313"/>
+      <c r="F64" s="315"/>
+      <c r="G64" s="191">
         <v>44006</v>
       </c>
-      <c r="H64" s="211"/>
-      <c r="I64" s="212"/>
+      <c r="H64" s="193"/>
+      <c r="I64" s="192"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="191">
+      <c r="B65" s="212">
         <v>43843</v>
       </c>
-      <c r="C65" s="192"/>
-      <c r="D65" s="193"/>
-      <c r="E65" s="191"/>
-      <c r="F65" s="193"/>
-      <c r="G65" s="210">
+      <c r="C65" s="213"/>
+      <c r="D65" s="214"/>
+      <c r="E65" s="212"/>
+      <c r="F65" s="214"/>
+      <c r="G65" s="191">
         <v>44020</v>
       </c>
-      <c r="H65" s="211"/>
-      <c r="I65" s="212"/>
+      <c r="H65" s="193"/>
+      <c r="I65" s="192"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B66" s="191" t="s">
+      <c r="B66" s="212" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="192"/>
-      <c r="D66" s="193"/>
-      <c r="E66" s="191"/>
-      <c r="F66" s="193"/>
-      <c r="G66" s="210" t="s">
+      <c r="C66" s="213"/>
+      <c r="D66" s="214"/>
+      <c r="E66" s="212"/>
+      <c r="F66" s="214"/>
+      <c r="G66" s="191" t="s">
         <v>169</v>
       </c>
-      <c r="H66" s="211"/>
-      <c r="I66" s="212"/>
+      <c r="H66" s="193"/>
+      <c r="I66" s="192"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="191" t="s">
+      <c r="B67" s="212" t="s">
         <v>168</v>
       </c>
-      <c r="C67" s="192"/>
-      <c r="D67" s="193"/>
-      <c r="E67" s="191"/>
-      <c r="F67" s="193"/>
-      <c r="G67" s="210">
+      <c r="C67" s="213"/>
+      <c r="D67" s="214"/>
+      <c r="E67" s="212"/>
+      <c r="F67" s="214"/>
+      <c r="G67" s="191">
         <v>44035</v>
       </c>
-      <c r="H67" s="211"/>
-      <c r="I67" s="212"/>
+      <c r="H67" s="193"/>
+      <c r="I67" s="192"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="191">
+      <c r="B68" s="212">
         <v>43847</v>
       </c>
-      <c r="C68" s="192"/>
-      <c r="D68" s="193"/>
-      <c r="E68" s="232">
+      <c r="C68" s="213"/>
+      <c r="D68" s="214"/>
+      <c r="E68" s="209">
         <v>43985</v>
       </c>
-      <c r="F68" s="232"/>
-      <c r="G68" s="210">
+      <c r="F68" s="209"/>
+      <c r="G68" s="191">
         <v>44036</v>
       </c>
-      <c r="H68" s="211"/>
-      <c r="I68" s="212"/>
+      <c r="H68" s="193"/>
+      <c r="I68" s="192"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="235"/>
-      <c r="B69" s="220"/>
-      <c r="C69" s="220"/>
-      <c r="D69" s="220"/>
-      <c r="E69" s="220"/>
-      <c r="F69" s="220"/>
-      <c r="G69" s="220"/>
-      <c r="H69" s="220"/>
-      <c r="I69" s="236"/>
+      <c r="A69" s="309"/>
+      <c r="B69" s="310"/>
+      <c r="C69" s="310"/>
+      <c r="D69" s="310"/>
+      <c r="E69" s="310"/>
+      <c r="F69" s="310"/>
+      <c r="G69" s="310"/>
+      <c r="H69" s="310"/>
+      <c r="I69" s="311"/>
     </row>
     <row r="70" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="244"/>
-      <c r="B70" s="245"/>
-      <c r="C70" s="245"/>
-      <c r="D70" s="245"/>
-      <c r="E70" s="245"/>
-      <c r="F70" s="245"/>
-      <c r="G70" s="245"/>
-      <c r="H70" s="245"/>
-      <c r="I70" s="246"/>
+      <c r="A70" s="297"/>
+      <c r="B70" s="298"/>
+      <c r="C70" s="298"/>
+      <c r="D70" s="298"/>
+      <c r="E70" s="298"/>
+      <c r="F70" s="298"/>
+      <c r="G70" s="298"/>
+      <c r="H70" s="298"/>
+      <c r="I70" s="299"/>
     </row>
     <row r="71" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="247" t="s">
+      <c r="A71" s="300" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="248"/>
-      <c r="C71" s="248"/>
-      <c r="D71" s="248"/>
-      <c r="E71" s="248"/>
-      <c r="F71" s="248"/>
-      <c r="G71" s="248"/>
-      <c r="H71" s="249"/>
-      <c r="I71" s="250"/>
+      <c r="B71" s="301"/>
+      <c r="C71" s="301"/>
+      <c r="D71" s="301"/>
+      <c r="E71" s="301"/>
+      <c r="F71" s="301"/>
+      <c r="G71" s="301"/>
+      <c r="H71" s="302"/>
+      <c r="I71" s="303"/>
     </row>
     <row r="72" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="237" t="s">
+      <c r="A72" s="312" t="s">
         <v>117</v>
       </c>
-      <c r="B72" s="201" t="s">
+      <c r="B72" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="202"/>
-      <c r="D72" s="203"/>
-      <c r="E72" s="204" t="s">
+      <c r="C72" s="198"/>
+      <c r="D72" s="199"/>
+      <c r="E72" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F72" s="205"/>
-      <c r="G72" s="206" t="s">
+      <c r="F72" s="201"/>
+      <c r="G72" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H72" s="207"/>
-      <c r="I72" s="208"/>
+      <c r="H72" s="203"/>
+      <c r="I72" s="204"/>
     </row>
     <row r="73" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="219"/>
+      <c r="A73" s="239"/>
       <c r="B73" s="25" t="s">
         <v>113</v>
       </c>
@@ -6000,13 +6000,13 @@
       <c r="A74" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="251" t="s">
+      <c r="B74" s="304" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="252"/>
-      <c r="D74" s="253"/>
-      <c r="E74" s="254"/>
-      <c r="F74" s="255"/>
+      <c r="C74" s="305"/>
+      <c r="D74" s="306"/>
+      <c r="E74" s="307"/>
+      <c r="F74" s="308"/>
       <c r="G74" s="103">
         <v>44034</v>
       </c>
@@ -6026,8 +6026,8 @@
       <c r="D75" s="100">
         <v>43847</v>
       </c>
-      <c r="E75" s="194"/>
-      <c r="F75" s="196"/>
+      <c r="E75" s="293"/>
+      <c r="F75" s="294"/>
       <c r="G75" s="41">
         <v>44036</v>
       </c>
@@ -6047,8 +6047,8 @@
       <c r="D76" s="100">
         <v>43845</v>
       </c>
-      <c r="E76" s="238"/>
-      <c r="F76" s="239"/>
+      <c r="E76" s="291"/>
+      <c r="F76" s="292"/>
       <c r="G76" s="41">
         <v>44034</v>
       </c>
@@ -6089,8 +6089,8 @@
       <c r="D78" s="96">
         <v>43847</v>
       </c>
-      <c r="E78" s="238"/>
-      <c r="F78" s="239"/>
+      <c r="E78" s="291"/>
+      <c r="F78" s="292"/>
       <c r="G78" s="41">
         <v>44036</v>
       </c>
@@ -6103,26 +6103,26 @@
       <c r="A79" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="238"/>
-      <c r="C79" s="242"/>
-      <c r="D79" s="239"/>
-      <c r="E79" s="194"/>
-      <c r="F79" s="196"/>
-      <c r="G79" s="238"/>
-      <c r="H79" s="242"/>
-      <c r="I79" s="243"/>
+      <c r="B79" s="291"/>
+      <c r="C79" s="295"/>
+      <c r="D79" s="292"/>
+      <c r="E79" s="293"/>
+      <c r="F79" s="294"/>
+      <c r="G79" s="291"/>
+      <c r="H79" s="295"/>
+      <c r="I79" s="296"/>
     </row>
     <row r="80" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A80" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="238">
+      <c r="B80" s="291">
         <v>43848</v>
       </c>
-      <c r="C80" s="242"/>
-      <c r="D80" s="239"/>
-      <c r="E80" s="194"/>
-      <c r="F80" s="196"/>
+      <c r="C80" s="295"/>
+      <c r="D80" s="292"/>
+      <c r="E80" s="293"/>
+      <c r="F80" s="294"/>
       <c r="G80" s="41">
         <v>44037</v>
       </c>
@@ -6142,8 +6142,8 @@
       <c r="D81" s="15">
         <v>43921</v>
       </c>
-      <c r="E81" s="240"/>
-      <c r="F81" s="241"/>
+      <c r="E81" s="254"/>
+      <c r="F81" s="255"/>
       <c r="G81" s="41">
         <v>44033</v>
       </c>
@@ -6153,17 +6153,17 @@
       </c>
     </row>
     <row r="82" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="263" t="s">
+      <c r="A82" s="277" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="264"/>
-      <c r="C82" s="264"/>
-      <c r="D82" s="264"/>
-      <c r="E82" s="265"/>
-      <c r="F82" s="265"/>
-      <c r="G82" s="265"/>
-      <c r="H82" s="265"/>
-      <c r="I82" s="266"/>
+      <c r="B82" s="278"/>
+      <c r="C82" s="278"/>
+      <c r="D82" s="278"/>
+      <c r="E82" s="279"/>
+      <c r="F82" s="279"/>
+      <c r="G82" s="279"/>
+      <c r="H82" s="279"/>
+      <c r="I82" s="280"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="92"/>
@@ -6177,39 +6177,39 @@
       <c r="I83" s="91"/>
     </row>
     <row r="84" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="197" t="s">
+      <c r="A84" s="243" t="s">
         <v>18</v>
       </c>
-      <c r="B84" s="197"/>
-      <c r="C84" s="197"/>
-      <c r="D84" s="197"/>
-      <c r="E84" s="197"/>
-      <c r="F84" s="197"/>
-      <c r="G84" s="197"/>
-      <c r="H84" s="197"/>
-      <c r="I84" s="197"/>
+      <c r="B84" s="243"/>
+      <c r="C84" s="243"/>
+      <c r="D84" s="243"/>
+      <c r="E84" s="243"/>
+      <c r="F84" s="243"/>
+      <c r="G84" s="243"/>
+      <c r="H84" s="243"/>
+      <c r="I84" s="243"/>
     </row>
     <row r="85" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="199" t="s">
+      <c r="A85" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="201" t="s">
+      <c r="B85" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="202"/>
-      <c r="D85" s="203"/>
-      <c r="E85" s="204" t="s">
+      <c r="C85" s="198"/>
+      <c r="D85" s="199"/>
+      <c r="E85" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F85" s="205"/>
-      <c r="G85" s="206" t="s">
+      <c r="F85" s="201"/>
+      <c r="G85" s="202" t="s">
         <v>163</v>
       </c>
-      <c r="H85" s="207"/>
-      <c r="I85" s="208"/>
+      <c r="H85" s="203"/>
+      <c r="I85" s="204"/>
     </row>
     <row r="86" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="200"/>
+      <c r="A86" s="196"/>
       <c r="B86" s="25" t="s">
         <v>113</v>
       </c>
@@ -6232,17 +6232,17 @@
       </c>
     </row>
     <row r="87" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="256" t="s">
+      <c r="A87" s="218" t="s">
         <v>162</v>
       </c>
-      <c r="B87" s="257"/>
-      <c r="C87" s="257"/>
-      <c r="D87" s="257"/>
-      <c r="E87" s="257"/>
-      <c r="F87" s="257"/>
-      <c r="G87" s="257"/>
-      <c r="H87" s="257"/>
-      <c r="I87" s="258"/>
+      <c r="B87" s="220"/>
+      <c r="C87" s="220"/>
+      <c r="D87" s="220"/>
+      <c r="E87" s="220"/>
+      <c r="F87" s="220"/>
+      <c r="G87" s="220"/>
+      <c r="H87" s="220"/>
+      <c r="I87" s="221"/>
     </row>
     <row r="88" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A88" s="81" t="s">
@@ -6324,18 +6324,18 @@
       <c r="A92" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="267">
+      <c r="B92" s="281">
         <v>43988</v>
       </c>
-      <c r="C92" s="268"/>
-      <c r="D92" s="269"/>
+      <c r="C92" s="282"/>
+      <c r="D92" s="283"/>
       <c r="E92" s="82"/>
       <c r="F92" s="82"/>
-      <c r="G92" s="267">
+      <c r="G92" s="281">
         <v>44170</v>
       </c>
-      <c r="H92" s="268"/>
-      <c r="I92" s="269"/>
+      <c r="H92" s="282"/>
+      <c r="I92" s="283"/>
     </row>
     <row r="93" spans="1:9" s="87" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A93" s="81" t="s">
@@ -6408,53 +6408,53 @@
       <c r="A96" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B96" s="270">
+      <c r="B96" s="284">
         <v>43974</v>
       </c>
-      <c r="C96" s="271"/>
-      <c r="D96" s="272"/>
+      <c r="C96" s="285"/>
+      <c r="D96" s="286"/>
       <c r="E96" s="82"/>
       <c r="F96" s="82"/>
-      <c r="G96" s="267">
+      <c r="G96" s="281">
         <v>44163</v>
       </c>
-      <c r="H96" s="268"/>
-      <c r="I96" s="269"/>
+      <c r="H96" s="282"/>
+      <c r="I96" s="283"/>
     </row>
     <row r="97" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="201" t="s">
+      <c r="A97" s="197" t="s">
         <v>160</v>
       </c>
-      <c r="B97" s="202"/>
-      <c r="C97" s="202"/>
-      <c r="D97" s="202"/>
-      <c r="E97" s="202"/>
-      <c r="F97" s="202"/>
-      <c r="G97" s="202"/>
-      <c r="H97" s="202"/>
-      <c r="I97" s="203"/>
+      <c r="B97" s="198"/>
+      <c r="C97" s="198"/>
+      <c r="D97" s="198"/>
+      <c r="E97" s="198"/>
+      <c r="F97" s="198"/>
+      <c r="G97" s="198"/>
+      <c r="H97" s="198"/>
+      <c r="I97" s="199"/>
     </row>
     <row r="98" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="199" t="s">
+      <c r="A98" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="201" t="s">
+      <c r="B98" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C98" s="202"/>
-      <c r="D98" s="203"/>
-      <c r="E98" s="204" t="s">
+      <c r="C98" s="198"/>
+      <c r="D98" s="199"/>
+      <c r="E98" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F98" s="205"/>
-      <c r="G98" s="206" t="s">
+      <c r="F98" s="201"/>
+      <c r="G98" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H98" s="207"/>
-      <c r="I98" s="208"/>
+      <c r="H98" s="203"/>
+      <c r="I98" s="204"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="231"/>
+      <c r="A99" s="257"/>
       <c r="B99" s="37" t="s">
         <v>113</v>
       </c>
@@ -6487,8 +6487,8 @@
       <c r="D100" s="15">
         <v>43960</v>
       </c>
-      <c r="E100" s="233"/>
-      <c r="F100" s="233"/>
+      <c r="E100" s="247"/>
+      <c r="F100" s="247"/>
       <c r="G100" s="82">
         <v>44046</v>
       </c>
@@ -6508,8 +6508,8 @@
       <c r="D101" s="15">
         <v>43967</v>
       </c>
-      <c r="E101" s="233"/>
-      <c r="F101" s="233"/>
+      <c r="E101" s="247"/>
+      <c r="F101" s="247"/>
       <c r="G101" s="15">
         <v>44152</v>
       </c>
@@ -6522,66 +6522,66 @@
       <c r="A102" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B102" s="233">
+      <c r="B102" s="247">
         <v>43967</v>
       </c>
-      <c r="C102" s="233"/>
-      <c r="D102" s="233"/>
-      <c r="E102" s="233"/>
-      <c r="F102" s="233"/>
-      <c r="G102" s="233">
+      <c r="C102" s="247"/>
+      <c r="D102" s="247"/>
+      <c r="E102" s="247"/>
+      <c r="F102" s="247"/>
+      <c r="G102" s="247">
         <v>44156</v>
       </c>
-      <c r="H102" s="233"/>
-      <c r="I102" s="233"/>
+      <c r="H102" s="247"/>
+      <c r="I102" s="247"/>
     </row>
     <row r="103" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="225" t="s">
+      <c r="A103" s="208" t="s">
         <v>159</v>
       </c>
-      <c r="B103" s="225"/>
-      <c r="C103" s="225"/>
-      <c r="D103" s="225"/>
-      <c r="E103" s="225"/>
-      <c r="F103" s="225"/>
-      <c r="G103" s="225"/>
-      <c r="H103" s="225"/>
-      <c r="I103" s="225"/>
+      <c r="B103" s="208"/>
+      <c r="C103" s="208"/>
+      <c r="D103" s="208"/>
+      <c r="E103" s="208"/>
+      <c r="F103" s="208"/>
+      <c r="G103" s="208"/>
+      <c r="H103" s="208"/>
+      <c r="I103" s="208"/>
     </row>
     <row r="104" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="256" t="s">
+      <c r="A104" s="218" t="s">
         <v>158</v>
       </c>
-      <c r="B104" s="257"/>
-      <c r="C104" s="257"/>
-      <c r="D104" s="257"/>
-      <c r="E104" s="257"/>
-      <c r="F104" s="257"/>
-      <c r="G104" s="257"/>
-      <c r="H104" s="257"/>
-      <c r="I104" s="258"/>
+      <c r="B104" s="220"/>
+      <c r="C104" s="220"/>
+      <c r="D104" s="220"/>
+      <c r="E104" s="220"/>
+      <c r="F104" s="220"/>
+      <c r="G104" s="220"/>
+      <c r="H104" s="220"/>
+      <c r="I104" s="221"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="218" t="s">
+      <c r="A105" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="B105" s="259" t="s">
+      <c r="B105" s="287" t="s">
         <v>116</v>
       </c>
-      <c r="C105" s="260"/>
-      <c r="D105" s="260"/>
-      <c r="E105" s="261" t="s">
+      <c r="C105" s="288"/>
+      <c r="D105" s="288"/>
+      <c r="E105" s="289" t="s">
         <v>115</v>
       </c>
-      <c r="F105" s="261"/>
-      <c r="G105" s="262" t="s">
+      <c r="F105" s="289"/>
+      <c r="G105" s="290" t="s">
         <v>114</v>
       </c>
-      <c r="H105" s="262"/>
-      <c r="I105" s="262"/>
+      <c r="H105" s="290"/>
+      <c r="I105" s="290"/>
     </row>
     <row r="106" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="219"/>
+      <c r="A106" s="239"/>
       <c r="B106" s="80" t="s">
         <v>113</v>
       </c>
@@ -6614,8 +6614,8 @@
       <c r="D107" s="15">
         <v>43967</v>
       </c>
-      <c r="E107" s="233"/>
-      <c r="F107" s="233"/>
+      <c r="E107" s="247"/>
+      <c r="F107" s="247"/>
       <c r="G107" s="15">
         <v>44046</v>
       </c>
@@ -6638,17 +6638,17 @@
       <c r="I108" s="74"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="225" t="s">
+      <c r="A109" s="208" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="225"/>
-      <c r="C109" s="225"/>
-      <c r="D109" s="225"/>
-      <c r="E109" s="225"/>
-      <c r="F109" s="225"/>
-      <c r="G109" s="225"/>
-      <c r="H109" s="225"/>
-      <c r="I109" s="225"/>
+      <c r="B109" s="208"/>
+      <c r="C109" s="208"/>
+      <c r="D109" s="208"/>
+      <c r="E109" s="208"/>
+      <c r="F109" s="208"/>
+      <c r="G109" s="208"/>
+      <c r="H109" s="208"/>
+      <c r="I109" s="208"/>
     </row>
     <row r="110" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="73"/>
@@ -6662,39 +6662,39 @@
       <c r="I110" s="73"/>
     </row>
     <row r="111" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="275" t="s">
+      <c r="A111" s="263" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="276"/>
-      <c r="C111" s="276"/>
-      <c r="D111" s="276"/>
-      <c r="E111" s="276"/>
-      <c r="F111" s="276"/>
-      <c r="G111" s="276"/>
-      <c r="H111" s="276"/>
-      <c r="I111" s="277"/>
+      <c r="B111" s="264"/>
+      <c r="C111" s="264"/>
+      <c r="D111" s="264"/>
+      <c r="E111" s="264"/>
+      <c r="F111" s="264"/>
+      <c r="G111" s="264"/>
+      <c r="H111" s="264"/>
+      <c r="I111" s="265"/>
     </row>
     <row r="112" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="281" t="s">
+      <c r="A112" s="266" t="s">
         <v>117</v>
       </c>
-      <c r="B112" s="283" t="s">
+      <c r="B112" s="268" t="s">
         <v>190</v>
       </c>
-      <c r="C112" s="284"/>
-      <c r="D112" s="285"/>
-      <c r="E112" s="286" t="s">
+      <c r="C112" s="269"/>
+      <c r="D112" s="270"/>
+      <c r="E112" s="271" t="s">
         <v>115</v>
       </c>
-      <c r="F112" s="287"/>
-      <c r="G112" s="288" t="s">
+      <c r="F112" s="272"/>
+      <c r="G112" s="273" t="s">
         <v>163</v>
       </c>
-      <c r="H112" s="289"/>
-      <c r="I112" s="290"/>
+      <c r="H112" s="274"/>
+      <c r="I112" s="275"/>
     </row>
     <row r="113" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="282"/>
+      <c r="A113" s="267"/>
       <c r="B113" s="124" t="s">
         <v>113</v>
       </c>
@@ -6720,149 +6720,149 @@
       <c r="A114" s="127" t="s">
         <v>191</v>
       </c>
-      <c r="B114" s="278">
+      <c r="B114" s="232">
         <v>43971</v>
       </c>
-      <c r="C114" s="279"/>
-      <c r="D114" s="280"/>
+      <c r="C114" s="233"/>
+      <c r="D114" s="234"/>
       <c r="E114" s="128"/>
       <c r="F114" s="128"/>
-      <c r="G114" s="278">
+      <c r="G114" s="232">
         <v>44158</v>
       </c>
-      <c r="H114" s="279"/>
-      <c r="I114" s="280"/>
+      <c r="H114" s="233"/>
+      <c r="I114" s="234"/>
     </row>
     <row r="115" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="B115" s="278">
+      <c r="B115" s="232">
         <v>43978</v>
       </c>
-      <c r="C115" s="279"/>
-      <c r="D115" s="280"/>
-      <c r="E115" s="278">
+      <c r="C115" s="233"/>
+      <c r="D115" s="234"/>
+      <c r="E115" s="232">
         <v>44029</v>
       </c>
-      <c r="F115" s="280"/>
-      <c r="G115" s="278">
+      <c r="F115" s="234"/>
+      <c r="G115" s="232">
         <v>44166</v>
       </c>
-      <c r="H115" s="279"/>
-      <c r="I115" s="280"/>
+      <c r="H115" s="233"/>
+      <c r="I115" s="234"/>
     </row>
     <row r="116" spans="1:9" ht="61.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="B116" s="278">
+      <c r="B116" s="232">
         <v>43991</v>
       </c>
-      <c r="C116" s="279"/>
-      <c r="D116" s="280"/>
-      <c r="E116" s="273"/>
-      <c r="F116" s="274"/>
-      <c r="G116" s="273" t="s">
+      <c r="C116" s="233"/>
+      <c r="D116" s="234"/>
+      <c r="E116" s="235"/>
+      <c r="F116" s="236"/>
+      <c r="G116" s="235" t="s">
         <v>193</v>
       </c>
-      <c r="H116" s="291"/>
-      <c r="I116" s="274"/>
+      <c r="H116" s="276"/>
+      <c r="I116" s="236"/>
     </row>
     <row r="117" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="B117" s="278">
+      <c r="B117" s="232">
         <v>43979</v>
       </c>
-      <c r="C117" s="279"/>
-      <c r="D117" s="280"/>
-      <c r="E117" s="278">
+      <c r="C117" s="233"/>
+      <c r="D117" s="234"/>
+      <c r="E117" s="232">
         <v>44029</v>
       </c>
-      <c r="F117" s="280"/>
-      <c r="G117" s="278">
+      <c r="F117" s="234"/>
+      <c r="G117" s="232">
         <v>44167</v>
       </c>
-      <c r="H117" s="279"/>
-      <c r="I117" s="280"/>
+      <c r="H117" s="233"/>
+      <c r="I117" s="234"/>
     </row>
     <row r="118" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B118" s="278">
+      <c r="B118" s="232">
         <v>43992</v>
       </c>
-      <c r="C118" s="279"/>
-      <c r="D118" s="280"/>
-      <c r="E118" s="273"/>
-      <c r="F118" s="274"/>
-      <c r="G118" s="278">
+      <c r="C118" s="233"/>
+      <c r="D118" s="234"/>
+      <c r="E118" s="235"/>
+      <c r="F118" s="236"/>
+      <c r="G118" s="232">
         <v>44175</v>
       </c>
-      <c r="H118" s="279"/>
-      <c r="I118" s="280"/>
+      <c r="H118" s="233"/>
+      <c r="I118" s="234"/>
     </row>
     <row r="119" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="308" t="s">
+      <c r="A119" s="244" t="s">
         <v>194</v>
       </c>
-      <c r="B119" s="309"/>
-      <c r="C119" s="309"/>
-      <c r="D119" s="309"/>
-      <c r="E119" s="309"/>
-      <c r="F119" s="309"/>
-      <c r="G119" s="309"/>
-      <c r="H119" s="309"/>
-      <c r="I119" s="310"/>
+      <c r="B119" s="245"/>
+      <c r="C119" s="245"/>
+      <c r="D119" s="245"/>
+      <c r="E119" s="245"/>
+      <c r="F119" s="245"/>
+      <c r="G119" s="245"/>
+      <c r="H119" s="245"/>
+      <c r="I119" s="246"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="210"/>
-      <c r="B120" s="211"/>
-      <c r="C120" s="211"/>
-      <c r="D120" s="211"/>
-      <c r="E120" s="211"/>
-      <c r="F120" s="211"/>
-      <c r="G120" s="211"/>
-      <c r="H120" s="211"/>
-      <c r="I120" s="212"/>
+      <c r="A120" s="191"/>
+      <c r="B120" s="193"/>
+      <c r="C120" s="193"/>
+      <c r="D120" s="193"/>
+      <c r="E120" s="193"/>
+      <c r="F120" s="193"/>
+      <c r="G120" s="193"/>
+      <c r="H120" s="193"/>
+      <c r="I120" s="192"/>
     </row>
     <row r="121" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="197" t="s">
+      <c r="A121" s="243" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="197"/>
-      <c r="C121" s="197"/>
-      <c r="D121" s="197"/>
-      <c r="E121" s="197"/>
-      <c r="F121" s="197"/>
-      <c r="G121" s="197"/>
-      <c r="H121" s="197"/>
-      <c r="I121" s="197"/>
+      <c r="B121" s="243"/>
+      <c r="C121" s="243"/>
+      <c r="D121" s="243"/>
+      <c r="E121" s="243"/>
+      <c r="F121" s="243"/>
+      <c r="G121" s="243"/>
+      <c r="H121" s="243"/>
+      <c r="I121" s="243"/>
     </row>
     <row r="122" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="199" t="s">
+      <c r="A122" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B122" s="201" t="s">
+      <c r="B122" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C122" s="202"/>
-      <c r="D122" s="203"/>
-      <c r="E122" s="204" t="s">
+      <c r="C122" s="198"/>
+      <c r="D122" s="199"/>
+      <c r="E122" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F122" s="205"/>
-      <c r="G122" s="206" t="s">
+      <c r="F122" s="201"/>
+      <c r="G122" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H122" s="207"/>
-      <c r="I122" s="208"/>
+      <c r="H122" s="203"/>
+      <c r="I122" s="204"/>
     </row>
     <row r="123" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="200"/>
+      <c r="A123" s="196"/>
       <c r="B123" s="48" t="s">
         <v>113</v>
       </c>
@@ -6948,58 +6948,58 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" s="209" t="s">
+      <c r="A127" s="194" t="s">
         <v>154</v>
       </c>
-      <c r="B127" s="209"/>
-      <c r="C127" s="209"/>
-      <c r="D127" s="209"/>
-      <c r="E127" s="209"/>
-      <c r="F127" s="209"/>
-      <c r="G127" s="209"/>
-      <c r="H127" s="209"/>
-      <c r="I127" s="209"/>
+      <c r="B127" s="194"/>
+      <c r="C127" s="194"/>
+      <c r="D127" s="194"/>
+      <c r="E127" s="194"/>
+      <c r="F127" s="194"/>
+      <c r="G127" s="194"/>
+      <c r="H127" s="194"/>
+      <c r="I127" s="194"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="210"/>
-      <c r="B128" s="211"/>
-      <c r="C128" s="211"/>
-      <c r="D128" s="211"/>
-      <c r="E128" s="211"/>
-      <c r="F128" s="211"/>
-      <c r="G128" s="211"/>
-      <c r="H128" s="211"/>
-      <c r="I128" s="212"/>
+      <c r="A128" s="191"/>
+      <c r="B128" s="193"/>
+      <c r="C128" s="193"/>
+      <c r="D128" s="193"/>
+      <c r="E128" s="193"/>
+      <c r="F128" s="193"/>
+      <c r="G128" s="193"/>
+      <c r="H128" s="193"/>
+      <c r="I128" s="192"/>
     </row>
     <row r="129" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="197" t="s">
+      <c r="A129" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="B129" s="197"/>
-      <c r="C129" s="197"/>
-      <c r="D129" s="197"/>
-      <c r="E129" s="197"/>
-      <c r="F129" s="197"/>
-      <c r="G129" s="197"/>
-      <c r="H129" s="197"/>
-      <c r="I129" s="197"/>
+      <c r="B129" s="243"/>
+      <c r="C129" s="243"/>
+      <c r="D129" s="243"/>
+      <c r="E129" s="243"/>
+      <c r="F129" s="243"/>
+      <c r="G129" s="243"/>
+      <c r="H129" s="243"/>
+      <c r="I129" s="243"/>
     </row>
     <row r="130" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="47"/>
-      <c r="B130" s="201" t="s">
+      <c r="B130" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C130" s="202"/>
-      <c r="D130" s="203"/>
-      <c r="E130" s="204" t="s">
+      <c r="C130" s="198"/>
+      <c r="D130" s="199"/>
+      <c r="E130" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F130" s="205"/>
-      <c r="G130" s="206" t="s">
+      <c r="F130" s="201"/>
+      <c r="G130" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H130" s="207"/>
-      <c r="I130" s="208"/>
+      <c r="H130" s="203"/>
+      <c r="I130" s="204"/>
     </row>
     <row r="131" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="25" t="s">
@@ -7037,19 +7037,19 @@
       <c r="D132" s="15">
         <v>43931</v>
       </c>
-      <c r="E132" s="233"/>
-      <c r="F132" s="233"/>
-      <c r="G132" s="295"/>
-      <c r="H132" s="296"/>
-      <c r="I132" s="297"/>
+      <c r="E132" s="247"/>
+      <c r="F132" s="247"/>
+      <c r="G132" s="248"/>
+      <c r="H132" s="228"/>
+      <c r="I132" s="249"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C133" s="15"/>
-      <c r="E133" s="233"/>
-      <c r="F133" s="233"/>
+      <c r="E133" s="247"/>
+      <c r="F133" s="247"/>
       <c r="G133" s="15">
         <v>44117</v>
       </c>
@@ -7091,8 +7091,8 @@
       <c r="B136" s="70"/>
       <c r="C136" s="14"/>
       <c r="D136" s="70"/>
-      <c r="E136" s="232"/>
-      <c r="F136" s="232"/>
+      <c r="E136" s="209"/>
+      <c r="F136" s="209"/>
       <c r="G136" s="69"/>
       <c r="H136" s="69"/>
       <c r="I136" s="69"/>
@@ -7175,17 +7175,17 @@
       <c r="I141" s="15"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" s="209" t="s">
+      <c r="A142" s="194" t="s">
         <v>140</v>
       </c>
-      <c r="B142" s="209"/>
-      <c r="C142" s="209"/>
-      <c r="D142" s="209"/>
-      <c r="E142" s="209"/>
-      <c r="F142" s="209"/>
-      <c r="G142" s="209"/>
-      <c r="H142" s="209"/>
-      <c r="I142" s="209"/>
+      <c r="B142" s="194"/>
+      <c r="C142" s="194"/>
+      <c r="D142" s="194"/>
+      <c r="E142" s="194"/>
+      <c r="F142" s="194"/>
+      <c r="G142" s="194"/>
+      <c r="H142" s="194"/>
+      <c r="I142" s="194"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="27"/>
@@ -7199,52 +7199,52 @@
       <c r="I143" s="27"/>
     </row>
     <row r="144" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="321" t="s">
+      <c r="A144" s="237" t="s">
         <v>90</v>
       </c>
-      <c r="B144" s="321"/>
-      <c r="C144" s="321"/>
-      <c r="D144" s="321"/>
-      <c r="E144" s="321"/>
-      <c r="F144" s="321"/>
-      <c r="G144" s="321"/>
-      <c r="H144" s="321"/>
-      <c r="I144" s="321"/>
+      <c r="B144" s="237"/>
+      <c r="C144" s="237"/>
+      <c r="D144" s="237"/>
+      <c r="E144" s="237"/>
+      <c r="F144" s="237"/>
+      <c r="G144" s="237"/>
+      <c r="H144" s="237"/>
+      <c r="I144" s="237"/>
     </row>
     <row r="145" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="201" t="s">
+      <c r="A145" s="197" t="s">
         <v>152</v>
       </c>
-      <c r="B145" s="202"/>
-      <c r="C145" s="202"/>
-      <c r="D145" s="202"/>
-      <c r="E145" s="202"/>
-      <c r="F145" s="202"/>
-      <c r="G145" s="202"/>
-      <c r="H145" s="202"/>
-      <c r="I145" s="203"/>
+      <c r="B145" s="198"/>
+      <c r="C145" s="198"/>
+      <c r="D145" s="198"/>
+      <c r="E145" s="198"/>
+      <c r="F145" s="198"/>
+      <c r="G145" s="198"/>
+      <c r="H145" s="198"/>
+      <c r="I145" s="199"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A146" s="218" t="s">
+      <c r="A146" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="B146" s="256" t="s">
+      <c r="B146" s="218" t="s">
         <v>116</v>
       </c>
-      <c r="C146" s="257"/>
-      <c r="D146" s="258"/>
-      <c r="E146" s="320" t="s">
+      <c r="C146" s="220"/>
+      <c r="D146" s="221"/>
+      <c r="E146" s="222" t="s">
         <v>115</v>
       </c>
-      <c r="F146" s="314"/>
-      <c r="G146" s="315" t="s">
+      <c r="F146" s="223"/>
+      <c r="G146" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="H146" s="316"/>
-      <c r="I146" s="317"/>
+      <c r="H146" s="225"/>
+      <c r="I146" s="226"/>
     </row>
     <row r="147" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="219"/>
+      <c r="A147" s="239"/>
       <c r="B147" s="64" t="s">
         <v>149</v>
       </c>
@@ -7322,22 +7322,22 @@
       <c r="A152" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B152" s="210"/>
-      <c r="C152" s="211"/>
-      <c r="D152" s="212"/>
-      <c r="E152" s="210"/>
-      <c r="F152" s="212"/>
-      <c r="G152" s="210"/>
-      <c r="H152" s="211"/>
-      <c r="I152" s="212"/>
+      <c r="B152" s="191"/>
+      <c r="C152" s="193"/>
+      <c r="D152" s="192"/>
+      <c r="E152" s="191"/>
+      <c r="F152" s="192"/>
+      <c r="G152" s="191"/>
+      <c r="H152" s="193"/>
+      <c r="I152" s="192"/>
     </row>
     <row r="153" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B153" s="210"/>
-      <c r="C153" s="211"/>
-      <c r="D153" s="212"/>
+      <c r="B153" s="191"/>
+      <c r="C153" s="193"/>
+      <c r="D153" s="192"/>
       <c r="E153" s="15"/>
       <c r="F153" s="15"/>
       <c r="G153" s="15"/>
@@ -7348,14 +7348,14 @@
       <c r="A154" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B154" s="210"/>
-      <c r="C154" s="211"/>
-      <c r="D154" s="212"/>
-      <c r="E154" s="210"/>
-      <c r="F154" s="212"/>
-      <c r="G154" s="210"/>
-      <c r="H154" s="211"/>
-      <c r="I154" s="212"/>
+      <c r="B154" s="191"/>
+      <c r="C154" s="193"/>
+      <c r="D154" s="192"/>
+      <c r="E154" s="191"/>
+      <c r="F154" s="192"/>
+      <c r="G154" s="191"/>
+      <c r="H154" s="193"/>
+      <c r="I154" s="192"/>
     </row>
     <row r="155" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
@@ -7387,14 +7387,14 @@
       <c r="A157" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B157" s="210"/>
-      <c r="C157" s="211"/>
-      <c r="D157" s="212"/>
-      <c r="E157" s="210"/>
-      <c r="F157" s="212"/>
-      <c r="G157" s="210"/>
-      <c r="H157" s="211"/>
-      <c r="I157" s="212"/>
+      <c r="B157" s="191"/>
+      <c r="C157" s="193"/>
+      <c r="D157" s="192"/>
+      <c r="E157" s="191"/>
+      <c r="F157" s="192"/>
+      <c r="G157" s="191"/>
+      <c r="H157" s="193"/>
+      <c r="I157" s="192"/>
     </row>
     <row r="158" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
@@ -7410,39 +7410,39 @@
       <c r="I158" s="66"/>
     </row>
     <row r="159" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="201" t="s">
+      <c r="A159" s="197" t="s">
         <v>151</v>
       </c>
-      <c r="B159" s="202"/>
-      <c r="C159" s="202"/>
-      <c r="D159" s="202"/>
-      <c r="E159" s="202"/>
-      <c r="F159" s="202"/>
-      <c r="G159" s="202"/>
-      <c r="H159" s="202"/>
-      <c r="I159" s="203"/>
+      <c r="B159" s="198"/>
+      <c r="C159" s="198"/>
+      <c r="D159" s="198"/>
+      <c r="E159" s="198"/>
+      <c r="F159" s="198"/>
+      <c r="G159" s="198"/>
+      <c r="H159" s="198"/>
+      <c r="I159" s="199"/>
     </row>
     <row r="160" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="256" t="s">
+      <c r="A160" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B160" s="256" t="s">
+      <c r="B160" s="218" t="s">
         <v>116</v>
       </c>
-      <c r="C160" s="257"/>
-      <c r="D160" s="258"/>
-      <c r="E160" s="320" t="s">
+      <c r="C160" s="220"/>
+      <c r="D160" s="221"/>
+      <c r="E160" s="222" t="s">
         <v>115</v>
       </c>
-      <c r="F160" s="314"/>
-      <c r="G160" s="315" t="s">
+      <c r="F160" s="223"/>
+      <c r="G160" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="H160" s="316"/>
-      <c r="I160" s="317"/>
+      <c r="H160" s="225"/>
+      <c r="I160" s="226"/>
     </row>
     <row r="161" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="323"/>
+      <c r="A161" s="219"/>
       <c r="B161" s="63" t="s">
         <v>149</v>
       </c>
@@ -7520,22 +7520,22 @@
       <c r="A166" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B166" s="210"/>
-      <c r="C166" s="211"/>
-      <c r="D166" s="212"/>
-      <c r="E166" s="210"/>
-      <c r="F166" s="212"/>
-      <c r="G166" s="210"/>
-      <c r="H166" s="211"/>
-      <c r="I166" s="212"/>
+      <c r="B166" s="191"/>
+      <c r="C166" s="193"/>
+      <c r="D166" s="192"/>
+      <c r="E166" s="191"/>
+      <c r="F166" s="192"/>
+      <c r="G166" s="191"/>
+      <c r="H166" s="193"/>
+      <c r="I166" s="192"/>
     </row>
     <row r="167" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B167" s="210"/>
-      <c r="C167" s="211"/>
-      <c r="D167" s="212"/>
+      <c r="B167" s="191"/>
+      <c r="C167" s="193"/>
+      <c r="D167" s="192"/>
       <c r="E167" s="15"/>
       <c r="F167" s="15"/>
       <c r="G167" s="15"/>
@@ -7546,14 +7546,14 @@
       <c r="A168" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B168" s="210"/>
-      <c r="C168" s="211"/>
-      <c r="D168" s="212"/>
-      <c r="E168" s="210"/>
-      <c r="F168" s="212"/>
-      <c r="G168" s="210"/>
-      <c r="H168" s="211"/>
-      <c r="I168" s="212"/>
+      <c r="B168" s="191"/>
+      <c r="C168" s="193"/>
+      <c r="D168" s="192"/>
+      <c r="E168" s="191"/>
+      <c r="F168" s="192"/>
+      <c r="G168" s="191"/>
+      <c r="H168" s="193"/>
+      <c r="I168" s="192"/>
     </row>
     <row r="169" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
@@ -7572,14 +7572,14 @@
       <c r="A170" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B170" s="210"/>
-      <c r="C170" s="211"/>
-      <c r="D170" s="212"/>
-      <c r="E170" s="210"/>
-      <c r="F170" s="212"/>
-      <c r="G170" s="210"/>
-      <c r="H170" s="211"/>
-      <c r="I170" s="212"/>
+      <c r="B170" s="191"/>
+      <c r="C170" s="193"/>
+      <c r="D170" s="192"/>
+      <c r="E170" s="191"/>
+      <c r="F170" s="192"/>
+      <c r="G170" s="191"/>
+      <c r="H170" s="193"/>
+      <c r="I170" s="192"/>
     </row>
     <row r="171" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
@@ -7595,39 +7595,39 @@
       <c r="I171" s="65"/>
     </row>
     <row r="172" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="201" t="s">
+      <c r="A172" s="197" t="s">
         <v>150</v>
       </c>
-      <c r="B172" s="202"/>
-      <c r="C172" s="202"/>
-      <c r="D172" s="202"/>
-      <c r="E172" s="202"/>
-      <c r="F172" s="202"/>
-      <c r="G172" s="202"/>
-      <c r="H172" s="202"/>
-      <c r="I172" s="203"/>
+      <c r="B172" s="198"/>
+      <c r="C172" s="198"/>
+      <c r="D172" s="198"/>
+      <c r="E172" s="198"/>
+      <c r="F172" s="198"/>
+      <c r="G172" s="198"/>
+      <c r="H172" s="198"/>
+      <c r="I172" s="199"/>
     </row>
     <row r="173" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="256" t="s">
+      <c r="A173" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B173" s="256" t="s">
+      <c r="B173" s="218" t="s">
         <v>116</v>
       </c>
-      <c r="C173" s="257"/>
-      <c r="D173" s="258"/>
-      <c r="E173" s="313" t="s">
+      <c r="C173" s="220"/>
+      <c r="D173" s="221"/>
+      <c r="E173" s="242" t="s">
         <v>115</v>
       </c>
-      <c r="F173" s="314"/>
-      <c r="G173" s="315" t="s">
+      <c r="F173" s="223"/>
+      <c r="G173" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="H173" s="316"/>
-      <c r="I173" s="317"/>
+      <c r="H173" s="225"/>
+      <c r="I173" s="226"/>
     </row>
     <row r="174" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="323"/>
+      <c r="A174" s="219"/>
       <c r="B174" s="64" t="s">
         <v>149</v>
       </c>
@@ -7705,22 +7705,22 @@
       <c r="A179" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B179" s="210"/>
-      <c r="C179" s="211"/>
-      <c r="D179" s="212"/>
-      <c r="E179" s="210"/>
-      <c r="F179" s="212"/>
-      <c r="G179" s="210"/>
-      <c r="H179" s="211"/>
-      <c r="I179" s="212"/>
+      <c r="B179" s="191"/>
+      <c r="C179" s="193"/>
+      <c r="D179" s="192"/>
+      <c r="E179" s="191"/>
+      <c r="F179" s="192"/>
+      <c r="G179" s="191"/>
+      <c r="H179" s="193"/>
+      <c r="I179" s="192"/>
     </row>
     <row r="180" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B180" s="210"/>
-      <c r="C180" s="211"/>
-      <c r="D180" s="212"/>
+      <c r="B180" s="191"/>
+      <c r="C180" s="193"/>
+      <c r="D180" s="192"/>
       <c r="E180" s="15"/>
       <c r="F180" s="15"/>
       <c r="G180" s="56"/>
@@ -7731,14 +7731,14 @@
       <c r="A181" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B181" s="210"/>
-      <c r="C181" s="211"/>
-      <c r="D181" s="212"/>
-      <c r="E181" s="210"/>
-      <c r="F181" s="212"/>
-      <c r="G181" s="210"/>
-      <c r="H181" s="211"/>
-      <c r="I181" s="212"/>
+      <c r="B181" s="191"/>
+      <c r="C181" s="193"/>
+      <c r="D181" s="192"/>
+      <c r="E181" s="191"/>
+      <c r="F181" s="192"/>
+      <c r="G181" s="191"/>
+      <c r="H181" s="193"/>
+      <c r="I181" s="192"/>
     </row>
     <row r="182" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
@@ -7757,14 +7757,14 @@
       <c r="A183" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B183" s="210"/>
-      <c r="C183" s="211"/>
-      <c r="D183" s="212"/>
-      <c r="E183" s="210"/>
-      <c r="F183" s="212"/>
-      <c r="G183" s="210"/>
-      <c r="H183" s="211"/>
-      <c r="I183" s="212"/>
+      <c r="B183" s="191"/>
+      <c r="C183" s="193"/>
+      <c r="D183" s="192"/>
+      <c r="E183" s="191"/>
+      <c r="F183" s="192"/>
+      <c r="G183" s="191"/>
+      <c r="H183" s="193"/>
+      <c r="I183" s="192"/>
     </row>
     <row r="184" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
@@ -7780,74 +7780,74 @@
       <c r="I184" s="15"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A185" s="322" t="s">
+      <c r="A185" s="229" t="s">
         <v>147</v>
       </c>
-      <c r="B185" s="322"/>
-      <c r="C185" s="322"/>
-      <c r="D185" s="322"/>
-      <c r="E185" s="322"/>
-      <c r="F185" s="322"/>
-      <c r="G185" s="322"/>
-      <c r="H185" s="322"/>
-      <c r="I185" s="322"/>
+      <c r="B185" s="229"/>
+      <c r="C185" s="229"/>
+      <c r="D185" s="229"/>
+      <c r="E185" s="229"/>
+      <c r="F185" s="229"/>
+      <c r="G185" s="229"/>
+      <c r="H185" s="229"/>
+      <c r="I185" s="229"/>
     </row>
     <row r="186" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="324"/>
-      <c r="B186" s="324"/>
-      <c r="C186" s="324"/>
-      <c r="D186" s="324"/>
-      <c r="E186" s="324"/>
-      <c r="F186" s="324"/>
-      <c r="G186" s="324"/>
-      <c r="H186" s="324"/>
-      <c r="I186" s="324"/>
+      <c r="A186" s="227"/>
+      <c r="B186" s="227"/>
+      <c r="C186" s="227"/>
+      <c r="D186" s="227"/>
+      <c r="E186" s="227"/>
+      <c r="F186" s="227"/>
+      <c r="G186" s="227"/>
+      <c r="H186" s="227"/>
+      <c r="I186" s="227"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A187" s="296"/>
-      <c r="B187" s="296"/>
-      <c r="C187" s="296"/>
-      <c r="D187" s="296"/>
-      <c r="E187" s="296"/>
-      <c r="F187" s="296"/>
-      <c r="G187" s="296"/>
-      <c r="H187" s="296"/>
-      <c r="I187" s="296"/>
+      <c r="A187" s="228"/>
+      <c r="B187" s="228"/>
+      <c r="C187" s="228"/>
+      <c r="D187" s="228"/>
+      <c r="E187" s="228"/>
+      <c r="F187" s="228"/>
+      <c r="G187" s="228"/>
+      <c r="H187" s="228"/>
+      <c r="I187" s="228"/>
     </row>
     <row r="188" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="226" t="s">
+      <c r="A188" s="205" t="s">
         <v>101</v>
       </c>
-      <c r="B188" s="227"/>
-      <c r="C188" s="227"/>
-      <c r="D188" s="227"/>
-      <c r="E188" s="227"/>
-      <c r="F188" s="227"/>
-      <c r="G188" s="227"/>
-      <c r="H188" s="227"/>
-      <c r="I188" s="228"/>
+      <c r="B188" s="206"/>
+      <c r="C188" s="206"/>
+      <c r="D188" s="206"/>
+      <c r="E188" s="206"/>
+      <c r="F188" s="206"/>
+      <c r="G188" s="206"/>
+      <c r="H188" s="206"/>
+      <c r="I188" s="207"/>
     </row>
     <row r="189" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="199" t="s">
+      <c r="A189" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B189" s="201" t="s">
+      <c r="B189" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C189" s="202"/>
-      <c r="D189" s="203"/>
-      <c r="E189" s="204" t="s">
+      <c r="C189" s="198"/>
+      <c r="D189" s="199"/>
+      <c r="E189" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F189" s="205"/>
-      <c r="G189" s="206" t="s">
+      <c r="F189" s="201"/>
+      <c r="G189" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H189" s="207"/>
-      <c r="I189" s="208"/>
+      <c r="H189" s="203"/>
+      <c r="I189" s="204"/>
     </row>
     <row r="190" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="200"/>
+      <c r="A190" s="196"/>
       <c r="B190" s="25" t="s">
         <v>113</v>
       </c>
@@ -7873,130 +7873,130 @@
       <c r="A191" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B191" s="232"/>
-      <c r="C191" s="232"/>
-      <c r="D191" s="232"/>
-      <c r="E191" s="318"/>
-      <c r="F191" s="319"/>
-      <c r="G191" s="232"/>
-      <c r="H191" s="232"/>
-      <c r="I191" s="232"/>
+      <c r="B191" s="209"/>
+      <c r="C191" s="209"/>
+      <c r="D191" s="209"/>
+      <c r="E191" s="230"/>
+      <c r="F191" s="231"/>
+      <c r="G191" s="209"/>
+      <c r="H191" s="209"/>
+      <c r="I191" s="209"/>
     </row>
     <row r="192" spans="1:9" ht="81" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B192" s="232">
+      <c r="B192" s="209">
         <v>43905</v>
       </c>
-      <c r="C192" s="232"/>
-      <c r="D192" s="232"/>
-      <c r="E192" s="318"/>
-      <c r="F192" s="319"/>
-      <c r="G192" s="232">
+      <c r="C192" s="209"/>
+      <c r="D192" s="209"/>
+      <c r="E192" s="230"/>
+      <c r="F192" s="231"/>
+      <c r="G192" s="209">
         <v>44094</v>
       </c>
-      <c r="H192" s="232"/>
-      <c r="I192" s="232"/>
+      <c r="H192" s="209"/>
+      <c r="I192" s="209"/>
     </row>
     <row r="193" spans="1:9" s="50" customFormat="1" ht="81" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B193" s="232">
+      <c r="B193" s="209">
         <v>43898</v>
       </c>
-      <c r="C193" s="232"/>
-      <c r="D193" s="232"/>
-      <c r="E193" s="325"/>
-      <c r="F193" s="326"/>
-      <c r="G193" s="232">
+      <c r="C193" s="209"/>
+      <c r="D193" s="209"/>
+      <c r="E193" s="210"/>
+      <c r="F193" s="211"/>
+      <c r="G193" s="209">
         <v>44080</v>
       </c>
-      <c r="H193" s="232"/>
-      <c r="I193" s="232"/>
+      <c r="H193" s="209"/>
+      <c r="I193" s="209"/>
     </row>
     <row r="194" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A194" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B194" s="191"/>
-      <c r="C194" s="192"/>
-      <c r="D194" s="193"/>
-      <c r="E194" s="191"/>
-      <c r="F194" s="193"/>
-      <c r="G194" s="292"/>
-      <c r="H194" s="293"/>
-      <c r="I194" s="294"/>
+      <c r="B194" s="212"/>
+      <c r="C194" s="213"/>
+      <c r="D194" s="214"/>
+      <c r="E194" s="212"/>
+      <c r="F194" s="214"/>
+      <c r="G194" s="215"/>
+      <c r="H194" s="216"/>
+      <c r="I194" s="217"/>
     </row>
     <row r="195" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B195" s="191"/>
-      <c r="C195" s="192"/>
-      <c r="D195" s="193"/>
-      <c r="E195" s="191"/>
-      <c r="F195" s="193"/>
-      <c r="G195" s="292"/>
-      <c r="H195" s="293"/>
-      <c r="I195" s="294"/>
+      <c r="B195" s="212"/>
+      <c r="C195" s="213"/>
+      <c r="D195" s="214"/>
+      <c r="E195" s="212"/>
+      <c r="F195" s="214"/>
+      <c r="G195" s="215"/>
+      <c r="H195" s="216"/>
+      <c r="I195" s="217"/>
     </row>
     <row r="196" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B196" s="191"/>
-      <c r="C196" s="192"/>
-      <c r="D196" s="193"/>
-      <c r="E196" s="191"/>
-      <c r="F196" s="193"/>
-      <c r="G196" s="292"/>
-      <c r="H196" s="293"/>
-      <c r="I196" s="294"/>
+      <c r="B196" s="212"/>
+      <c r="C196" s="213"/>
+      <c r="D196" s="214"/>
+      <c r="E196" s="212"/>
+      <c r="F196" s="214"/>
+      <c r="G196" s="215"/>
+      <c r="H196" s="216"/>
+      <c r="I196" s="217"/>
     </row>
     <row r="197" spans="1:9" s="50" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B197" s="232">
+      <c r="B197" s="209">
         <v>43905</v>
       </c>
-      <c r="C197" s="232"/>
-      <c r="D197" s="232"/>
+      <c r="C197" s="209"/>
+      <c r="D197" s="209"/>
       <c r="E197" s="52"/>
       <c r="F197" s="51"/>
-      <c r="G197" s="232">
+      <c r="G197" s="209">
         <v>44094</v>
       </c>
-      <c r="H197" s="232"/>
-      <c r="I197" s="232"/>
+      <c r="H197" s="209"/>
+      <c r="I197" s="209"/>
     </row>
     <row r="198" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B198" s="191"/>
-      <c r="C198" s="192"/>
-      <c r="D198" s="193"/>
-      <c r="E198" s="191"/>
-      <c r="F198" s="193"/>
-      <c r="G198" s="292"/>
-      <c r="H198" s="293"/>
-      <c r="I198" s="294"/>
+      <c r="B198" s="212"/>
+      <c r="C198" s="213"/>
+      <c r="D198" s="214"/>
+      <c r="E198" s="212"/>
+      <c r="F198" s="214"/>
+      <c r="G198" s="215"/>
+      <c r="H198" s="216"/>
+      <c r="I198" s="217"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" s="225" t="s">
+      <c r="A199" s="208" t="s">
         <v>140</v>
       </c>
-      <c r="B199" s="225"/>
-      <c r="C199" s="225"/>
-      <c r="D199" s="225"/>
-      <c r="E199" s="225"/>
-      <c r="F199" s="225"/>
-      <c r="G199" s="225"/>
-      <c r="H199" s="225"/>
-      <c r="I199" s="225"/>
+      <c r="B199" s="208"/>
+      <c r="C199" s="208"/>
+      <c r="D199" s="208"/>
+      <c r="E199" s="208"/>
+      <c r="F199" s="208"/>
+      <c r="G199" s="208"/>
+      <c r="H199" s="208"/>
+      <c r="I199" s="208"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="49"/>
@@ -8010,61 +8010,61 @@
       <c r="I200" s="49"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" s="298"/>
-      <c r="B201" s="298"/>
-      <c r="C201" s="298"/>
-      <c r="D201" s="298"/>
-      <c r="E201" s="298"/>
-      <c r="F201" s="298"/>
-      <c r="G201" s="298"/>
-      <c r="H201" s="298"/>
-      <c r="I201" s="298"/>
+      <c r="A201" s="258"/>
+      <c r="B201" s="258"/>
+      <c r="C201" s="258"/>
+      <c r="D201" s="258"/>
+      <c r="E201" s="258"/>
+      <c r="F201" s="258"/>
+      <c r="G201" s="258"/>
+      <c r="H201" s="258"/>
+      <c r="I201" s="258"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="299"/>
-      <c r="B202" s="300"/>
-      <c r="C202" s="300"/>
-      <c r="D202" s="300"/>
-      <c r="E202" s="300"/>
-      <c r="F202" s="300"/>
-      <c r="G202" s="300"/>
-      <c r="H202" s="300"/>
-      <c r="I202" s="301"/>
+      <c r="A202" s="259"/>
+      <c r="B202" s="260"/>
+      <c r="C202" s="260"/>
+      <c r="D202" s="260"/>
+      <c r="E202" s="260"/>
+      <c r="F202" s="260"/>
+      <c r="G202" s="260"/>
+      <c r="H202" s="260"/>
+      <c r="I202" s="261"/>
     </row>
     <row r="203" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="226" t="s">
+      <c r="A203" s="205" t="s">
         <v>146</v>
       </c>
-      <c r="B203" s="227"/>
-      <c r="C203" s="227"/>
-      <c r="D203" s="227"/>
-      <c r="E203" s="227"/>
-      <c r="F203" s="227"/>
-      <c r="G203" s="227"/>
-      <c r="H203" s="227"/>
-      <c r="I203" s="228"/>
+      <c r="B203" s="206"/>
+      <c r="C203" s="206"/>
+      <c r="D203" s="206"/>
+      <c r="E203" s="206"/>
+      <c r="F203" s="206"/>
+      <c r="G203" s="206"/>
+      <c r="H203" s="206"/>
+      <c r="I203" s="207"/>
     </row>
     <row r="204" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="218" t="s">
+      <c r="A204" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="B204" s="201" t="s">
+      <c r="B204" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C204" s="202"/>
-      <c r="D204" s="203"/>
-      <c r="E204" s="204" t="s">
+      <c r="C204" s="198"/>
+      <c r="D204" s="199"/>
+      <c r="E204" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F204" s="205"/>
-      <c r="G204" s="206" t="s">
+      <c r="F204" s="201"/>
+      <c r="G204" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H204" s="207"/>
-      <c r="I204" s="208"/>
+      <c r="H204" s="203"/>
+      <c r="I204" s="204"/>
     </row>
     <row r="205" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="219"/>
+      <c r="A205" s="239"/>
       <c r="B205" s="25" t="s">
         <v>113</v>
       </c>
@@ -8090,117 +8090,117 @@
       <c r="A206" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B206" s="295"/>
-      <c r="C206" s="296"/>
-      <c r="D206" s="297"/>
-      <c r="E206" s="295"/>
-      <c r="F206" s="297"/>
-      <c r="G206" s="210"/>
-      <c r="H206" s="211"/>
-      <c r="I206" s="212"/>
+      <c r="B206" s="248"/>
+      <c r="C206" s="228"/>
+      <c r="D206" s="249"/>
+      <c r="E206" s="248"/>
+      <c r="F206" s="249"/>
+      <c r="G206" s="191"/>
+      <c r="H206" s="193"/>
+      <c r="I206" s="192"/>
     </row>
     <row r="207" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A207" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B207" s="210"/>
-      <c r="C207" s="211"/>
-      <c r="D207" s="212"/>
-      <c r="E207" s="210"/>
-      <c r="F207" s="212"/>
-      <c r="G207" s="210"/>
-      <c r="H207" s="211"/>
-      <c r="I207" s="212"/>
+      <c r="B207" s="191"/>
+      <c r="C207" s="193"/>
+      <c r="D207" s="192"/>
+      <c r="E207" s="191"/>
+      <c r="F207" s="192"/>
+      <c r="G207" s="191"/>
+      <c r="H207" s="193"/>
+      <c r="I207" s="192"/>
     </row>
     <row r="208" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A208" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B208" s="210"/>
-      <c r="C208" s="211"/>
-      <c r="D208" s="212"/>
-      <c r="E208" s="210"/>
-      <c r="F208" s="212"/>
-      <c r="G208" s="210"/>
-      <c r="H208" s="211"/>
-      <c r="I208" s="212"/>
+      <c r="B208" s="191"/>
+      <c r="C208" s="193"/>
+      <c r="D208" s="192"/>
+      <c r="E208" s="191"/>
+      <c r="F208" s="192"/>
+      <c r="G208" s="191"/>
+      <c r="H208" s="193"/>
+      <c r="I208" s="192"/>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B209" s="210"/>
-      <c r="C209" s="211"/>
-      <c r="D209" s="212"/>
-      <c r="E209" s="210"/>
-      <c r="F209" s="212"/>
-      <c r="G209" s="210"/>
-      <c r="H209" s="211"/>
-      <c r="I209" s="212"/>
+      <c r="B209" s="191"/>
+      <c r="C209" s="193"/>
+      <c r="D209" s="192"/>
+      <c r="E209" s="191"/>
+      <c r="F209" s="192"/>
+      <c r="G209" s="191"/>
+      <c r="H209" s="193"/>
+      <c r="I209" s="192"/>
     </row>
     <row r="210" spans="1:10" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A210" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B210" s="210"/>
-      <c r="C210" s="211"/>
-      <c r="D210" s="212"/>
-      <c r="E210" s="210"/>
-      <c r="F210" s="212"/>
-      <c r="G210" s="210"/>
-      <c r="H210" s="211"/>
-      <c r="I210" s="212"/>
+      <c r="B210" s="191"/>
+      <c r="C210" s="193"/>
+      <c r="D210" s="192"/>
+      <c r="E210" s="191"/>
+      <c r="F210" s="192"/>
+      <c r="G210" s="191"/>
+      <c r="H210" s="193"/>
+      <c r="I210" s="192"/>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A211" s="209" t="s">
+      <c r="A211" s="194" t="s">
         <v>140</v>
       </c>
-      <c r="B211" s="209"/>
-      <c r="C211" s="209"/>
-      <c r="D211" s="209"/>
-      <c r="E211" s="209"/>
-      <c r="F211" s="209"/>
-      <c r="G211" s="209"/>
-      <c r="H211" s="209"/>
-      <c r="I211" s="209"/>
+      <c r="B211" s="194"/>
+      <c r="C211" s="194"/>
+      <c r="D211" s="194"/>
+      <c r="E211" s="194"/>
+      <c r="F211" s="194"/>
+      <c r="G211" s="194"/>
+      <c r="H211" s="194"/>
+      <c r="I211" s="194"/>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" s="11"/>
     </row>
     <row r="213" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="226" t="s">
+      <c r="A213" s="205" t="s">
         <v>139</v>
       </c>
-      <c r="B213" s="227"/>
-      <c r="C213" s="227"/>
-      <c r="D213" s="227"/>
-      <c r="E213" s="227"/>
-      <c r="F213" s="227"/>
-      <c r="G213" s="227"/>
-      <c r="H213" s="227"/>
-      <c r="I213" s="228"/>
+      <c r="B213" s="206"/>
+      <c r="C213" s="206"/>
+      <c r="D213" s="206"/>
+      <c r="E213" s="206"/>
+      <c r="F213" s="206"/>
+      <c r="G213" s="206"/>
+      <c r="H213" s="206"/>
+      <c r="I213" s="207"/>
     </row>
     <row r="214" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="199" t="s">
+      <c r="A214" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B214" s="201" t="s">
+      <c r="B214" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C214" s="202"/>
-      <c r="D214" s="203"/>
-      <c r="E214" s="204" t="s">
+      <c r="C214" s="198"/>
+      <c r="D214" s="199"/>
+      <c r="E214" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F214" s="205"/>
-      <c r="G214" s="206" t="s">
+      <c r="F214" s="201"/>
+      <c r="G214" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H214" s="207"/>
-      <c r="I214" s="208"/>
+      <c r="H214" s="203"/>
+      <c r="I214" s="204"/>
     </row>
     <row r="215" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="200"/>
+      <c r="A215" s="196"/>
       <c r="B215" s="48" t="s">
         <v>113</v>
       </c>
@@ -8236,17 +8236,17 @@
       <c r="I216" s="15"/>
     </row>
     <row r="217" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="209" t="s">
+      <c r="A217" s="194" t="s">
         <v>137</v>
       </c>
-      <c r="B217" s="209"/>
-      <c r="C217" s="209"/>
-      <c r="D217" s="209"/>
-      <c r="E217" s="209"/>
-      <c r="F217" s="209"/>
-      <c r="G217" s="209"/>
-      <c r="H217" s="209"/>
-      <c r="I217" s="209"/>
+      <c r="B217" s="194"/>
+      <c r="C217" s="194"/>
+      <c r="D217" s="194"/>
+      <c r="E217" s="194"/>
+      <c r="F217" s="194"/>
+      <c r="G217" s="194"/>
+      <c r="H217" s="194"/>
+      <c r="I217" s="194"/>
     </row>
     <row r="218" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="11"/>
@@ -8254,39 +8254,39 @@
       <c r="C218" s="44"/>
     </row>
     <row r="219" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A219" s="226" t="s">
+      <c r="A219" s="205" t="s">
         <v>136</v>
       </c>
-      <c r="B219" s="227"/>
-      <c r="C219" s="227"/>
-      <c r="D219" s="227"/>
-      <c r="E219" s="227"/>
-      <c r="F219" s="227"/>
-      <c r="G219" s="227"/>
-      <c r="H219" s="227"/>
-      <c r="I219" s="228"/>
+      <c r="B219" s="206"/>
+      <c r="C219" s="206"/>
+      <c r="D219" s="206"/>
+      <c r="E219" s="206"/>
+      <c r="F219" s="206"/>
+      <c r="G219" s="206"/>
+      <c r="H219" s="206"/>
+      <c r="I219" s="207"/>
     </row>
     <row r="220" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="199" t="s">
+      <c r="A220" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B220" s="201" t="s">
+      <c r="B220" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C220" s="202"/>
-      <c r="D220" s="203"/>
-      <c r="E220" s="204" t="s">
+      <c r="C220" s="198"/>
+      <c r="D220" s="199"/>
+      <c r="E220" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F220" s="205"/>
-      <c r="G220" s="206" t="s">
+      <c r="F220" s="201"/>
+      <c r="G220" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H220" s="207"/>
-      <c r="I220" s="208"/>
+      <c r="H220" s="203"/>
+      <c r="I220" s="204"/>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A221" s="231"/>
+      <c r="A221" s="257"/>
       <c r="B221" s="33" t="s">
         <v>135</v>
       </c>
@@ -8319,8 +8319,8 @@
       <c r="D222" s="15">
         <v>43945</v>
       </c>
-      <c r="E222" s="240"/>
-      <c r="F222" s="241"/>
+      <c r="E222" s="254"/>
+      <c r="F222" s="255"/>
       <c r="G222" s="41">
         <v>44095</v>
       </c>
@@ -8340,8 +8340,8 @@
       <c r="D223" s="15">
         <v>43921</v>
       </c>
-      <c r="E223" s="240"/>
-      <c r="F223" s="241"/>
+      <c r="E223" s="254"/>
+      <c r="F223" s="255"/>
       <c r="G223" s="41">
         <v>44033</v>
       </c>
@@ -8378,39 +8378,39 @@
       <c r="I225" s="38"/>
     </row>
     <row r="226" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="226" t="s">
+      <c r="A226" s="205" t="s">
         <v>129</v>
       </c>
-      <c r="B226" s="227"/>
-      <c r="C226" s="227"/>
-      <c r="D226" s="227"/>
-      <c r="E226" s="227"/>
-      <c r="F226" s="227"/>
-      <c r="G226" s="227"/>
-      <c r="H226" s="227"/>
-      <c r="I226" s="228"/>
+      <c r="B226" s="206"/>
+      <c r="C226" s="206"/>
+      <c r="D226" s="206"/>
+      <c r="E226" s="206"/>
+      <c r="F226" s="206"/>
+      <c r="G226" s="206"/>
+      <c r="H226" s="206"/>
+      <c r="I226" s="207"/>
     </row>
     <row r="227" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A227" s="199" t="s">
+      <c r="A227" s="195" t="s">
         <v>117</v>
       </c>
-      <c r="B227" s="201" t="s">
+      <c r="B227" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C227" s="202"/>
-      <c r="D227" s="203"/>
-      <c r="E227" s="204" t="s">
+      <c r="C227" s="198"/>
+      <c r="D227" s="199"/>
+      <c r="E227" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F227" s="205"/>
-      <c r="G227" s="206" t="s">
+      <c r="F227" s="201"/>
+      <c r="G227" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="H227" s="207"/>
-      <c r="I227" s="208"/>
+      <c r="H227" s="203"/>
+      <c r="I227" s="204"/>
     </row>
     <row r="228" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="200"/>
+      <c r="A228" s="196"/>
       <c r="B228" s="37" t="s">
         <v>113</v>
       </c>
@@ -8497,17 +8497,17 @@
       <c r="I233" s="15"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A234" s="209" t="s">
+      <c r="A234" s="194" t="s">
         <v>102</v>
       </c>
-      <c r="B234" s="209"/>
-      <c r="C234" s="209"/>
-      <c r="D234" s="209"/>
-      <c r="E234" s="209"/>
-      <c r="F234" s="209"/>
-      <c r="G234" s="209"/>
-      <c r="H234" s="209"/>
-      <c r="I234" s="209"/>
+      <c r="B234" s="194"/>
+      <c r="C234" s="194"/>
+      <c r="D234" s="194"/>
+      <c r="E234" s="194"/>
+      <c r="F234" s="194"/>
+      <c r="G234" s="194"/>
+      <c r="H234" s="194"/>
+      <c r="I234" s="194"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="11"/>
@@ -8532,35 +8532,35 @@
       <c r="I236" s="9"/>
     </row>
     <row r="237" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="303" t="s">
+      <c r="A237" s="250" t="s">
         <v>124</v>
       </c>
-      <c r="B237" s="304"/>
-      <c r="C237" s="304"/>
+      <c r="B237" s="251"/>
+      <c r="C237" s="251"/>
       <c r="D237" s="9"/>
-      <c r="E237" s="306"/>
-      <c r="F237" s="306"/>
-      <c r="G237" s="306"/>
+      <c r="E237" s="253"/>
+      <c r="F237" s="253"/>
+      <c r="G237" s="253"/>
       <c r="H237" s="9"/>
       <c r="I237" s="9"/>
     </row>
     <row r="238" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="218" t="s">
+      <c r="A238" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="B238" s="201" t="s">
+      <c r="B238" s="197" t="s">
         <v>123</v>
       </c>
-      <c r="C238" s="203"/>
+      <c r="C238" s="199"/>
       <c r="D238" s="9"/>
-      <c r="E238" s="307"/>
-      <c r="F238" s="307"/>
-      <c r="G238" s="307"/>
+      <c r="E238" s="256"/>
+      <c r="F238" s="256"/>
+      <c r="G238" s="256"/>
       <c r="H238" s="9"/>
       <c r="I238" s="9"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A239" s="305"/>
+      <c r="A239" s="252"/>
       <c r="B239" s="33" t="s">
         <v>113</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>112</v>
       </c>
       <c r="D239" s="9"/>
-      <c r="E239" s="307"/>
+      <c r="E239" s="256"/>
       <c r="F239" s="32"/>
       <c r="G239" s="32"/>
       <c r="H239" s="9"/>
@@ -8643,15 +8643,15 @@
       <c r="I243" s="9"/>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A244" s="311" t="s">
+      <c r="A244" s="240" t="s">
         <v>102</v>
       </c>
-      <c r="B244" s="209"/>
-      <c r="C244" s="312"/>
+      <c r="B244" s="194"/>
+      <c r="C244" s="241"/>
       <c r="D244" s="9"/>
-      <c r="E244" s="302"/>
-      <c r="F244" s="302"/>
-      <c r="G244" s="302"/>
+      <c r="E244" s="262"/>
+      <c r="F244" s="262"/>
+      <c r="G244" s="262"/>
       <c r="H244" s="9"/>
       <c r="I244" s="9"/>
     </row>
@@ -8700,39 +8700,39 @@
       <c r="I248" s="9"/>
     </row>
     <row r="249" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="226" t="s">
+      <c r="A249" s="205" t="s">
         <v>118</v>
       </c>
-      <c r="B249" s="227"/>
-      <c r="C249" s="227"/>
-      <c r="D249" s="227"/>
-      <c r="E249" s="227"/>
-      <c r="F249" s="227"/>
-      <c r="G249" s="228"/>
+      <c r="B249" s="206"/>
+      <c r="C249" s="206"/>
+      <c r="D249" s="206"/>
+      <c r="E249" s="206"/>
+      <c r="F249" s="206"/>
+      <c r="G249" s="207"/>
       <c r="H249" s="9"/>
       <c r="I249" s="9"/>
     </row>
     <row r="250" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A250" s="218" t="s">
+      <c r="A250" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="B250" s="201" t="s">
+      <c r="B250" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C250" s="203"/>
-      <c r="D250" s="204" t="s">
+      <c r="C250" s="199"/>
+      <c r="D250" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="E250" s="205"/>
-      <c r="F250" s="206" t="s">
+      <c r="E250" s="201"/>
+      <c r="F250" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="G250" s="208"/>
+      <c r="G250" s="204"/>
       <c r="H250" s="9"/>
       <c r="I250" s="9"/>
     </row>
     <row r="251" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A251" s="219"/>
+      <c r="A251" s="239"/>
       <c r="B251" s="25" t="s">
         <v>113</v>
       </c>
@@ -8868,15 +8868,15 @@
       <c r="I257" s="9"/>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A258" s="225" t="s">
+      <c r="A258" s="208" t="s">
         <v>102</v>
       </c>
-      <c r="B258" s="225"/>
-      <c r="C258" s="225"/>
-      <c r="D258" s="225"/>
-      <c r="E258" s="225"/>
-      <c r="F258" s="225"/>
-      <c r="G258" s="225"/>
+      <c r="B258" s="208"/>
+      <c r="C258" s="208"/>
+      <c r="D258" s="208"/>
+      <c r="E258" s="208"/>
+      <c r="F258" s="208"/>
+      <c r="G258" s="208"/>
       <c r="H258" s="9"/>
       <c r="I258" s="9"/>
     </row>
@@ -13076,53 +13076,241 @@
     <filterColumn colId="7" showButton="0"/>
   </autoFilter>
   <mergeCells count="306">
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="G207:I207"/>
-    <mergeCell ref="A211:I211"/>
-    <mergeCell ref="A214:A215"/>
-    <mergeCell ref="B214:D214"/>
-    <mergeCell ref="E214:F214"/>
-    <mergeCell ref="G214:I214"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="G209:I209"/>
-    <mergeCell ref="A213:I213"/>
-    <mergeCell ref="B207:D207"/>
-    <mergeCell ref="A199:I199"/>
-    <mergeCell ref="B193:D193"/>
-    <mergeCell ref="E193:F193"/>
-    <mergeCell ref="G193:I193"/>
-    <mergeCell ref="B194:D194"/>
-    <mergeCell ref="E194:F194"/>
-    <mergeCell ref="G194:I194"/>
-    <mergeCell ref="E195:F195"/>
-    <mergeCell ref="G195:I195"/>
-    <mergeCell ref="B197:D197"/>
-    <mergeCell ref="G197:I197"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="E198:F198"/>
-    <mergeCell ref="G198:I198"/>
-    <mergeCell ref="A173:A174"/>
-    <mergeCell ref="A188:I188"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="B160:D160"/>
-    <mergeCell ref="E160:F160"/>
-    <mergeCell ref="G160:I160"/>
-    <mergeCell ref="E157:F157"/>
-    <mergeCell ref="G157:I157"/>
-    <mergeCell ref="A159:I159"/>
-    <mergeCell ref="A186:I186"/>
-    <mergeCell ref="B180:D180"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="B189:D189"/>
-    <mergeCell ref="E189:F189"/>
-    <mergeCell ref="G189:I189"/>
-    <mergeCell ref="A187:I187"/>
-    <mergeCell ref="E183:F183"/>
-    <mergeCell ref="G183:I183"/>
-    <mergeCell ref="B181:D181"/>
-    <mergeCell ref="E181:F181"/>
-    <mergeCell ref="G181:I181"/>
-    <mergeCell ref="A185:I185"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="A71:I71"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="G105:I105"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A97:I97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="G114:I114"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="G112:I112"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="G115:I115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="G116:I116"/>
+    <mergeCell ref="G206:I206"/>
+    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="G208:I208"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="A258:G258"/>
+    <mergeCell ref="A219:I219"/>
+    <mergeCell ref="E222:F222"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="G196:I196"/>
+    <mergeCell ref="A217:I217"/>
+    <mergeCell ref="B210:D210"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="G210:I210"/>
+    <mergeCell ref="B209:D209"/>
+    <mergeCell ref="B206:D206"/>
+    <mergeCell ref="E206:F206"/>
+    <mergeCell ref="A201:I201"/>
+    <mergeCell ref="A203:I203"/>
+    <mergeCell ref="A202:I202"/>
+    <mergeCell ref="E244:G244"/>
+    <mergeCell ref="A234:I234"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:C238"/>
+    <mergeCell ref="E237:G237"/>
+    <mergeCell ref="E220:F220"/>
+    <mergeCell ref="G220:I220"/>
+    <mergeCell ref="E223:F223"/>
+    <mergeCell ref="A226:I226"/>
+    <mergeCell ref="A227:A228"/>
+    <mergeCell ref="B227:D227"/>
+    <mergeCell ref="E227:F227"/>
+    <mergeCell ref="G227:I227"/>
+    <mergeCell ref="F238:G238"/>
+    <mergeCell ref="E238:E239"/>
+    <mergeCell ref="A121:I121"/>
+    <mergeCell ref="A119:I119"/>
+    <mergeCell ref="A120:I120"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="G168:I168"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="A172:I172"/>
+    <mergeCell ref="A129:I129"/>
+    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="G132:I132"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G122:I122"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="G166:I166"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="A127:I127"/>
+    <mergeCell ref="A128:I128"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="E170:F170"/>
+    <mergeCell ref="G170:I170"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="A249:G249"/>
+    <mergeCell ref="A250:A251"/>
+    <mergeCell ref="B250:C250"/>
+    <mergeCell ref="D250:E250"/>
+    <mergeCell ref="F250:G250"/>
+    <mergeCell ref="A244:C244"/>
+    <mergeCell ref="B195:D195"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="E173:F173"/>
+    <mergeCell ref="G173:I173"/>
+    <mergeCell ref="B179:D179"/>
+    <mergeCell ref="E179:F179"/>
+    <mergeCell ref="G179:I179"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="E191:F191"/>
+    <mergeCell ref="G191:I191"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="B204:D204"/>
+    <mergeCell ref="E204:F204"/>
+    <mergeCell ref="G204:I204"/>
+    <mergeCell ref="B192:D192"/>
     <mergeCell ref="E192:F192"/>
     <mergeCell ref="G192:I192"/>
     <mergeCell ref="G117:I117"/>
@@ -13147,241 +13335,53 @@
     <mergeCell ref="A144:I144"/>
     <mergeCell ref="B153:D153"/>
     <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="A249:G249"/>
-    <mergeCell ref="A250:A251"/>
-    <mergeCell ref="B250:C250"/>
-    <mergeCell ref="D250:E250"/>
-    <mergeCell ref="F250:G250"/>
-    <mergeCell ref="A244:C244"/>
-    <mergeCell ref="B195:D195"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="E173:F173"/>
-    <mergeCell ref="G173:I173"/>
-    <mergeCell ref="B179:D179"/>
-    <mergeCell ref="E179:F179"/>
-    <mergeCell ref="G179:I179"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="E191:F191"/>
-    <mergeCell ref="G191:I191"/>
-    <mergeCell ref="A204:A205"/>
-    <mergeCell ref="B204:D204"/>
-    <mergeCell ref="E204:F204"/>
-    <mergeCell ref="G204:I204"/>
-    <mergeCell ref="B192:D192"/>
-    <mergeCell ref="A121:I121"/>
-    <mergeCell ref="A119:I119"/>
-    <mergeCell ref="A120:I120"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="G168:I168"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="A172:I172"/>
-    <mergeCell ref="A129:I129"/>
-    <mergeCell ref="E132:F132"/>
-    <mergeCell ref="G132:I132"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="G122:I122"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="G166:I166"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="A127:I127"/>
-    <mergeCell ref="A128:I128"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="E170:F170"/>
-    <mergeCell ref="G170:I170"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="A234:I234"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:C238"/>
-    <mergeCell ref="E237:G237"/>
-    <mergeCell ref="E220:F220"/>
-    <mergeCell ref="G220:I220"/>
-    <mergeCell ref="E223:F223"/>
-    <mergeCell ref="A226:I226"/>
-    <mergeCell ref="A227:A228"/>
-    <mergeCell ref="B227:D227"/>
-    <mergeCell ref="E227:F227"/>
-    <mergeCell ref="G227:I227"/>
-    <mergeCell ref="F238:G238"/>
-    <mergeCell ref="E238:E239"/>
-    <mergeCell ref="G206:I206"/>
-    <mergeCell ref="B208:D208"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="G208:I208"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="A258:G258"/>
-    <mergeCell ref="A219:I219"/>
-    <mergeCell ref="E222:F222"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="G196:I196"/>
-    <mergeCell ref="A217:I217"/>
-    <mergeCell ref="B210:D210"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="G210:I210"/>
-    <mergeCell ref="B209:D209"/>
-    <mergeCell ref="B206:D206"/>
-    <mergeCell ref="E206:F206"/>
-    <mergeCell ref="A201:I201"/>
-    <mergeCell ref="A203:I203"/>
-    <mergeCell ref="A202:I202"/>
-    <mergeCell ref="E244:G244"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="A111:I111"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="G114:I114"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="G112:I112"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="G115:I115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="G116:I116"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A97:I97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="A87:I87"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="A103:I103"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="G105:I105"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="A70:I70"/>
-    <mergeCell ref="A71:I71"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="A69:I69"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="B189:D189"/>
+    <mergeCell ref="E189:F189"/>
+    <mergeCell ref="G189:I189"/>
+    <mergeCell ref="A187:I187"/>
+    <mergeCell ref="E183:F183"/>
+    <mergeCell ref="G183:I183"/>
+    <mergeCell ref="B181:D181"/>
+    <mergeCell ref="E181:F181"/>
+    <mergeCell ref="G181:I181"/>
+    <mergeCell ref="A185:I185"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="A188:I188"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:D160"/>
+    <mergeCell ref="E160:F160"/>
+    <mergeCell ref="G160:I160"/>
+    <mergeCell ref="E157:F157"/>
+    <mergeCell ref="G157:I157"/>
+    <mergeCell ref="A159:I159"/>
+    <mergeCell ref="A186:I186"/>
+    <mergeCell ref="B180:D180"/>
+    <mergeCell ref="A199:I199"/>
+    <mergeCell ref="B193:D193"/>
+    <mergeCell ref="E193:F193"/>
+    <mergeCell ref="G193:I193"/>
+    <mergeCell ref="B194:D194"/>
+    <mergeCell ref="E194:F194"/>
+    <mergeCell ref="G194:I194"/>
+    <mergeCell ref="E195:F195"/>
+    <mergeCell ref="G195:I195"/>
+    <mergeCell ref="B197:D197"/>
+    <mergeCell ref="G197:I197"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="E198:F198"/>
+    <mergeCell ref="G198:I198"/>
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="G207:I207"/>
+    <mergeCell ref="A211:I211"/>
+    <mergeCell ref="A214:A215"/>
+    <mergeCell ref="B214:D214"/>
+    <mergeCell ref="E214:F214"/>
+    <mergeCell ref="G214:I214"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="G209:I209"/>
+    <mergeCell ref="A213:I213"/>
+    <mergeCell ref="B207:D207"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13392,8 +13392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ya llamo los programs
</commit_message>
<xml_diff>
--- a/Versión Página web. Calendario Academico UR 2021. V. 17-11-2020 CAMBIOS.xlsx
+++ b/Versión Página web. Calendario Academico UR 2021. V. 17-11-2020 CAMBIOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_33946041C23A0D7F2B53E0C4FFB685BA09870FAE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{640389F9-EF47-451F-9A39-377143ACBA6C}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_33946041C23A0D7F2B53E0C4FFB685BA09870FAE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2EAF4497-F60A-49D5-9A27-90CAD44C79AA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 " sheetId="4" state="hidden" r:id="rId1"/>
@@ -3958,17 +3958,29 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4000,6 +4012,57 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4009,253 +4072,31 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4264,10 +4105,10 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4312,58 +4153,217 @@
     <xf numFmtId="164" fontId="7" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4680,63 +4680,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="197" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="243"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
     </row>
     <row r="2" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="321"/>
-      <c r="B2" s="321"/>
-      <c r="C2" s="321"/>
-      <c r="D2" s="321"/>
-      <c r="E2" s="321"/>
-      <c r="F2" s="321"/>
-      <c r="G2" s="321"/>
-      <c r="H2" s="321"/>
-      <c r="I2" s="321"/>
+      <c r="A2" s="198"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
     </row>
     <row r="3" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="243" t="s">
+      <c r="A3" s="197" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="243"/>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
-      <c r="E3" s="243"/>
-      <c r="F3" s="243"/>
-      <c r="G3" s="243"/>
-      <c r="H3" s="243"/>
-      <c r="I3" s="243"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
     </row>
     <row r="4" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="195" t="s">
+      <c r="A4" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="199"/>
-      <c r="E4" s="200" t="s">
+      <c r="C4" s="202"/>
+      <c r="D4" s="203"/>
+      <c r="E4" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="201"/>
-      <c r="G4" s="202" t="s">
+      <c r="F4" s="205"/>
+      <c r="G4" s="206" t="s">
         <v>163</v>
       </c>
-      <c r="H4" s="203"/>
-      <c r="I4" s="204"/>
+      <c r="H4" s="207"/>
+      <c r="I4" s="208"/>
     </row>
     <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="196"/>
+      <c r="A5" s="200"/>
       <c r="B5" s="48" t="s">
         <v>113</v>
       </c>
@@ -4822,63 +4822,63 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="194" t="s">
+      <c r="A9" s="209" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
+      <c r="B9" s="209"/>
+      <c r="C9" s="209"/>
+      <c r="D9" s="209"/>
+      <c r="E9" s="209"/>
+      <c r="F9" s="209"/>
+      <c r="G9" s="209"/>
+      <c r="H9" s="209"/>
+      <c r="I9" s="209"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="310"/>
-      <c r="B10" s="310"/>
-      <c r="C10" s="310"/>
-      <c r="D10" s="310"/>
-      <c r="E10" s="310"/>
-      <c r="F10" s="310"/>
-      <c r="G10" s="310"/>
-      <c r="H10" s="310"/>
-      <c r="I10" s="310"/>
+      <c r="A10" s="220"/>
+      <c r="B10" s="220"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="220"/>
+      <c r="H10" s="220"/>
+      <c r="I10" s="220"/>
     </row>
     <row r="11" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="243" t="s">
+      <c r="A11" s="197" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="243"/>
-      <c r="C11" s="243"/>
-      <c r="D11" s="243"/>
-      <c r="E11" s="243"/>
-      <c r="F11" s="243"/>
-      <c r="G11" s="243"/>
-      <c r="H11" s="243"/>
-      <c r="I11" s="243"/>
+      <c r="B11" s="197"/>
+      <c r="C11" s="197"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
     </row>
     <row r="12" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="197" t="s">
+      <c r="B12" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="198"/>
-      <c r="D12" s="199"/>
-      <c r="E12" s="200" t="s">
+      <c r="C12" s="202"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="201"/>
-      <c r="G12" s="202" t="s">
+      <c r="F12" s="205"/>
+      <c r="G12" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="203"/>
-      <c r="I12" s="204"/>
+      <c r="H12" s="207"/>
+      <c r="I12" s="208"/>
     </row>
     <row r="13" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="196"/>
+      <c r="A13" s="200"/>
       <c r="B13" s="48" t="s">
         <v>113</v>
       </c>
@@ -4978,33 +4978,33 @@
       <c r="A18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="212">
+      <c r="B18" s="191">
         <v>43794</v>
       </c>
-      <c r="C18" s="213"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="212">
+      <c r="C18" s="192"/>
+      <c r="D18" s="193"/>
+      <c r="E18" s="191">
         <v>43924</v>
       </c>
-      <c r="F18" s="214"/>
-      <c r="G18" s="191">
+      <c r="F18" s="193"/>
+      <c r="G18" s="210">
         <v>43974</v>
       </c>
-      <c r="H18" s="193"/>
-      <c r="I18" s="192"/>
+      <c r="H18" s="211"/>
+      <c r="I18" s="212"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="194" t="s">
+      <c r="A19" s="209" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="194"/>
-      <c r="C19" s="194"/>
-      <c r="D19" s="194"/>
-      <c r="E19" s="194"/>
-      <c r="F19" s="194"/>
-      <c r="G19" s="194"/>
-      <c r="H19" s="194"/>
-      <c r="I19" s="194"/>
+      <c r="B19" s="209"/>
+      <c r="C19" s="209"/>
+      <c r="D19" s="209"/>
+      <c r="E19" s="209"/>
+      <c r="F19" s="209"/>
+      <c r="G19" s="209"/>
+      <c r="H19" s="209"/>
+      <c r="I19" s="209"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
@@ -5018,63 +5018,63 @@
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="243" t="s">
+      <c r="A21" s="197" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="243"/>
-      <c r="C21" s="243"/>
-      <c r="D21" s="243"/>
-      <c r="E21" s="243"/>
-      <c r="F21" s="243"/>
-      <c r="G21" s="243"/>
-      <c r="H21" s="243"/>
-      <c r="I21" s="243"/>
+      <c r="B21" s="197"/>
+      <c r="C21" s="197"/>
+      <c r="D21" s="197"/>
+      <c r="E21" s="197"/>
+      <c r="F21" s="197"/>
+      <c r="G21" s="197"/>
+      <c r="H21" s="197"/>
+      <c r="I21" s="197"/>
     </row>
     <row r="22" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="322" t="s">
+      <c r="A22" s="213" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="197" t="s">
+      <c r="B22" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="198"/>
-      <c r="D22" s="199"/>
-      <c r="E22" s="325" t="s">
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="216" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="326"/>
-      <c r="G22" s="202" t="s">
+      <c r="F22" s="217"/>
+      <c r="G22" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="203"/>
-      <c r="I22" s="204"/>
+      <c r="H22" s="207"/>
+      <c r="I22" s="208"/>
     </row>
     <row r="23" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="323"/>
-      <c r="B23" s="238" t="s">
+      <c r="A23" s="214"/>
+      <c r="B23" s="218" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="198" t="s">
+      <c r="C23" s="202" t="s">
         <v>184</v>
       </c>
-      <c r="D23" s="199"/>
+      <c r="D23" s="203"/>
       <c r="E23" s="119" t="s">
         <v>148</v>
       </c>
       <c r="F23" s="118" t="s">
         <v>112</v>
       </c>
-      <c r="G23" s="318" t="s">
+      <c r="G23" s="229" t="s">
         <v>185</v>
       </c>
-      <c r="H23" s="202" t="s">
+      <c r="H23" s="206" t="s">
         <v>184</v>
       </c>
-      <c r="I23" s="204"/>
+      <c r="I23" s="208"/>
     </row>
     <row r="24" spans="1:9" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="324"/>
-      <c r="B24" s="239"/>
+      <c r="A24" s="215"/>
+      <c r="B24" s="219"/>
       <c r="C24" s="117">
         <v>0.05</v>
       </c>
@@ -5087,7 +5087,7 @@
       <c r="F24" s="115" t="s">
         <v>182</v>
       </c>
-      <c r="G24" s="319"/>
+      <c r="G24" s="230"/>
       <c r="H24" s="114">
         <v>0.05</v>
       </c>
@@ -5249,30 +5249,30 @@
       <c r="A31" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="212">
+      <c r="B31" s="191">
         <v>43857</v>
       </c>
-      <c r="C31" s="213"/>
-      <c r="D31" s="214"/>
+      <c r="C31" s="192"/>
+      <c r="D31" s="193"/>
       <c r="E31" s="112"/>
       <c r="F31" s="112"/>
-      <c r="G31" s="293">
+      <c r="G31" s="194">
         <v>44046</v>
       </c>
-      <c r="H31" s="320"/>
-      <c r="I31" s="294"/>
+      <c r="H31" s="195"/>
+      <c r="I31" s="196"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="212"/>
-      <c r="C32" s="213"/>
-      <c r="D32" s="214"/>
-      <c r="E32" s="293">
+      <c r="B32" s="191"/>
+      <c r="C32" s="192"/>
+      <c r="D32" s="193"/>
+      <c r="E32" s="194">
         <v>43626</v>
       </c>
-      <c r="F32" s="294"/>
+      <c r="F32" s="196"/>
       <c r="G32" s="52"/>
       <c r="H32" s="108"/>
       <c r="I32" s="51"/>
@@ -5281,77 +5281,77 @@
       <c r="A33" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="212">
+      <c r="B33" s="191">
         <v>43781</v>
       </c>
-      <c r="C33" s="213"/>
-      <c r="D33" s="214"/>
-      <c r="E33" s="293"/>
-      <c r="F33" s="294"/>
-      <c r="G33" s="212">
+      <c r="C33" s="192"/>
+      <c r="D33" s="193"/>
+      <c r="E33" s="194"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="191">
         <v>43964</v>
       </c>
-      <c r="H33" s="213"/>
-      <c r="I33" s="214"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="193"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="208" t="s">
+      <c r="A34" s="225" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="208"/>
-      <c r="C34" s="208"/>
-      <c r="D34" s="208"/>
-      <c r="E34" s="208"/>
-      <c r="F34" s="208"/>
-      <c r="G34" s="208"/>
-      <c r="H34" s="208"/>
-      <c r="I34" s="208"/>
+      <c r="B34" s="225"/>
+      <c r="C34" s="225"/>
+      <c r="D34" s="225"/>
+      <c r="E34" s="225"/>
+      <c r="F34" s="225"/>
+      <c r="G34" s="225"/>
+      <c r="H34" s="225"/>
+      <c r="I34" s="225"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="191"/>
-      <c r="B35" s="193"/>
-      <c r="C35" s="193"/>
-      <c r="D35" s="193"/>
-      <c r="E35" s="193"/>
-      <c r="F35" s="193"/>
-      <c r="G35" s="193"/>
-      <c r="H35" s="193"/>
-      <c r="I35" s="192"/>
+      <c r="A35" s="210"/>
+      <c r="B35" s="211"/>
+      <c r="C35" s="211"/>
+      <c r="D35" s="211"/>
+      <c r="E35" s="211"/>
+      <c r="F35" s="211"/>
+      <c r="G35" s="211"/>
+      <c r="H35" s="211"/>
+      <c r="I35" s="212"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="205" t="s">
+      <c r="A36" s="226" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="206"/>
-      <c r="C36" s="206"/>
-      <c r="D36" s="206"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="207"/>
+      <c r="B36" s="227"/>
+      <c r="C36" s="227"/>
+      <c r="D36" s="227"/>
+      <c r="E36" s="227"/>
+      <c r="F36" s="227"/>
+      <c r="G36" s="227"/>
+      <c r="H36" s="227"/>
+      <c r="I36" s="228"/>
     </row>
     <row r="37" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="195" t="s">
+      <c r="A37" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="197" t="s">
+      <c r="B37" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="198"/>
-      <c r="D37" s="199"/>
-      <c r="E37" s="200" t="s">
+      <c r="C37" s="202"/>
+      <c r="D37" s="203"/>
+      <c r="E37" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="201"/>
-      <c r="G37" s="202" t="s">
+      <c r="F37" s="205"/>
+      <c r="G37" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H37" s="203"/>
-      <c r="I37" s="204"/>
+      <c r="H37" s="207"/>
+      <c r="I37" s="208"/>
     </row>
     <row r="38" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="196"/>
+      <c r="A38" s="200"/>
       <c r="B38" s="48" t="s">
         <v>113</v>
       </c>
@@ -5402,18 +5402,18 @@
       <c r="A40" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="212">
+      <c r="B40" s="191">
         <v>43846</v>
       </c>
-      <c r="C40" s="213"/>
-      <c r="D40" s="214"/>
-      <c r="E40" s="313"/>
-      <c r="F40" s="315"/>
-      <c r="G40" s="212">
+      <c r="C40" s="192"/>
+      <c r="D40" s="193"/>
+      <c r="E40" s="223"/>
+      <c r="F40" s="224"/>
+      <c r="G40" s="191">
         <v>44035</v>
       </c>
-      <c r="H40" s="213"/>
-      <c r="I40" s="214"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="193"/>
     </row>
     <row r="41" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A41" s="81" t="s">
@@ -5451,8 +5451,8 @@
       <c r="D42" s="14">
         <v>43816</v>
       </c>
-      <c r="E42" s="212"/>
-      <c r="F42" s="214"/>
+      <c r="E42" s="191"/>
+      <c r="F42" s="193"/>
       <c r="G42" s="15">
         <v>44000</v>
       </c>
@@ -5511,22 +5511,22 @@
       <c r="A45" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="212">
+      <c r="B45" s="191">
         <v>43837</v>
       </c>
-      <c r="C45" s="213"/>
-      <c r="D45" s="214"/>
+      <c r="C45" s="192"/>
+      <c r="D45" s="193"/>
       <c r="E45" s="14">
         <v>43616</v>
       </c>
       <c r="F45" s="14">
         <v>43619</v>
       </c>
-      <c r="G45" s="191">
+      <c r="G45" s="210">
         <v>44018</v>
       </c>
-      <c r="H45" s="193"/>
-      <c r="I45" s="192"/>
+      <c r="H45" s="211"/>
+      <c r="I45" s="212"/>
     </row>
     <row r="46" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A46" s="81" t="s">
@@ -5574,9 +5574,9 @@
       <c r="A48" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="212"/>
-      <c r="C48" s="213"/>
-      <c r="D48" s="214"/>
+      <c r="B48" s="191"/>
+      <c r="C48" s="192"/>
+      <c r="D48" s="193"/>
       <c r="E48" s="107"/>
       <c r="F48" s="106"/>
       <c r="G48" s="15">
@@ -5588,17 +5588,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="194" t="s">
+      <c r="A49" s="209" t="s">
         <v>172</v>
       </c>
-      <c r="B49" s="194"/>
-      <c r="C49" s="194"/>
-      <c r="D49" s="194"/>
-      <c r="E49" s="194"/>
-      <c r="F49" s="194"/>
-      <c r="G49" s="194"/>
-      <c r="H49" s="194"/>
-      <c r="I49" s="194"/>
+      <c r="B49" s="209"/>
+      <c r="C49" s="209"/>
+      <c r="D49" s="209"/>
+      <c r="E49" s="209"/>
+      <c r="F49" s="209"/>
+      <c r="G49" s="209"/>
+      <c r="H49" s="209"/>
+      <c r="I49" s="209"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="105"/>
@@ -5612,39 +5612,39 @@
       <c r="I50" s="105"/>
     </row>
     <row r="51" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="205" t="s">
+      <c r="A51" s="226" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="206"/>
-      <c r="C51" s="206"/>
-      <c r="D51" s="206"/>
-      <c r="E51" s="206"/>
-      <c r="F51" s="206"/>
-      <c r="G51" s="206"/>
-      <c r="H51" s="206"/>
-      <c r="I51" s="207"/>
+      <c r="B51" s="227"/>
+      <c r="C51" s="227"/>
+      <c r="D51" s="227"/>
+      <c r="E51" s="227"/>
+      <c r="F51" s="227"/>
+      <c r="G51" s="227"/>
+      <c r="H51" s="227"/>
+      <c r="I51" s="228"/>
     </row>
     <row r="52" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="195" t="s">
+      <c r="A52" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="197" t="s">
+      <c r="B52" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="198"/>
-      <c r="D52" s="199"/>
-      <c r="E52" s="200" t="s">
+      <c r="C52" s="202"/>
+      <c r="D52" s="203"/>
+      <c r="E52" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="201"/>
-      <c r="G52" s="202" t="s">
+      <c r="F52" s="205"/>
+      <c r="G52" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="203"/>
-      <c r="I52" s="204"/>
+      <c r="H52" s="207"/>
+      <c r="I52" s="208"/>
     </row>
     <row r="53" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="257"/>
+      <c r="A53" s="231"/>
       <c r="B53" s="25" t="s">
         <v>113</v>
       </c>
@@ -5670,67 +5670,67 @@
       <c r="A54" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="316">
+      <c r="B54" s="221">
         <v>43817</v>
       </c>
-      <c r="C54" s="316"/>
-      <c r="D54" s="316"/>
-      <c r="E54" s="316"/>
-      <c r="F54" s="316"/>
-      <c r="G54" s="317">
+      <c r="C54" s="221"/>
+      <c r="D54" s="221"/>
+      <c r="E54" s="221"/>
+      <c r="F54" s="221"/>
+      <c r="G54" s="222">
         <v>44005</v>
       </c>
-      <c r="H54" s="317"/>
-      <c r="I54" s="317"/>
+      <c r="H54" s="222"/>
+      <c r="I54" s="222"/>
     </row>
     <row r="55" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B55" s="209">
+      <c r="B55" s="232">
         <v>43840</v>
       </c>
-      <c r="C55" s="209"/>
-      <c r="D55" s="209"/>
-      <c r="E55" s="209"/>
-      <c r="F55" s="209"/>
-      <c r="G55" s="247">
+      <c r="C55" s="232"/>
+      <c r="D55" s="232"/>
+      <c r="E55" s="232"/>
+      <c r="F55" s="232"/>
+      <c r="G55" s="233">
         <v>44018</v>
       </c>
-      <c r="H55" s="247"/>
-      <c r="I55" s="247"/>
+      <c r="H55" s="233"/>
+      <c r="I55" s="233"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="209">
+      <c r="B56" s="232">
         <v>43844</v>
       </c>
-      <c r="C56" s="209"/>
-      <c r="D56" s="209"/>
-      <c r="E56" s="209"/>
-      <c r="F56" s="209"/>
-      <c r="G56" s="247">
+      <c r="C56" s="232"/>
+      <c r="D56" s="232"/>
+      <c r="E56" s="232"/>
+      <c r="F56" s="232"/>
+      <c r="G56" s="233">
         <v>44029</v>
       </c>
-      <c r="H56" s="247"/>
-      <c r="I56" s="247"/>
+      <c r="H56" s="233"/>
+      <c r="I56" s="233"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="209"/>
-      <c r="C57" s="209"/>
-      <c r="D57" s="209"/>
-      <c r="E57" s="209">
+      <c r="B57" s="232"/>
+      <c r="C57" s="232"/>
+      <c r="D57" s="232"/>
+      <c r="E57" s="232">
         <v>43984</v>
       </c>
-      <c r="F57" s="209"/>
-      <c r="G57" s="247"/>
-      <c r="H57" s="247"/>
-      <c r="I57" s="247"/>
+      <c r="F57" s="232"/>
+      <c r="G57" s="233"/>
+      <c r="H57" s="233"/>
+      <c r="I57" s="233"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="81" t="s">
@@ -5743,8 +5743,8 @@
       <c r="D58" s="15">
         <v>43858</v>
       </c>
-      <c r="E58" s="209"/>
-      <c r="F58" s="209"/>
+      <c r="E58" s="232"/>
+      <c r="F58" s="232"/>
       <c r="G58" s="15">
         <v>44035</v>
       </c>
@@ -5754,17 +5754,17 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="208" t="s">
+      <c r="A59" s="225" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="208"/>
-      <c r="C59" s="208"/>
-      <c r="D59" s="208"/>
-      <c r="E59" s="208"/>
-      <c r="F59" s="208"/>
-      <c r="G59" s="208"/>
-      <c r="H59" s="208"/>
-      <c r="I59" s="208"/>
+      <c r="B59" s="225"/>
+      <c r="C59" s="225"/>
+      <c r="D59" s="225"/>
+      <c r="E59" s="225"/>
+      <c r="F59" s="225"/>
+      <c r="G59" s="225"/>
+      <c r="H59" s="225"/>
+      <c r="I59" s="225"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="53"/>
@@ -5778,39 +5778,39 @@
       <c r="I60" s="53"/>
     </row>
     <row r="61" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="243" t="s">
+      <c r="A61" s="197" t="s">
         <v>30</v>
       </c>
-      <c r="B61" s="243"/>
-      <c r="C61" s="243"/>
-      <c r="D61" s="243"/>
-      <c r="E61" s="243"/>
-      <c r="F61" s="243"/>
-      <c r="G61" s="243"/>
-      <c r="H61" s="243"/>
-      <c r="I61" s="243"/>
+      <c r="B61" s="197"/>
+      <c r="C61" s="197"/>
+      <c r="D61" s="197"/>
+      <c r="E61" s="197"/>
+      <c r="F61" s="197"/>
+      <c r="G61" s="197"/>
+      <c r="H61" s="197"/>
+      <c r="I61" s="197"/>
     </row>
     <row r="62" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="195" t="s">
+      <c r="A62" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="197" t="s">
+      <c r="B62" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C62" s="198"/>
-      <c r="D62" s="199"/>
-      <c r="E62" s="200" t="s">
+      <c r="C62" s="202"/>
+      <c r="D62" s="203"/>
+      <c r="E62" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F62" s="201"/>
-      <c r="G62" s="202" t="s">
+      <c r="F62" s="205"/>
+      <c r="G62" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H62" s="203"/>
-      <c r="I62" s="204"/>
+      <c r="H62" s="207"/>
+      <c r="I62" s="208"/>
     </row>
     <row r="63" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="196"/>
+      <c r="A63" s="200"/>
       <c r="B63" s="48" t="s">
         <v>113</v>
       </c>
@@ -5836,145 +5836,145 @@
       <c r="A64" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B64" s="313">
+      <c r="B64" s="223">
         <v>43818</v>
       </c>
-      <c r="C64" s="314"/>
-      <c r="D64" s="315"/>
-      <c r="E64" s="313"/>
-      <c r="F64" s="315"/>
-      <c r="G64" s="191">
+      <c r="C64" s="234"/>
+      <c r="D64" s="224"/>
+      <c r="E64" s="223"/>
+      <c r="F64" s="224"/>
+      <c r="G64" s="210">
         <v>44006</v>
       </c>
-      <c r="H64" s="193"/>
-      <c r="I64" s="192"/>
+      <c r="H64" s="211"/>
+      <c r="I64" s="212"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="212">
+      <c r="B65" s="191">
         <v>43843</v>
       </c>
-      <c r="C65" s="213"/>
-      <c r="D65" s="214"/>
-      <c r="E65" s="212"/>
-      <c r="F65" s="214"/>
-      <c r="G65" s="191">
+      <c r="C65" s="192"/>
+      <c r="D65" s="193"/>
+      <c r="E65" s="191"/>
+      <c r="F65" s="193"/>
+      <c r="G65" s="210">
         <v>44020</v>
       </c>
-      <c r="H65" s="193"/>
-      <c r="I65" s="192"/>
+      <c r="H65" s="211"/>
+      <c r="I65" s="212"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B66" s="212" t="s">
+      <c r="B66" s="191" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="213"/>
-      <c r="D66" s="214"/>
-      <c r="E66" s="212"/>
-      <c r="F66" s="214"/>
-      <c r="G66" s="191" t="s">
+      <c r="C66" s="192"/>
+      <c r="D66" s="193"/>
+      <c r="E66" s="191"/>
+      <c r="F66" s="193"/>
+      <c r="G66" s="210" t="s">
         <v>169</v>
       </c>
-      <c r="H66" s="193"/>
-      <c r="I66" s="192"/>
+      <c r="H66" s="211"/>
+      <c r="I66" s="212"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="212" t="s">
+      <c r="B67" s="191" t="s">
         <v>168</v>
       </c>
-      <c r="C67" s="213"/>
-      <c r="D67" s="214"/>
-      <c r="E67" s="212"/>
-      <c r="F67" s="214"/>
-      <c r="G67" s="191">
+      <c r="C67" s="192"/>
+      <c r="D67" s="193"/>
+      <c r="E67" s="191"/>
+      <c r="F67" s="193"/>
+      <c r="G67" s="210">
         <v>44035</v>
       </c>
-      <c r="H67" s="193"/>
-      <c r="I67" s="192"/>
+      <c r="H67" s="211"/>
+      <c r="I67" s="212"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="212">
+      <c r="B68" s="191">
         <v>43847</v>
       </c>
-      <c r="C68" s="213"/>
-      <c r="D68" s="214"/>
-      <c r="E68" s="209">
+      <c r="C68" s="192"/>
+      <c r="D68" s="193"/>
+      <c r="E68" s="232">
         <v>43985</v>
       </c>
-      <c r="F68" s="209"/>
-      <c r="G68" s="191">
+      <c r="F68" s="232"/>
+      <c r="G68" s="210">
         <v>44036</v>
       </c>
-      <c r="H68" s="193"/>
-      <c r="I68" s="192"/>
+      <c r="H68" s="211"/>
+      <c r="I68" s="212"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="309"/>
-      <c r="B69" s="310"/>
-      <c r="C69" s="310"/>
-      <c r="D69" s="310"/>
-      <c r="E69" s="310"/>
-      <c r="F69" s="310"/>
-      <c r="G69" s="310"/>
-      <c r="H69" s="310"/>
-      <c r="I69" s="311"/>
+      <c r="A69" s="235"/>
+      <c r="B69" s="220"/>
+      <c r="C69" s="220"/>
+      <c r="D69" s="220"/>
+      <c r="E69" s="220"/>
+      <c r="F69" s="220"/>
+      <c r="G69" s="220"/>
+      <c r="H69" s="220"/>
+      <c r="I69" s="236"/>
     </row>
     <row r="70" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="297"/>
-      <c r="B70" s="298"/>
-      <c r="C70" s="298"/>
-      <c r="D70" s="298"/>
-      <c r="E70" s="298"/>
-      <c r="F70" s="298"/>
-      <c r="G70" s="298"/>
-      <c r="H70" s="298"/>
-      <c r="I70" s="299"/>
+      <c r="A70" s="244"/>
+      <c r="B70" s="245"/>
+      <c r="C70" s="245"/>
+      <c r="D70" s="245"/>
+      <c r="E70" s="245"/>
+      <c r="F70" s="245"/>
+      <c r="G70" s="245"/>
+      <c r="H70" s="245"/>
+      <c r="I70" s="246"/>
     </row>
     <row r="71" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="300" t="s">
+      <c r="A71" s="247" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="301"/>
-      <c r="C71" s="301"/>
-      <c r="D71" s="301"/>
-      <c r="E71" s="301"/>
-      <c r="F71" s="301"/>
-      <c r="G71" s="301"/>
-      <c r="H71" s="302"/>
-      <c r="I71" s="303"/>
+      <c r="B71" s="248"/>
+      <c r="C71" s="248"/>
+      <c r="D71" s="248"/>
+      <c r="E71" s="248"/>
+      <c r="F71" s="248"/>
+      <c r="G71" s="248"/>
+      <c r="H71" s="249"/>
+      <c r="I71" s="250"/>
     </row>
     <row r="72" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="312" t="s">
+      <c r="A72" s="237" t="s">
         <v>117</v>
       </c>
-      <c r="B72" s="197" t="s">
+      <c r="B72" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="198"/>
-      <c r="D72" s="199"/>
-      <c r="E72" s="200" t="s">
+      <c r="C72" s="202"/>
+      <c r="D72" s="203"/>
+      <c r="E72" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F72" s="201"/>
-      <c r="G72" s="202" t="s">
+      <c r="F72" s="205"/>
+      <c r="G72" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H72" s="203"/>
-      <c r="I72" s="204"/>
+      <c r="H72" s="207"/>
+      <c r="I72" s="208"/>
     </row>
     <row r="73" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="239"/>
+      <c r="A73" s="219"/>
       <c r="B73" s="25" t="s">
         <v>113</v>
       </c>
@@ -6000,13 +6000,13 @@
       <c r="A74" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="304" t="s">
+      <c r="B74" s="251" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="305"/>
-      <c r="D74" s="306"/>
-      <c r="E74" s="307"/>
-      <c r="F74" s="308"/>
+      <c r="C74" s="252"/>
+      <c r="D74" s="253"/>
+      <c r="E74" s="254"/>
+      <c r="F74" s="255"/>
       <c r="G74" s="103">
         <v>44034</v>
       </c>
@@ -6026,8 +6026,8 @@
       <c r="D75" s="100">
         <v>43847</v>
       </c>
-      <c r="E75" s="293"/>
-      <c r="F75" s="294"/>
+      <c r="E75" s="194"/>
+      <c r="F75" s="196"/>
       <c r="G75" s="41">
         <v>44036</v>
       </c>
@@ -6047,8 +6047,8 @@
       <c r="D76" s="100">
         <v>43845</v>
       </c>
-      <c r="E76" s="291"/>
-      <c r="F76" s="292"/>
+      <c r="E76" s="238"/>
+      <c r="F76" s="239"/>
       <c r="G76" s="41">
         <v>44034</v>
       </c>
@@ -6089,8 +6089,8 @@
       <c r="D78" s="96">
         <v>43847</v>
       </c>
-      <c r="E78" s="291"/>
-      <c r="F78" s="292"/>
+      <c r="E78" s="238"/>
+      <c r="F78" s="239"/>
       <c r="G78" s="41">
         <v>44036</v>
       </c>
@@ -6103,26 +6103,26 @@
       <c r="A79" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="291"/>
-      <c r="C79" s="295"/>
-      <c r="D79" s="292"/>
-      <c r="E79" s="293"/>
-      <c r="F79" s="294"/>
-      <c r="G79" s="291"/>
-      <c r="H79" s="295"/>
-      <c r="I79" s="296"/>
+      <c r="B79" s="238"/>
+      <c r="C79" s="242"/>
+      <c r="D79" s="239"/>
+      <c r="E79" s="194"/>
+      <c r="F79" s="196"/>
+      <c r="G79" s="238"/>
+      <c r="H79" s="242"/>
+      <c r="I79" s="243"/>
     </row>
     <row r="80" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A80" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="291">
+      <c r="B80" s="238">
         <v>43848</v>
       </c>
-      <c r="C80" s="295"/>
-      <c r="D80" s="292"/>
-      <c r="E80" s="293"/>
-      <c r="F80" s="294"/>
+      <c r="C80" s="242"/>
+      <c r="D80" s="239"/>
+      <c r="E80" s="194"/>
+      <c r="F80" s="196"/>
       <c r="G80" s="41">
         <v>44037</v>
       </c>
@@ -6142,8 +6142,8 @@
       <c r="D81" s="15">
         <v>43921</v>
       </c>
-      <c r="E81" s="254"/>
-      <c r="F81" s="255"/>
+      <c r="E81" s="240"/>
+      <c r="F81" s="241"/>
       <c r="G81" s="41">
         <v>44033</v>
       </c>
@@ -6153,17 +6153,17 @@
       </c>
     </row>
     <row r="82" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="277" t="s">
+      <c r="A82" s="263" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="278"/>
-      <c r="C82" s="278"/>
-      <c r="D82" s="278"/>
-      <c r="E82" s="279"/>
-      <c r="F82" s="279"/>
-      <c r="G82" s="279"/>
-      <c r="H82" s="279"/>
-      <c r="I82" s="280"/>
+      <c r="B82" s="264"/>
+      <c r="C82" s="264"/>
+      <c r="D82" s="264"/>
+      <c r="E82" s="265"/>
+      <c r="F82" s="265"/>
+      <c r="G82" s="265"/>
+      <c r="H82" s="265"/>
+      <c r="I82" s="266"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="92"/>
@@ -6177,39 +6177,39 @@
       <c r="I83" s="91"/>
     </row>
     <row r="84" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="243" t="s">
+      <c r="A84" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="B84" s="243"/>
-      <c r="C84" s="243"/>
-      <c r="D84" s="243"/>
-      <c r="E84" s="243"/>
-      <c r="F84" s="243"/>
-      <c r="G84" s="243"/>
-      <c r="H84" s="243"/>
-      <c r="I84" s="243"/>
+      <c r="B84" s="197"/>
+      <c r="C84" s="197"/>
+      <c r="D84" s="197"/>
+      <c r="E84" s="197"/>
+      <c r="F84" s="197"/>
+      <c r="G84" s="197"/>
+      <c r="H84" s="197"/>
+      <c r="I84" s="197"/>
     </row>
     <row r="85" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="195" t="s">
+      <c r="A85" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="197" t="s">
+      <c r="B85" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="198"/>
-      <c r="D85" s="199"/>
-      <c r="E85" s="200" t="s">
+      <c r="C85" s="202"/>
+      <c r="D85" s="203"/>
+      <c r="E85" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F85" s="201"/>
-      <c r="G85" s="202" t="s">
+      <c r="F85" s="205"/>
+      <c r="G85" s="206" t="s">
         <v>163</v>
       </c>
-      <c r="H85" s="203"/>
-      <c r="I85" s="204"/>
+      <c r="H85" s="207"/>
+      <c r="I85" s="208"/>
     </row>
     <row r="86" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="196"/>
+      <c r="A86" s="200"/>
       <c r="B86" s="25" t="s">
         <v>113</v>
       </c>
@@ -6232,17 +6232,17 @@
       </c>
     </row>
     <row r="87" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="218" t="s">
+      <c r="A87" s="256" t="s">
         <v>162</v>
       </c>
-      <c r="B87" s="220"/>
-      <c r="C87" s="220"/>
-      <c r="D87" s="220"/>
-      <c r="E87" s="220"/>
-      <c r="F87" s="220"/>
-      <c r="G87" s="220"/>
-      <c r="H87" s="220"/>
-      <c r="I87" s="221"/>
+      <c r="B87" s="257"/>
+      <c r="C87" s="257"/>
+      <c r="D87" s="257"/>
+      <c r="E87" s="257"/>
+      <c r="F87" s="257"/>
+      <c r="G87" s="257"/>
+      <c r="H87" s="257"/>
+      <c r="I87" s="258"/>
     </row>
     <row r="88" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A88" s="81" t="s">
@@ -6324,18 +6324,18 @@
       <c r="A92" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="281">
+      <c r="B92" s="267">
         <v>43988</v>
       </c>
-      <c r="C92" s="282"/>
-      <c r="D92" s="283"/>
+      <c r="C92" s="268"/>
+      <c r="D92" s="269"/>
       <c r="E92" s="82"/>
       <c r="F92" s="82"/>
-      <c r="G92" s="281">
+      <c r="G92" s="267">
         <v>44170</v>
       </c>
-      <c r="H92" s="282"/>
-      <c r="I92" s="283"/>
+      <c r="H92" s="268"/>
+      <c r="I92" s="269"/>
     </row>
     <row r="93" spans="1:9" s="87" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A93" s="81" t="s">
@@ -6408,53 +6408,53 @@
       <c r="A96" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B96" s="284">
+      <c r="B96" s="270">
         <v>43974</v>
       </c>
-      <c r="C96" s="285"/>
-      <c r="D96" s="286"/>
+      <c r="C96" s="271"/>
+      <c r="D96" s="272"/>
       <c r="E96" s="82"/>
       <c r="F96" s="82"/>
-      <c r="G96" s="281">
+      <c r="G96" s="267">
         <v>44163</v>
       </c>
-      <c r="H96" s="282"/>
-      <c r="I96" s="283"/>
+      <c r="H96" s="268"/>
+      <c r="I96" s="269"/>
     </row>
     <row r="97" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="197" t="s">
+      <c r="A97" s="201" t="s">
         <v>160</v>
       </c>
-      <c r="B97" s="198"/>
-      <c r="C97" s="198"/>
-      <c r="D97" s="198"/>
-      <c r="E97" s="198"/>
-      <c r="F97" s="198"/>
-      <c r="G97" s="198"/>
-      <c r="H97" s="198"/>
-      <c r="I97" s="199"/>
+      <c r="B97" s="202"/>
+      <c r="C97" s="202"/>
+      <c r="D97" s="202"/>
+      <c r="E97" s="202"/>
+      <c r="F97" s="202"/>
+      <c r="G97" s="202"/>
+      <c r="H97" s="202"/>
+      <c r="I97" s="203"/>
     </row>
     <row r="98" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="195" t="s">
+      <c r="A98" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="197" t="s">
+      <c r="B98" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C98" s="198"/>
-      <c r="D98" s="199"/>
-      <c r="E98" s="200" t="s">
+      <c r="C98" s="202"/>
+      <c r="D98" s="203"/>
+      <c r="E98" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F98" s="201"/>
-      <c r="G98" s="202" t="s">
+      <c r="F98" s="205"/>
+      <c r="G98" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H98" s="203"/>
-      <c r="I98" s="204"/>
+      <c r="H98" s="207"/>
+      <c r="I98" s="208"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="257"/>
+      <c r="A99" s="231"/>
       <c r="B99" s="37" t="s">
         <v>113</v>
       </c>
@@ -6487,8 +6487,8 @@
       <c r="D100" s="15">
         <v>43960</v>
       </c>
-      <c r="E100" s="247"/>
-      <c r="F100" s="247"/>
+      <c r="E100" s="233"/>
+      <c r="F100" s="233"/>
       <c r="G100" s="82">
         <v>44046</v>
       </c>
@@ -6508,8 +6508,8 @@
       <c r="D101" s="15">
         <v>43967</v>
       </c>
-      <c r="E101" s="247"/>
-      <c r="F101" s="247"/>
+      <c r="E101" s="233"/>
+      <c r="F101" s="233"/>
       <c r="G101" s="15">
         <v>44152</v>
       </c>
@@ -6522,66 +6522,66 @@
       <c r="A102" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B102" s="247">
+      <c r="B102" s="233">
         <v>43967</v>
       </c>
-      <c r="C102" s="247"/>
-      <c r="D102" s="247"/>
-      <c r="E102" s="247"/>
-      <c r="F102" s="247"/>
-      <c r="G102" s="247">
+      <c r="C102" s="233"/>
+      <c r="D102" s="233"/>
+      <c r="E102" s="233"/>
+      <c r="F102" s="233"/>
+      <c r="G102" s="233">
         <v>44156</v>
       </c>
-      <c r="H102" s="247"/>
-      <c r="I102" s="247"/>
+      <c r="H102" s="233"/>
+      <c r="I102" s="233"/>
     </row>
     <row r="103" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="208" t="s">
+      <c r="A103" s="225" t="s">
         <v>159</v>
       </c>
-      <c r="B103" s="208"/>
-      <c r="C103" s="208"/>
-      <c r="D103" s="208"/>
-      <c r="E103" s="208"/>
-      <c r="F103" s="208"/>
-      <c r="G103" s="208"/>
-      <c r="H103" s="208"/>
-      <c r="I103" s="208"/>
+      <c r="B103" s="225"/>
+      <c r="C103" s="225"/>
+      <c r="D103" s="225"/>
+      <c r="E103" s="225"/>
+      <c r="F103" s="225"/>
+      <c r="G103" s="225"/>
+      <c r="H103" s="225"/>
+      <c r="I103" s="225"/>
     </row>
     <row r="104" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="218" t="s">
+      <c r="A104" s="256" t="s">
         <v>158</v>
       </c>
-      <c r="B104" s="220"/>
-      <c r="C104" s="220"/>
-      <c r="D104" s="220"/>
-      <c r="E104" s="220"/>
-      <c r="F104" s="220"/>
-      <c r="G104" s="220"/>
-      <c r="H104" s="220"/>
-      <c r="I104" s="221"/>
+      <c r="B104" s="257"/>
+      <c r="C104" s="257"/>
+      <c r="D104" s="257"/>
+      <c r="E104" s="257"/>
+      <c r="F104" s="257"/>
+      <c r="G104" s="257"/>
+      <c r="H104" s="257"/>
+      <c r="I104" s="258"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="238" t="s">
+      <c r="A105" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B105" s="287" t="s">
+      <c r="B105" s="259" t="s">
         <v>116</v>
       </c>
-      <c r="C105" s="288"/>
-      <c r="D105" s="288"/>
-      <c r="E105" s="289" t="s">
+      <c r="C105" s="260"/>
+      <c r="D105" s="260"/>
+      <c r="E105" s="261" t="s">
         <v>115</v>
       </c>
-      <c r="F105" s="289"/>
-      <c r="G105" s="290" t="s">
+      <c r="F105" s="261"/>
+      <c r="G105" s="262" t="s">
         <v>114</v>
       </c>
-      <c r="H105" s="290"/>
-      <c r="I105" s="290"/>
+      <c r="H105" s="262"/>
+      <c r="I105" s="262"/>
     </row>
     <row r="106" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="239"/>
+      <c r="A106" s="219"/>
       <c r="B106" s="80" t="s">
         <v>113</v>
       </c>
@@ -6614,8 +6614,8 @@
       <c r="D107" s="15">
         <v>43967</v>
       </c>
-      <c r="E107" s="247"/>
-      <c r="F107" s="247"/>
+      <c r="E107" s="233"/>
+      <c r="F107" s="233"/>
       <c r="G107" s="15">
         <v>44046</v>
       </c>
@@ -6638,17 +6638,17 @@
       <c r="I108" s="74"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="208" t="s">
+      <c r="A109" s="225" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="208"/>
-      <c r="C109" s="208"/>
-      <c r="D109" s="208"/>
-      <c r="E109" s="208"/>
-      <c r="F109" s="208"/>
-      <c r="G109" s="208"/>
-      <c r="H109" s="208"/>
-      <c r="I109" s="208"/>
+      <c r="B109" s="225"/>
+      <c r="C109" s="225"/>
+      <c r="D109" s="225"/>
+      <c r="E109" s="225"/>
+      <c r="F109" s="225"/>
+      <c r="G109" s="225"/>
+      <c r="H109" s="225"/>
+      <c r="I109" s="225"/>
     </row>
     <row r="110" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="73"/>
@@ -6662,39 +6662,39 @@
       <c r="I110" s="73"/>
     </row>
     <row r="111" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="263" t="s">
+      <c r="A111" s="275" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="264"/>
-      <c r="C111" s="264"/>
-      <c r="D111" s="264"/>
-      <c r="E111" s="264"/>
-      <c r="F111" s="264"/>
-      <c r="G111" s="264"/>
-      <c r="H111" s="264"/>
-      <c r="I111" s="265"/>
+      <c r="B111" s="276"/>
+      <c r="C111" s="276"/>
+      <c r="D111" s="276"/>
+      <c r="E111" s="276"/>
+      <c r="F111" s="276"/>
+      <c r="G111" s="276"/>
+      <c r="H111" s="276"/>
+      <c r="I111" s="277"/>
     </row>
     <row r="112" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="266" t="s">
+      <c r="A112" s="281" t="s">
         <v>117</v>
       </c>
-      <c r="B112" s="268" t="s">
+      <c r="B112" s="283" t="s">
         <v>190</v>
       </c>
-      <c r="C112" s="269"/>
-      <c r="D112" s="270"/>
-      <c r="E112" s="271" t="s">
+      <c r="C112" s="284"/>
+      <c r="D112" s="285"/>
+      <c r="E112" s="286" t="s">
         <v>115</v>
       </c>
-      <c r="F112" s="272"/>
-      <c r="G112" s="273" t="s">
+      <c r="F112" s="287"/>
+      <c r="G112" s="288" t="s">
         <v>163</v>
       </c>
-      <c r="H112" s="274"/>
-      <c r="I112" s="275"/>
+      <c r="H112" s="289"/>
+      <c r="I112" s="290"/>
     </row>
     <row r="113" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="267"/>
+      <c r="A113" s="282"/>
       <c r="B113" s="124" t="s">
         <v>113</v>
       </c>
@@ -6720,149 +6720,149 @@
       <c r="A114" s="127" t="s">
         <v>191</v>
       </c>
-      <c r="B114" s="232">
+      <c r="B114" s="278">
         <v>43971</v>
       </c>
-      <c r="C114" s="233"/>
-      <c r="D114" s="234"/>
+      <c r="C114" s="279"/>
+      <c r="D114" s="280"/>
       <c r="E114" s="128"/>
       <c r="F114" s="128"/>
-      <c r="G114" s="232">
+      <c r="G114" s="278">
         <v>44158</v>
       </c>
-      <c r="H114" s="233"/>
-      <c r="I114" s="234"/>
+      <c r="H114" s="279"/>
+      <c r="I114" s="280"/>
     </row>
     <row r="115" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="B115" s="232">
+      <c r="B115" s="278">
         <v>43978</v>
       </c>
-      <c r="C115" s="233"/>
-      <c r="D115" s="234"/>
-      <c r="E115" s="232">
+      <c r="C115" s="279"/>
+      <c r="D115" s="280"/>
+      <c r="E115" s="278">
         <v>44029</v>
       </c>
-      <c r="F115" s="234"/>
-      <c r="G115" s="232">
+      <c r="F115" s="280"/>
+      <c r="G115" s="278">
         <v>44166</v>
       </c>
-      <c r="H115" s="233"/>
-      <c r="I115" s="234"/>
+      <c r="H115" s="279"/>
+      <c r="I115" s="280"/>
     </row>
     <row r="116" spans="1:9" ht="61.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="129" t="s">
         <v>192</v>
       </c>
-      <c r="B116" s="232">
+      <c r="B116" s="278">
         <v>43991</v>
       </c>
-      <c r="C116" s="233"/>
-      <c r="D116" s="234"/>
-      <c r="E116" s="235"/>
-      <c r="F116" s="236"/>
-      <c r="G116" s="235" t="s">
+      <c r="C116" s="279"/>
+      <c r="D116" s="280"/>
+      <c r="E116" s="273"/>
+      <c r="F116" s="274"/>
+      <c r="G116" s="273" t="s">
         <v>193</v>
       </c>
-      <c r="H116" s="276"/>
-      <c r="I116" s="236"/>
+      <c r="H116" s="291"/>
+      <c r="I116" s="274"/>
     </row>
     <row r="117" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="B117" s="232">
+      <c r="B117" s="278">
         <v>43979</v>
       </c>
-      <c r="C117" s="233"/>
-      <c r="D117" s="234"/>
-      <c r="E117" s="232">
+      <c r="C117" s="279"/>
+      <c r="D117" s="280"/>
+      <c r="E117" s="278">
         <v>44029</v>
       </c>
-      <c r="F117" s="234"/>
-      <c r="G117" s="232">
+      <c r="F117" s="280"/>
+      <c r="G117" s="278">
         <v>44167</v>
       </c>
-      <c r="H117" s="233"/>
-      <c r="I117" s="234"/>
+      <c r="H117" s="279"/>
+      <c r="I117" s="280"/>
     </row>
     <row r="118" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B118" s="232">
+      <c r="B118" s="278">
         <v>43992</v>
       </c>
-      <c r="C118" s="233"/>
-      <c r="D118" s="234"/>
-      <c r="E118" s="235"/>
-      <c r="F118" s="236"/>
-      <c r="G118" s="232">
+      <c r="C118" s="279"/>
+      <c r="D118" s="280"/>
+      <c r="E118" s="273"/>
+      <c r="F118" s="274"/>
+      <c r="G118" s="278">
         <v>44175</v>
       </c>
-      <c r="H118" s="233"/>
-      <c r="I118" s="234"/>
+      <c r="H118" s="279"/>
+      <c r="I118" s="280"/>
     </row>
     <row r="119" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="244" t="s">
+      <c r="A119" s="308" t="s">
         <v>194</v>
       </c>
-      <c r="B119" s="245"/>
-      <c r="C119" s="245"/>
-      <c r="D119" s="245"/>
-      <c r="E119" s="245"/>
-      <c r="F119" s="245"/>
-      <c r="G119" s="245"/>
-      <c r="H119" s="245"/>
-      <c r="I119" s="246"/>
+      <c r="B119" s="309"/>
+      <c r="C119" s="309"/>
+      <c r="D119" s="309"/>
+      <c r="E119" s="309"/>
+      <c r="F119" s="309"/>
+      <c r="G119" s="309"/>
+      <c r="H119" s="309"/>
+      <c r="I119" s="310"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="191"/>
-      <c r="B120" s="193"/>
-      <c r="C120" s="193"/>
-      <c r="D120" s="193"/>
-      <c r="E120" s="193"/>
-      <c r="F120" s="193"/>
-      <c r="G120" s="193"/>
-      <c r="H120" s="193"/>
-      <c r="I120" s="192"/>
+      <c r="A120" s="210"/>
+      <c r="B120" s="211"/>
+      <c r="C120" s="211"/>
+      <c r="D120" s="211"/>
+      <c r="E120" s="211"/>
+      <c r="F120" s="211"/>
+      <c r="G120" s="211"/>
+      <c r="H120" s="211"/>
+      <c r="I120" s="212"/>
     </row>
     <row r="121" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="243" t="s">
+      <c r="A121" s="197" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="243"/>
-      <c r="C121" s="243"/>
-      <c r="D121" s="243"/>
-      <c r="E121" s="243"/>
-      <c r="F121" s="243"/>
-      <c r="G121" s="243"/>
-      <c r="H121" s="243"/>
-      <c r="I121" s="243"/>
+      <c r="B121" s="197"/>
+      <c r="C121" s="197"/>
+      <c r="D121" s="197"/>
+      <c r="E121" s="197"/>
+      <c r="F121" s="197"/>
+      <c r="G121" s="197"/>
+      <c r="H121" s="197"/>
+      <c r="I121" s="197"/>
     </row>
     <row r="122" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="195" t="s">
+      <c r="A122" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B122" s="197" t="s">
+      <c r="B122" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C122" s="198"/>
-      <c r="D122" s="199"/>
-      <c r="E122" s="200" t="s">
+      <c r="C122" s="202"/>
+      <c r="D122" s="203"/>
+      <c r="E122" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F122" s="201"/>
-      <c r="G122" s="202" t="s">
+      <c r="F122" s="205"/>
+      <c r="G122" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H122" s="203"/>
-      <c r="I122" s="204"/>
+      <c r="H122" s="207"/>
+      <c r="I122" s="208"/>
     </row>
     <row r="123" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="196"/>
+      <c r="A123" s="200"/>
       <c r="B123" s="48" t="s">
         <v>113</v>
       </c>
@@ -6948,58 +6948,58 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" s="194" t="s">
+      <c r="A127" s="209" t="s">
         <v>154</v>
       </c>
-      <c r="B127" s="194"/>
-      <c r="C127" s="194"/>
-      <c r="D127" s="194"/>
-      <c r="E127" s="194"/>
-      <c r="F127" s="194"/>
-      <c r="G127" s="194"/>
-      <c r="H127" s="194"/>
-      <c r="I127" s="194"/>
+      <c r="B127" s="209"/>
+      <c r="C127" s="209"/>
+      <c r="D127" s="209"/>
+      <c r="E127" s="209"/>
+      <c r="F127" s="209"/>
+      <c r="G127" s="209"/>
+      <c r="H127" s="209"/>
+      <c r="I127" s="209"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="191"/>
-      <c r="B128" s="193"/>
-      <c r="C128" s="193"/>
-      <c r="D128" s="193"/>
-      <c r="E128" s="193"/>
-      <c r="F128" s="193"/>
-      <c r="G128" s="193"/>
-      <c r="H128" s="193"/>
-      <c r="I128" s="192"/>
+      <c r="A128" s="210"/>
+      <c r="B128" s="211"/>
+      <c r="C128" s="211"/>
+      <c r="D128" s="211"/>
+      <c r="E128" s="211"/>
+      <c r="F128" s="211"/>
+      <c r="G128" s="211"/>
+      <c r="H128" s="211"/>
+      <c r="I128" s="212"/>
     </row>
     <row r="129" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="243" t="s">
+      <c r="A129" s="197" t="s">
         <v>78</v>
       </c>
-      <c r="B129" s="243"/>
-      <c r="C129" s="243"/>
-      <c r="D129" s="243"/>
-      <c r="E129" s="243"/>
-      <c r="F129" s="243"/>
-      <c r="G129" s="243"/>
-      <c r="H129" s="243"/>
-      <c r="I129" s="243"/>
+      <c r="B129" s="197"/>
+      <c r="C129" s="197"/>
+      <c r="D129" s="197"/>
+      <c r="E129" s="197"/>
+      <c r="F129" s="197"/>
+      <c r="G129" s="197"/>
+      <c r="H129" s="197"/>
+      <c r="I129" s="197"/>
     </row>
     <row r="130" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="47"/>
-      <c r="B130" s="197" t="s">
+      <c r="B130" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C130" s="198"/>
-      <c r="D130" s="199"/>
-      <c r="E130" s="200" t="s">
+      <c r="C130" s="202"/>
+      <c r="D130" s="203"/>
+      <c r="E130" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F130" s="201"/>
-      <c r="G130" s="202" t="s">
+      <c r="F130" s="205"/>
+      <c r="G130" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H130" s="203"/>
-      <c r="I130" s="204"/>
+      <c r="H130" s="207"/>
+      <c r="I130" s="208"/>
     </row>
     <row r="131" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="25" t="s">
@@ -7037,19 +7037,19 @@
       <c r="D132" s="15">
         <v>43931</v>
       </c>
-      <c r="E132" s="247"/>
-      <c r="F132" s="247"/>
-      <c r="G132" s="248"/>
-      <c r="H132" s="228"/>
-      <c r="I132" s="249"/>
+      <c r="E132" s="233"/>
+      <c r="F132" s="233"/>
+      <c r="G132" s="295"/>
+      <c r="H132" s="296"/>
+      <c r="I132" s="297"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C133" s="15"/>
-      <c r="E133" s="247"/>
-      <c r="F133" s="247"/>
+      <c r="E133" s="233"/>
+      <c r="F133" s="233"/>
       <c r="G133" s="15">
         <v>44117</v>
       </c>
@@ -7091,8 +7091,8 @@
       <c r="B136" s="70"/>
       <c r="C136" s="14"/>
       <c r="D136" s="70"/>
-      <c r="E136" s="209"/>
-      <c r="F136" s="209"/>
+      <c r="E136" s="232"/>
+      <c r="F136" s="232"/>
       <c r="G136" s="69"/>
       <c r="H136" s="69"/>
       <c r="I136" s="69"/>
@@ -7175,17 +7175,17 @@
       <c r="I141" s="15"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" s="194" t="s">
+      <c r="A142" s="209" t="s">
         <v>140</v>
       </c>
-      <c r="B142" s="194"/>
-      <c r="C142" s="194"/>
-      <c r="D142" s="194"/>
-      <c r="E142" s="194"/>
-      <c r="F142" s="194"/>
-      <c r="G142" s="194"/>
-      <c r="H142" s="194"/>
-      <c r="I142" s="194"/>
+      <c r="B142" s="209"/>
+      <c r="C142" s="209"/>
+      <c r="D142" s="209"/>
+      <c r="E142" s="209"/>
+      <c r="F142" s="209"/>
+      <c r="G142" s="209"/>
+      <c r="H142" s="209"/>
+      <c r="I142" s="209"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="27"/>
@@ -7199,52 +7199,52 @@
       <c r="I143" s="27"/>
     </row>
     <row r="144" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="237" t="s">
+      <c r="A144" s="321" t="s">
         <v>90</v>
       </c>
-      <c r="B144" s="237"/>
-      <c r="C144" s="237"/>
-      <c r="D144" s="237"/>
-      <c r="E144" s="237"/>
-      <c r="F144" s="237"/>
-      <c r="G144" s="237"/>
-      <c r="H144" s="237"/>
-      <c r="I144" s="237"/>
+      <c r="B144" s="321"/>
+      <c r="C144" s="321"/>
+      <c r="D144" s="321"/>
+      <c r="E144" s="321"/>
+      <c r="F144" s="321"/>
+      <c r="G144" s="321"/>
+      <c r="H144" s="321"/>
+      <c r="I144" s="321"/>
     </row>
     <row r="145" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="197" t="s">
+      <c r="A145" s="201" t="s">
         <v>152</v>
       </c>
-      <c r="B145" s="198"/>
-      <c r="C145" s="198"/>
-      <c r="D145" s="198"/>
-      <c r="E145" s="198"/>
-      <c r="F145" s="198"/>
-      <c r="G145" s="198"/>
-      <c r="H145" s="198"/>
-      <c r="I145" s="199"/>
+      <c r="B145" s="202"/>
+      <c r="C145" s="202"/>
+      <c r="D145" s="202"/>
+      <c r="E145" s="202"/>
+      <c r="F145" s="202"/>
+      <c r="G145" s="202"/>
+      <c r="H145" s="202"/>
+      <c r="I145" s="203"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A146" s="238" t="s">
+      <c r="A146" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B146" s="218" t="s">
+      <c r="B146" s="256" t="s">
         <v>116</v>
       </c>
-      <c r="C146" s="220"/>
-      <c r="D146" s="221"/>
-      <c r="E146" s="222" t="s">
+      <c r="C146" s="257"/>
+      <c r="D146" s="258"/>
+      <c r="E146" s="320" t="s">
         <v>115</v>
       </c>
-      <c r="F146" s="223"/>
-      <c r="G146" s="224" t="s">
+      <c r="F146" s="314"/>
+      <c r="G146" s="315" t="s">
         <v>114</v>
       </c>
-      <c r="H146" s="225"/>
-      <c r="I146" s="226"/>
+      <c r="H146" s="316"/>
+      <c r="I146" s="317"/>
     </row>
     <row r="147" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="239"/>
+      <c r="A147" s="219"/>
       <c r="B147" s="64" t="s">
         <v>149</v>
       </c>
@@ -7322,22 +7322,22 @@
       <c r="A152" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B152" s="191"/>
-      <c r="C152" s="193"/>
-      <c r="D152" s="192"/>
-      <c r="E152" s="191"/>
-      <c r="F152" s="192"/>
-      <c r="G152" s="191"/>
-      <c r="H152" s="193"/>
-      <c r="I152" s="192"/>
+      <c r="B152" s="210"/>
+      <c r="C152" s="211"/>
+      <c r="D152" s="212"/>
+      <c r="E152" s="210"/>
+      <c r="F152" s="212"/>
+      <c r="G152" s="210"/>
+      <c r="H152" s="211"/>
+      <c r="I152" s="212"/>
     </row>
     <row r="153" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B153" s="191"/>
-      <c r="C153" s="193"/>
-      <c r="D153" s="192"/>
+      <c r="B153" s="210"/>
+      <c r="C153" s="211"/>
+      <c r="D153" s="212"/>
       <c r="E153" s="15"/>
       <c r="F153" s="15"/>
       <c r="G153" s="15"/>
@@ -7348,14 +7348,14 @@
       <c r="A154" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B154" s="191"/>
-      <c r="C154" s="193"/>
-      <c r="D154" s="192"/>
-      <c r="E154" s="191"/>
-      <c r="F154" s="192"/>
-      <c r="G154" s="191"/>
-      <c r="H154" s="193"/>
-      <c r="I154" s="192"/>
+      <c r="B154" s="210"/>
+      <c r="C154" s="211"/>
+      <c r="D154" s="212"/>
+      <c r="E154" s="210"/>
+      <c r="F154" s="212"/>
+      <c r="G154" s="210"/>
+      <c r="H154" s="211"/>
+      <c r="I154" s="212"/>
     </row>
     <row r="155" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
@@ -7387,14 +7387,14 @@
       <c r="A157" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B157" s="191"/>
-      <c r="C157" s="193"/>
-      <c r="D157" s="192"/>
-      <c r="E157" s="191"/>
-      <c r="F157" s="192"/>
-      <c r="G157" s="191"/>
-      <c r="H157" s="193"/>
-      <c r="I157" s="192"/>
+      <c r="B157" s="210"/>
+      <c r="C157" s="211"/>
+      <c r="D157" s="212"/>
+      <c r="E157" s="210"/>
+      <c r="F157" s="212"/>
+      <c r="G157" s="210"/>
+      <c r="H157" s="211"/>
+      <c r="I157" s="212"/>
     </row>
     <row r="158" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
@@ -7410,39 +7410,39 @@
       <c r="I158" s="66"/>
     </row>
     <row r="159" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="197" t="s">
+      <c r="A159" s="201" t="s">
         <v>151</v>
       </c>
-      <c r="B159" s="198"/>
-      <c r="C159" s="198"/>
-      <c r="D159" s="198"/>
-      <c r="E159" s="198"/>
-      <c r="F159" s="198"/>
-      <c r="G159" s="198"/>
-      <c r="H159" s="198"/>
-      <c r="I159" s="199"/>
+      <c r="B159" s="202"/>
+      <c r="C159" s="202"/>
+      <c r="D159" s="202"/>
+      <c r="E159" s="202"/>
+      <c r="F159" s="202"/>
+      <c r="G159" s="202"/>
+      <c r="H159" s="202"/>
+      <c r="I159" s="203"/>
     </row>
     <row r="160" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="218" t="s">
+      <c r="A160" s="256" t="s">
         <v>117</v>
       </c>
-      <c r="B160" s="218" t="s">
+      <c r="B160" s="256" t="s">
         <v>116</v>
       </c>
-      <c r="C160" s="220"/>
-      <c r="D160" s="221"/>
-      <c r="E160" s="222" t="s">
+      <c r="C160" s="257"/>
+      <c r="D160" s="258"/>
+      <c r="E160" s="320" t="s">
         <v>115</v>
       </c>
-      <c r="F160" s="223"/>
-      <c r="G160" s="224" t="s">
+      <c r="F160" s="314"/>
+      <c r="G160" s="315" t="s">
         <v>114</v>
       </c>
-      <c r="H160" s="225"/>
-      <c r="I160" s="226"/>
+      <c r="H160" s="316"/>
+      <c r="I160" s="317"/>
     </row>
     <row r="161" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="219"/>
+      <c r="A161" s="323"/>
       <c r="B161" s="63" t="s">
         <v>149</v>
       </c>
@@ -7520,22 +7520,22 @@
       <c r="A166" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B166" s="191"/>
-      <c r="C166" s="193"/>
-      <c r="D166" s="192"/>
-      <c r="E166" s="191"/>
-      <c r="F166" s="192"/>
-      <c r="G166" s="191"/>
-      <c r="H166" s="193"/>
-      <c r="I166" s="192"/>
+      <c r="B166" s="210"/>
+      <c r="C166" s="211"/>
+      <c r="D166" s="212"/>
+      <c r="E166" s="210"/>
+      <c r="F166" s="212"/>
+      <c r="G166" s="210"/>
+      <c r="H166" s="211"/>
+      <c r="I166" s="212"/>
     </row>
     <row r="167" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B167" s="191"/>
-      <c r="C167" s="193"/>
-      <c r="D167" s="192"/>
+      <c r="B167" s="210"/>
+      <c r="C167" s="211"/>
+      <c r="D167" s="212"/>
       <c r="E167" s="15"/>
       <c r="F167" s="15"/>
       <c r="G167" s="15"/>
@@ -7546,14 +7546,14 @@
       <c r="A168" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B168" s="191"/>
-      <c r="C168" s="193"/>
-      <c r="D168" s="192"/>
-      <c r="E168" s="191"/>
-      <c r="F168" s="192"/>
-      <c r="G168" s="191"/>
-      <c r="H168" s="193"/>
-      <c r="I168" s="192"/>
+      <c r="B168" s="210"/>
+      <c r="C168" s="211"/>
+      <c r="D168" s="212"/>
+      <c r="E168" s="210"/>
+      <c r="F168" s="212"/>
+      <c r="G168" s="210"/>
+      <c r="H168" s="211"/>
+      <c r="I168" s="212"/>
     </row>
     <row r="169" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
@@ -7572,14 +7572,14 @@
       <c r="A170" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B170" s="191"/>
-      <c r="C170" s="193"/>
-      <c r="D170" s="192"/>
-      <c r="E170" s="191"/>
-      <c r="F170" s="192"/>
-      <c r="G170" s="191"/>
-      <c r="H170" s="193"/>
-      <c r="I170" s="192"/>
+      <c r="B170" s="210"/>
+      <c r="C170" s="211"/>
+      <c r="D170" s="212"/>
+      <c r="E170" s="210"/>
+      <c r="F170" s="212"/>
+      <c r="G170" s="210"/>
+      <c r="H170" s="211"/>
+      <c r="I170" s="212"/>
     </row>
     <row r="171" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
@@ -7595,39 +7595,39 @@
       <c r="I171" s="65"/>
     </row>
     <row r="172" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="197" t="s">
+      <c r="A172" s="201" t="s">
         <v>150</v>
       </c>
-      <c r="B172" s="198"/>
-      <c r="C172" s="198"/>
-      <c r="D172" s="198"/>
-      <c r="E172" s="198"/>
-      <c r="F172" s="198"/>
-      <c r="G172" s="198"/>
-      <c r="H172" s="198"/>
-      <c r="I172" s="199"/>
+      <c r="B172" s="202"/>
+      <c r="C172" s="202"/>
+      <c r="D172" s="202"/>
+      <c r="E172" s="202"/>
+      <c r="F172" s="202"/>
+      <c r="G172" s="202"/>
+      <c r="H172" s="202"/>
+      <c r="I172" s="203"/>
     </row>
     <row r="173" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="218" t="s">
+      <c r="A173" s="256" t="s">
         <v>117</v>
       </c>
-      <c r="B173" s="218" t="s">
+      <c r="B173" s="256" t="s">
         <v>116</v>
       </c>
-      <c r="C173" s="220"/>
-      <c r="D173" s="221"/>
-      <c r="E173" s="242" t="s">
+      <c r="C173" s="257"/>
+      <c r="D173" s="258"/>
+      <c r="E173" s="313" t="s">
         <v>115</v>
       </c>
-      <c r="F173" s="223"/>
-      <c r="G173" s="224" t="s">
+      <c r="F173" s="314"/>
+      <c r="G173" s="315" t="s">
         <v>114</v>
       </c>
-      <c r="H173" s="225"/>
-      <c r="I173" s="226"/>
+      <c r="H173" s="316"/>
+      <c r="I173" s="317"/>
     </row>
     <row r="174" spans="1:9" s="53" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="219"/>
+      <c r="A174" s="323"/>
       <c r="B174" s="64" t="s">
         <v>149</v>
       </c>
@@ -7705,22 +7705,22 @@
       <c r="A179" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B179" s="191"/>
-      <c r="C179" s="193"/>
-      <c r="D179" s="192"/>
-      <c r="E179" s="191"/>
-      <c r="F179" s="192"/>
-      <c r="G179" s="191"/>
-      <c r="H179" s="193"/>
-      <c r="I179" s="192"/>
+      <c r="B179" s="210"/>
+      <c r="C179" s="211"/>
+      <c r="D179" s="212"/>
+      <c r="E179" s="210"/>
+      <c r="F179" s="212"/>
+      <c r="G179" s="210"/>
+      <c r="H179" s="211"/>
+      <c r="I179" s="212"/>
     </row>
     <row r="180" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B180" s="191"/>
-      <c r="C180" s="193"/>
-      <c r="D180" s="192"/>
+      <c r="B180" s="210"/>
+      <c r="C180" s="211"/>
+      <c r="D180" s="212"/>
       <c r="E180" s="15"/>
       <c r="F180" s="15"/>
       <c r="G180" s="56"/>
@@ -7731,14 +7731,14 @@
       <c r="A181" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B181" s="191"/>
-      <c r="C181" s="193"/>
-      <c r="D181" s="192"/>
-      <c r="E181" s="191"/>
-      <c r="F181" s="192"/>
-      <c r="G181" s="191"/>
-      <c r="H181" s="193"/>
-      <c r="I181" s="192"/>
+      <c r="B181" s="210"/>
+      <c r="C181" s="211"/>
+      <c r="D181" s="212"/>
+      <c r="E181" s="210"/>
+      <c r="F181" s="212"/>
+      <c r="G181" s="210"/>
+      <c r="H181" s="211"/>
+      <c r="I181" s="212"/>
     </row>
     <row r="182" spans="1:9" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
@@ -7757,14 +7757,14 @@
       <c r="A183" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B183" s="191"/>
-      <c r="C183" s="193"/>
-      <c r="D183" s="192"/>
-      <c r="E183" s="191"/>
-      <c r="F183" s="192"/>
-      <c r="G183" s="191"/>
-      <c r="H183" s="193"/>
-      <c r="I183" s="192"/>
+      <c r="B183" s="210"/>
+      <c r="C183" s="211"/>
+      <c r="D183" s="212"/>
+      <c r="E183" s="210"/>
+      <c r="F183" s="212"/>
+      <c r="G183" s="210"/>
+      <c r="H183" s="211"/>
+      <c r="I183" s="212"/>
     </row>
     <row r="184" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
@@ -7780,74 +7780,74 @@
       <c r="I184" s="15"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A185" s="229" t="s">
+      <c r="A185" s="322" t="s">
         <v>147</v>
       </c>
-      <c r="B185" s="229"/>
-      <c r="C185" s="229"/>
-      <c r="D185" s="229"/>
-      <c r="E185" s="229"/>
-      <c r="F185" s="229"/>
-      <c r="G185" s="229"/>
-      <c r="H185" s="229"/>
-      <c r="I185" s="229"/>
+      <c r="B185" s="322"/>
+      <c r="C185" s="322"/>
+      <c r="D185" s="322"/>
+      <c r="E185" s="322"/>
+      <c r="F185" s="322"/>
+      <c r="G185" s="322"/>
+      <c r="H185" s="322"/>
+      <c r="I185" s="322"/>
     </row>
     <row r="186" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="227"/>
-      <c r="B186" s="227"/>
-      <c r="C186" s="227"/>
-      <c r="D186" s="227"/>
-      <c r="E186" s="227"/>
-      <c r="F186" s="227"/>
-      <c r="G186" s="227"/>
-      <c r="H186" s="227"/>
-      <c r="I186" s="227"/>
+      <c r="A186" s="324"/>
+      <c r="B186" s="324"/>
+      <c r="C186" s="324"/>
+      <c r="D186" s="324"/>
+      <c r="E186" s="324"/>
+      <c r="F186" s="324"/>
+      <c r="G186" s="324"/>
+      <c r="H186" s="324"/>
+      <c r="I186" s="324"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A187" s="228"/>
-      <c r="B187" s="228"/>
-      <c r="C187" s="228"/>
-      <c r="D187" s="228"/>
-      <c r="E187" s="228"/>
-      <c r="F187" s="228"/>
-      <c r="G187" s="228"/>
-      <c r="H187" s="228"/>
-      <c r="I187" s="228"/>
+      <c r="A187" s="296"/>
+      <c r="B187" s="296"/>
+      <c r="C187" s="296"/>
+      <c r="D187" s="296"/>
+      <c r="E187" s="296"/>
+      <c r="F187" s="296"/>
+      <c r="G187" s="296"/>
+      <c r="H187" s="296"/>
+      <c r="I187" s="296"/>
     </row>
     <row r="188" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="205" t="s">
+      <c r="A188" s="226" t="s">
         <v>101</v>
       </c>
-      <c r="B188" s="206"/>
-      <c r="C188" s="206"/>
-      <c r="D188" s="206"/>
-      <c r="E188" s="206"/>
-      <c r="F188" s="206"/>
-      <c r="G188" s="206"/>
-      <c r="H188" s="206"/>
-      <c r="I188" s="207"/>
+      <c r="B188" s="227"/>
+      <c r="C188" s="227"/>
+      <c r="D188" s="227"/>
+      <c r="E188" s="227"/>
+      <c r="F188" s="227"/>
+      <c r="G188" s="227"/>
+      <c r="H188" s="227"/>
+      <c r="I188" s="228"/>
     </row>
     <row r="189" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="195" t="s">
+      <c r="A189" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B189" s="197" t="s">
+      <c r="B189" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C189" s="198"/>
-      <c r="D189" s="199"/>
-      <c r="E189" s="200" t="s">
+      <c r="C189" s="202"/>
+      <c r="D189" s="203"/>
+      <c r="E189" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F189" s="201"/>
-      <c r="G189" s="202" t="s">
+      <c r="F189" s="205"/>
+      <c r="G189" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H189" s="203"/>
-      <c r="I189" s="204"/>
+      <c r="H189" s="207"/>
+      <c r="I189" s="208"/>
     </row>
     <row r="190" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="196"/>
+      <c r="A190" s="200"/>
       <c r="B190" s="25" t="s">
         <v>113</v>
       </c>
@@ -7873,130 +7873,130 @@
       <c r="A191" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B191" s="209"/>
-      <c r="C191" s="209"/>
-      <c r="D191" s="209"/>
-      <c r="E191" s="230"/>
-      <c r="F191" s="231"/>
-      <c r="G191" s="209"/>
-      <c r="H191" s="209"/>
-      <c r="I191" s="209"/>
+      <c r="B191" s="232"/>
+      <c r="C191" s="232"/>
+      <c r="D191" s="232"/>
+      <c r="E191" s="318"/>
+      <c r="F191" s="319"/>
+      <c r="G191" s="232"/>
+      <c r="H191" s="232"/>
+      <c r="I191" s="232"/>
     </row>
     <row r="192" spans="1:9" ht="81" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B192" s="209">
+      <c r="B192" s="232">
         <v>43905</v>
       </c>
-      <c r="C192" s="209"/>
-      <c r="D192" s="209"/>
-      <c r="E192" s="230"/>
-      <c r="F192" s="231"/>
-      <c r="G192" s="209">
+      <c r="C192" s="232"/>
+      <c r="D192" s="232"/>
+      <c r="E192" s="318"/>
+      <c r="F192" s="319"/>
+      <c r="G192" s="232">
         <v>44094</v>
       </c>
-      <c r="H192" s="209"/>
-      <c r="I192" s="209"/>
+      <c r="H192" s="232"/>
+      <c r="I192" s="232"/>
     </row>
     <row r="193" spans="1:9" s="50" customFormat="1" ht="81" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B193" s="209">
+      <c r="B193" s="232">
         <v>43898</v>
       </c>
-      <c r="C193" s="209"/>
-      <c r="D193" s="209"/>
-      <c r="E193" s="210"/>
-      <c r="F193" s="211"/>
-      <c r="G193" s="209">
+      <c r="C193" s="232"/>
+      <c r="D193" s="232"/>
+      <c r="E193" s="325"/>
+      <c r="F193" s="326"/>
+      <c r="G193" s="232">
         <v>44080</v>
       </c>
-      <c r="H193" s="209"/>
-      <c r="I193" s="209"/>
+      <c r="H193" s="232"/>
+      <c r="I193" s="232"/>
     </row>
     <row r="194" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A194" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B194" s="212"/>
-      <c r="C194" s="213"/>
-      <c r="D194" s="214"/>
-      <c r="E194" s="212"/>
-      <c r="F194" s="214"/>
-      <c r="G194" s="215"/>
-      <c r="H194" s="216"/>
-      <c r="I194" s="217"/>
+      <c r="B194" s="191"/>
+      <c r="C194" s="192"/>
+      <c r="D194" s="193"/>
+      <c r="E194" s="191"/>
+      <c r="F194" s="193"/>
+      <c r="G194" s="292"/>
+      <c r="H194" s="293"/>
+      <c r="I194" s="294"/>
     </row>
     <row r="195" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B195" s="212"/>
-      <c r="C195" s="213"/>
-      <c r="D195" s="214"/>
-      <c r="E195" s="212"/>
-      <c r="F195" s="214"/>
-      <c r="G195" s="215"/>
-      <c r="H195" s="216"/>
-      <c r="I195" s="217"/>
+      <c r="B195" s="191"/>
+      <c r="C195" s="192"/>
+      <c r="D195" s="193"/>
+      <c r="E195" s="191"/>
+      <c r="F195" s="193"/>
+      <c r="G195" s="292"/>
+      <c r="H195" s="293"/>
+      <c r="I195" s="294"/>
     </row>
     <row r="196" spans="1:9" s="50" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B196" s="212"/>
-      <c r="C196" s="213"/>
-      <c r="D196" s="214"/>
-      <c r="E196" s="212"/>
-      <c r="F196" s="214"/>
-      <c r="G196" s="215"/>
-      <c r="H196" s="216"/>
-      <c r="I196" s="217"/>
+      <c r="B196" s="191"/>
+      <c r="C196" s="192"/>
+      <c r="D196" s="193"/>
+      <c r="E196" s="191"/>
+      <c r="F196" s="193"/>
+      <c r="G196" s="292"/>
+      <c r="H196" s="293"/>
+      <c r="I196" s="294"/>
     </row>
     <row r="197" spans="1:9" s="50" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B197" s="209">
+      <c r="B197" s="232">
         <v>43905</v>
       </c>
-      <c r="C197" s="209"/>
-      <c r="D197" s="209"/>
+      <c r="C197" s="232"/>
+      <c r="D197" s="232"/>
       <c r="E197" s="52"/>
       <c r="F197" s="51"/>
-      <c r="G197" s="209">
+      <c r="G197" s="232">
         <v>44094</v>
       </c>
-      <c r="H197" s="209"/>
-      <c r="I197" s="209"/>
+      <c r="H197" s="232"/>
+      <c r="I197" s="232"/>
     </row>
     <row r="198" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B198" s="212"/>
-      <c r="C198" s="213"/>
-      <c r="D198" s="214"/>
-      <c r="E198" s="212"/>
-      <c r="F198" s="214"/>
-      <c r="G198" s="215"/>
-      <c r="H198" s="216"/>
-      <c r="I198" s="217"/>
+      <c r="B198" s="191"/>
+      <c r="C198" s="192"/>
+      <c r="D198" s="193"/>
+      <c r="E198" s="191"/>
+      <c r="F198" s="193"/>
+      <c r="G198" s="292"/>
+      <c r="H198" s="293"/>
+      <c r="I198" s="294"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" s="208" t="s">
+      <c r="A199" s="225" t="s">
         <v>140</v>
       </c>
-      <c r="B199" s="208"/>
-      <c r="C199" s="208"/>
-      <c r="D199" s="208"/>
-      <c r="E199" s="208"/>
-      <c r="F199" s="208"/>
-      <c r="G199" s="208"/>
-      <c r="H199" s="208"/>
-      <c r="I199" s="208"/>
+      <c r="B199" s="225"/>
+      <c r="C199" s="225"/>
+      <c r="D199" s="225"/>
+      <c r="E199" s="225"/>
+      <c r="F199" s="225"/>
+      <c r="G199" s="225"/>
+      <c r="H199" s="225"/>
+      <c r="I199" s="225"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="49"/>
@@ -8010,61 +8010,61 @@
       <c r="I200" s="49"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" s="258"/>
-      <c r="B201" s="258"/>
-      <c r="C201" s="258"/>
-      <c r="D201" s="258"/>
-      <c r="E201" s="258"/>
-      <c r="F201" s="258"/>
-      <c r="G201" s="258"/>
-      <c r="H201" s="258"/>
-      <c r="I201" s="258"/>
+      <c r="A201" s="298"/>
+      <c r="B201" s="298"/>
+      <c r="C201" s="298"/>
+      <c r="D201" s="298"/>
+      <c r="E201" s="298"/>
+      <c r="F201" s="298"/>
+      <c r="G201" s="298"/>
+      <c r="H201" s="298"/>
+      <c r="I201" s="298"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="259"/>
-      <c r="B202" s="260"/>
-      <c r="C202" s="260"/>
-      <c r="D202" s="260"/>
-      <c r="E202" s="260"/>
-      <c r="F202" s="260"/>
-      <c r="G202" s="260"/>
-      <c r="H202" s="260"/>
-      <c r="I202" s="261"/>
+      <c r="A202" s="299"/>
+      <c r="B202" s="300"/>
+      <c r="C202" s="300"/>
+      <c r="D202" s="300"/>
+      <c r="E202" s="300"/>
+      <c r="F202" s="300"/>
+      <c r="G202" s="300"/>
+      <c r="H202" s="300"/>
+      <c r="I202" s="301"/>
     </row>
     <row r="203" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="205" t="s">
+      <c r="A203" s="226" t="s">
         <v>146</v>
       </c>
-      <c r="B203" s="206"/>
-      <c r="C203" s="206"/>
-      <c r="D203" s="206"/>
-      <c r="E203" s="206"/>
-      <c r="F203" s="206"/>
-      <c r="G203" s="206"/>
-      <c r="H203" s="206"/>
-      <c r="I203" s="207"/>
+      <c r="B203" s="227"/>
+      <c r="C203" s="227"/>
+      <c r="D203" s="227"/>
+      <c r="E203" s="227"/>
+      <c r="F203" s="227"/>
+      <c r="G203" s="227"/>
+      <c r="H203" s="227"/>
+      <c r="I203" s="228"/>
     </row>
     <row r="204" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="238" t="s">
+      <c r="A204" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B204" s="197" t="s">
+      <c r="B204" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C204" s="198"/>
-      <c r="D204" s="199"/>
-      <c r="E204" s="200" t="s">
+      <c r="C204" s="202"/>
+      <c r="D204" s="203"/>
+      <c r="E204" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F204" s="201"/>
-      <c r="G204" s="202" t="s">
+      <c r="F204" s="205"/>
+      <c r="G204" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H204" s="203"/>
-      <c r="I204" s="204"/>
+      <c r="H204" s="207"/>
+      <c r="I204" s="208"/>
     </row>
     <row r="205" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="239"/>
+      <c r="A205" s="219"/>
       <c r="B205" s="25" t="s">
         <v>113</v>
       </c>
@@ -8090,117 +8090,117 @@
       <c r="A206" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B206" s="248"/>
-      <c r="C206" s="228"/>
-      <c r="D206" s="249"/>
-      <c r="E206" s="248"/>
-      <c r="F206" s="249"/>
-      <c r="G206" s="191"/>
-      <c r="H206" s="193"/>
-      <c r="I206" s="192"/>
+      <c r="B206" s="295"/>
+      <c r="C206" s="296"/>
+      <c r="D206" s="297"/>
+      <c r="E206" s="295"/>
+      <c r="F206" s="297"/>
+      <c r="G206" s="210"/>
+      <c r="H206" s="211"/>
+      <c r="I206" s="212"/>
     </row>
     <row r="207" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A207" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B207" s="191"/>
-      <c r="C207" s="193"/>
-      <c r="D207" s="192"/>
-      <c r="E207" s="191"/>
-      <c r="F207" s="192"/>
-      <c r="G207" s="191"/>
-      <c r="H207" s="193"/>
-      <c r="I207" s="192"/>
+      <c r="B207" s="210"/>
+      <c r="C207" s="211"/>
+      <c r="D207" s="212"/>
+      <c r="E207" s="210"/>
+      <c r="F207" s="212"/>
+      <c r="G207" s="210"/>
+      <c r="H207" s="211"/>
+      <c r="I207" s="212"/>
     </row>
     <row r="208" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A208" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B208" s="191"/>
-      <c r="C208" s="193"/>
-      <c r="D208" s="192"/>
-      <c r="E208" s="191"/>
-      <c r="F208" s="192"/>
-      <c r="G208" s="191"/>
-      <c r="H208" s="193"/>
-      <c r="I208" s="192"/>
+      <c r="B208" s="210"/>
+      <c r="C208" s="211"/>
+      <c r="D208" s="212"/>
+      <c r="E208" s="210"/>
+      <c r="F208" s="212"/>
+      <c r="G208" s="210"/>
+      <c r="H208" s="211"/>
+      <c r="I208" s="212"/>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B209" s="191"/>
-      <c r="C209" s="193"/>
-      <c r="D209" s="192"/>
-      <c r="E209" s="191"/>
-      <c r="F209" s="192"/>
-      <c r="G209" s="191"/>
-      <c r="H209" s="193"/>
-      <c r="I209" s="192"/>
+      <c r="B209" s="210"/>
+      <c r="C209" s="211"/>
+      <c r="D209" s="212"/>
+      <c r="E209" s="210"/>
+      <c r="F209" s="212"/>
+      <c r="G209" s="210"/>
+      <c r="H209" s="211"/>
+      <c r="I209" s="212"/>
     </row>
     <row r="210" spans="1:10" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A210" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B210" s="191"/>
-      <c r="C210" s="193"/>
-      <c r="D210" s="192"/>
-      <c r="E210" s="191"/>
-      <c r="F210" s="192"/>
-      <c r="G210" s="191"/>
-      <c r="H210" s="193"/>
-      <c r="I210" s="192"/>
+      <c r="B210" s="210"/>
+      <c r="C210" s="211"/>
+      <c r="D210" s="212"/>
+      <c r="E210" s="210"/>
+      <c r="F210" s="212"/>
+      <c r="G210" s="210"/>
+      <c r="H210" s="211"/>
+      <c r="I210" s="212"/>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A211" s="194" t="s">
+      <c r="A211" s="209" t="s">
         <v>140</v>
       </c>
-      <c r="B211" s="194"/>
-      <c r="C211" s="194"/>
-      <c r="D211" s="194"/>
-      <c r="E211" s="194"/>
-      <c r="F211" s="194"/>
-      <c r="G211" s="194"/>
-      <c r="H211" s="194"/>
-      <c r="I211" s="194"/>
+      <c r="B211" s="209"/>
+      <c r="C211" s="209"/>
+      <c r="D211" s="209"/>
+      <c r="E211" s="209"/>
+      <c r="F211" s="209"/>
+      <c r="G211" s="209"/>
+      <c r="H211" s="209"/>
+      <c r="I211" s="209"/>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" s="11"/>
     </row>
     <row r="213" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="205" t="s">
+      <c r="A213" s="226" t="s">
         <v>139</v>
       </c>
-      <c r="B213" s="206"/>
-      <c r="C213" s="206"/>
-      <c r="D213" s="206"/>
-      <c r="E213" s="206"/>
-      <c r="F213" s="206"/>
-      <c r="G213" s="206"/>
-      <c r="H213" s="206"/>
-      <c r="I213" s="207"/>
+      <c r="B213" s="227"/>
+      <c r="C213" s="227"/>
+      <c r="D213" s="227"/>
+      <c r="E213" s="227"/>
+      <c r="F213" s="227"/>
+      <c r="G213" s="227"/>
+      <c r="H213" s="227"/>
+      <c r="I213" s="228"/>
     </row>
     <row r="214" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="195" t="s">
+      <c r="A214" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B214" s="197" t="s">
+      <c r="B214" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C214" s="198"/>
-      <c r="D214" s="199"/>
-      <c r="E214" s="200" t="s">
+      <c r="C214" s="202"/>
+      <c r="D214" s="203"/>
+      <c r="E214" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F214" s="201"/>
-      <c r="G214" s="202" t="s">
+      <c r="F214" s="205"/>
+      <c r="G214" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H214" s="203"/>
-      <c r="I214" s="204"/>
+      <c r="H214" s="207"/>
+      <c r="I214" s="208"/>
     </row>
     <row r="215" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="196"/>
+      <c r="A215" s="200"/>
       <c r="B215" s="48" t="s">
         <v>113</v>
       </c>
@@ -8236,17 +8236,17 @@
       <c r="I216" s="15"/>
     </row>
     <row r="217" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="194" t="s">
+      <c r="A217" s="209" t="s">
         <v>137</v>
       </c>
-      <c r="B217" s="194"/>
-      <c r="C217" s="194"/>
-      <c r="D217" s="194"/>
-      <c r="E217" s="194"/>
-      <c r="F217" s="194"/>
-      <c r="G217" s="194"/>
-      <c r="H217" s="194"/>
-      <c r="I217" s="194"/>
+      <c r="B217" s="209"/>
+      <c r="C217" s="209"/>
+      <c r="D217" s="209"/>
+      <c r="E217" s="209"/>
+      <c r="F217" s="209"/>
+      <c r="G217" s="209"/>
+      <c r="H217" s="209"/>
+      <c r="I217" s="209"/>
     </row>
     <row r="218" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="11"/>
@@ -8254,39 +8254,39 @@
       <c r="C218" s="44"/>
     </row>
     <row r="219" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A219" s="205" t="s">
+      <c r="A219" s="226" t="s">
         <v>136</v>
       </c>
-      <c r="B219" s="206"/>
-      <c r="C219" s="206"/>
-      <c r="D219" s="206"/>
-      <c r="E219" s="206"/>
-      <c r="F219" s="206"/>
-      <c r="G219" s="206"/>
-      <c r="H219" s="206"/>
-      <c r="I219" s="207"/>
+      <c r="B219" s="227"/>
+      <c r="C219" s="227"/>
+      <c r="D219" s="227"/>
+      <c r="E219" s="227"/>
+      <c r="F219" s="227"/>
+      <c r="G219" s="227"/>
+      <c r="H219" s="227"/>
+      <c r="I219" s="228"/>
     </row>
     <row r="220" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="195" t="s">
+      <c r="A220" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B220" s="197" t="s">
+      <c r="B220" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C220" s="198"/>
-      <c r="D220" s="199"/>
-      <c r="E220" s="200" t="s">
+      <c r="C220" s="202"/>
+      <c r="D220" s="203"/>
+      <c r="E220" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F220" s="201"/>
-      <c r="G220" s="202" t="s">
+      <c r="F220" s="205"/>
+      <c r="G220" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H220" s="203"/>
-      <c r="I220" s="204"/>
+      <c r="H220" s="207"/>
+      <c r="I220" s="208"/>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A221" s="257"/>
+      <c r="A221" s="231"/>
       <c r="B221" s="33" t="s">
         <v>135</v>
       </c>
@@ -8319,8 +8319,8 @@
       <c r="D222" s="15">
         <v>43945</v>
       </c>
-      <c r="E222" s="254"/>
-      <c r="F222" s="255"/>
+      <c r="E222" s="240"/>
+      <c r="F222" s="241"/>
       <c r="G222" s="41">
         <v>44095</v>
       </c>
@@ -8340,8 +8340,8 @@
       <c r="D223" s="15">
         <v>43921</v>
       </c>
-      <c r="E223" s="254"/>
-      <c r="F223" s="255"/>
+      <c r="E223" s="240"/>
+      <c r="F223" s="241"/>
       <c r="G223" s="41">
         <v>44033</v>
       </c>
@@ -8378,39 +8378,39 @@
       <c r="I225" s="38"/>
     </row>
     <row r="226" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="205" t="s">
+      <c r="A226" s="226" t="s">
         <v>129</v>
       </c>
-      <c r="B226" s="206"/>
-      <c r="C226" s="206"/>
-      <c r="D226" s="206"/>
-      <c r="E226" s="206"/>
-      <c r="F226" s="206"/>
-      <c r="G226" s="206"/>
-      <c r="H226" s="206"/>
-      <c r="I226" s="207"/>
+      <c r="B226" s="227"/>
+      <c r="C226" s="227"/>
+      <c r="D226" s="227"/>
+      <c r="E226" s="227"/>
+      <c r="F226" s="227"/>
+      <c r="G226" s="227"/>
+      <c r="H226" s="227"/>
+      <c r="I226" s="228"/>
     </row>
     <row r="227" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A227" s="195" t="s">
+      <c r="A227" s="199" t="s">
         <v>117</v>
       </c>
-      <c r="B227" s="197" t="s">
+      <c r="B227" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C227" s="198"/>
-      <c r="D227" s="199"/>
-      <c r="E227" s="200" t="s">
+      <c r="C227" s="202"/>
+      <c r="D227" s="203"/>
+      <c r="E227" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="F227" s="201"/>
-      <c r="G227" s="202" t="s">
+      <c r="F227" s="205"/>
+      <c r="G227" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="H227" s="203"/>
-      <c r="I227" s="204"/>
+      <c r="H227" s="207"/>
+      <c r="I227" s="208"/>
     </row>
     <row r="228" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="196"/>
+      <c r="A228" s="200"/>
       <c r="B228" s="37" t="s">
         <v>113</v>
       </c>
@@ -8497,17 +8497,17 @@
       <c r="I233" s="15"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A234" s="194" t="s">
+      <c r="A234" s="209" t="s">
         <v>102</v>
       </c>
-      <c r="B234" s="194"/>
-      <c r="C234" s="194"/>
-      <c r="D234" s="194"/>
-      <c r="E234" s="194"/>
-      <c r="F234" s="194"/>
-      <c r="G234" s="194"/>
-      <c r="H234" s="194"/>
-      <c r="I234" s="194"/>
+      <c r="B234" s="209"/>
+      <c r="C234" s="209"/>
+      <c r="D234" s="209"/>
+      <c r="E234" s="209"/>
+      <c r="F234" s="209"/>
+      <c r="G234" s="209"/>
+      <c r="H234" s="209"/>
+      <c r="I234" s="209"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="11"/>
@@ -8532,35 +8532,35 @@
       <c r="I236" s="9"/>
     </row>
     <row r="237" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="250" t="s">
+      <c r="A237" s="303" t="s">
         <v>124</v>
       </c>
-      <c r="B237" s="251"/>
-      <c r="C237" s="251"/>
+      <c r="B237" s="304"/>
+      <c r="C237" s="304"/>
       <c r="D237" s="9"/>
-      <c r="E237" s="253"/>
-      <c r="F237" s="253"/>
-      <c r="G237" s="253"/>
+      <c r="E237" s="306"/>
+      <c r="F237" s="306"/>
+      <c r="G237" s="306"/>
       <c r="H237" s="9"/>
       <c r="I237" s="9"/>
     </row>
     <row r="238" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="238" t="s">
+      <c r="A238" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B238" s="197" t="s">
+      <c r="B238" s="201" t="s">
         <v>123</v>
       </c>
-      <c r="C238" s="199"/>
+      <c r="C238" s="203"/>
       <c r="D238" s="9"/>
-      <c r="E238" s="256"/>
-      <c r="F238" s="256"/>
-      <c r="G238" s="256"/>
+      <c r="E238" s="307"/>
+      <c r="F238" s="307"/>
+      <c r="G238" s="307"/>
       <c r="H238" s="9"/>
       <c r="I238" s="9"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A239" s="252"/>
+      <c r="A239" s="305"/>
       <c r="B239" s="33" t="s">
         <v>113</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>112</v>
       </c>
       <c r="D239" s="9"/>
-      <c r="E239" s="256"/>
+      <c r="E239" s="307"/>
       <c r="F239" s="32"/>
       <c r="G239" s="32"/>
       <c r="H239" s="9"/>
@@ -8643,15 +8643,15 @@
       <c r="I243" s="9"/>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A244" s="240" t="s">
+      <c r="A244" s="311" t="s">
         <v>102</v>
       </c>
-      <c r="B244" s="194"/>
-      <c r="C244" s="241"/>
+      <c r="B244" s="209"/>
+      <c r="C244" s="312"/>
       <c r="D244" s="9"/>
-      <c r="E244" s="262"/>
-      <c r="F244" s="262"/>
-      <c r="G244" s="262"/>
+      <c r="E244" s="302"/>
+      <c r="F244" s="302"/>
+      <c r="G244" s="302"/>
       <c r="H244" s="9"/>
       <c r="I244" s="9"/>
     </row>
@@ -8700,39 +8700,39 @@
       <c r="I248" s="9"/>
     </row>
     <row r="249" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="205" t="s">
+      <c r="A249" s="226" t="s">
         <v>118</v>
       </c>
-      <c r="B249" s="206"/>
-      <c r="C249" s="206"/>
-      <c r="D249" s="206"/>
-      <c r="E249" s="206"/>
-      <c r="F249" s="206"/>
-      <c r="G249" s="207"/>
+      <c r="B249" s="227"/>
+      <c r="C249" s="227"/>
+      <c r="D249" s="227"/>
+      <c r="E249" s="227"/>
+      <c r="F249" s="227"/>
+      <c r="G249" s="228"/>
       <c r="H249" s="9"/>
       <c r="I249" s="9"/>
     </row>
     <row r="250" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A250" s="238" t="s">
+      <c r="A250" s="218" t="s">
         <v>117</v>
       </c>
-      <c r="B250" s="197" t="s">
+      <c r="B250" s="201" t="s">
         <v>116</v>
       </c>
-      <c r="C250" s="199"/>
-      <c r="D250" s="200" t="s">
+      <c r="C250" s="203"/>
+      <c r="D250" s="204" t="s">
         <v>115</v>
       </c>
-      <c r="E250" s="201"/>
-      <c r="F250" s="202" t="s">
+      <c r="E250" s="205"/>
+      <c r="F250" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="G250" s="204"/>
+      <c r="G250" s="208"/>
       <c r="H250" s="9"/>
       <c r="I250" s="9"/>
     </row>
     <row r="251" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A251" s="239"/>
+      <c r="A251" s="219"/>
       <c r="B251" s="25" t="s">
         <v>113</v>
       </c>
@@ -8868,15 +8868,15 @@
       <c r="I257" s="9"/>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A258" s="208" t="s">
+      <c r="A258" s="225" t="s">
         <v>102</v>
       </c>
-      <c r="B258" s="208"/>
-      <c r="C258" s="208"/>
-      <c r="D258" s="208"/>
-      <c r="E258" s="208"/>
-      <c r="F258" s="208"/>
-      <c r="G258" s="208"/>
+      <c r="B258" s="225"/>
+      <c r="C258" s="225"/>
+      <c r="D258" s="225"/>
+      <c r="E258" s="225"/>
+      <c r="F258" s="225"/>
+      <c r="G258" s="225"/>
       <c r="H258" s="9"/>
       <c r="I258" s="9"/>
     </row>
@@ -13076,6 +13076,288 @@
     <filterColumn colId="7" showButton="0"/>
   </autoFilter>
   <mergeCells count="306">
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="G207:I207"/>
+    <mergeCell ref="A211:I211"/>
+    <mergeCell ref="A214:A215"/>
+    <mergeCell ref="B214:D214"/>
+    <mergeCell ref="E214:F214"/>
+    <mergeCell ref="G214:I214"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="G209:I209"/>
+    <mergeCell ref="A213:I213"/>
+    <mergeCell ref="B207:D207"/>
+    <mergeCell ref="A199:I199"/>
+    <mergeCell ref="B193:D193"/>
+    <mergeCell ref="E193:F193"/>
+    <mergeCell ref="G193:I193"/>
+    <mergeCell ref="B194:D194"/>
+    <mergeCell ref="E194:F194"/>
+    <mergeCell ref="G194:I194"/>
+    <mergeCell ref="E195:F195"/>
+    <mergeCell ref="G195:I195"/>
+    <mergeCell ref="B197:D197"/>
+    <mergeCell ref="G197:I197"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="E198:F198"/>
+    <mergeCell ref="G198:I198"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="A188:I188"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:D160"/>
+    <mergeCell ref="E160:F160"/>
+    <mergeCell ref="G160:I160"/>
+    <mergeCell ref="E157:F157"/>
+    <mergeCell ref="G157:I157"/>
+    <mergeCell ref="A159:I159"/>
+    <mergeCell ref="A186:I186"/>
+    <mergeCell ref="B180:D180"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="B189:D189"/>
+    <mergeCell ref="E189:F189"/>
+    <mergeCell ref="G189:I189"/>
+    <mergeCell ref="A187:I187"/>
+    <mergeCell ref="E183:F183"/>
+    <mergeCell ref="G183:I183"/>
+    <mergeCell ref="B181:D181"/>
+    <mergeCell ref="E181:F181"/>
+    <mergeCell ref="G181:I181"/>
+    <mergeCell ref="A185:I185"/>
+    <mergeCell ref="E192:F192"/>
+    <mergeCell ref="G192:I192"/>
+    <mergeCell ref="G117:I117"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="G118:I118"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="G130:I130"/>
+    <mergeCell ref="B146:D146"/>
+    <mergeCell ref="E146:F146"/>
+    <mergeCell ref="G146:I146"/>
+    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="E154:F154"/>
+    <mergeCell ref="G154:I154"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="G152:I152"/>
+    <mergeCell ref="E136:F136"/>
+    <mergeCell ref="A142:I142"/>
+    <mergeCell ref="A145:I145"/>
+    <mergeCell ref="A144:I144"/>
+    <mergeCell ref="B153:D153"/>
+    <mergeCell ref="B166:D166"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="A249:G249"/>
+    <mergeCell ref="A250:A251"/>
+    <mergeCell ref="B250:C250"/>
+    <mergeCell ref="D250:E250"/>
+    <mergeCell ref="F250:G250"/>
+    <mergeCell ref="A244:C244"/>
+    <mergeCell ref="B195:D195"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="E173:F173"/>
+    <mergeCell ref="G173:I173"/>
+    <mergeCell ref="B179:D179"/>
+    <mergeCell ref="E179:F179"/>
+    <mergeCell ref="G179:I179"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="E191:F191"/>
+    <mergeCell ref="G191:I191"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="B204:D204"/>
+    <mergeCell ref="E204:F204"/>
+    <mergeCell ref="G204:I204"/>
+    <mergeCell ref="B192:D192"/>
+    <mergeCell ref="A121:I121"/>
+    <mergeCell ref="A119:I119"/>
+    <mergeCell ref="A120:I120"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="G168:I168"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="A172:I172"/>
+    <mergeCell ref="A129:I129"/>
+    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="G132:I132"/>
+    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G122:I122"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="G166:I166"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="A127:I127"/>
+    <mergeCell ref="A128:I128"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="E170:F170"/>
+    <mergeCell ref="G170:I170"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="A234:I234"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:C238"/>
+    <mergeCell ref="E237:G237"/>
+    <mergeCell ref="E220:F220"/>
+    <mergeCell ref="G220:I220"/>
+    <mergeCell ref="E223:F223"/>
+    <mergeCell ref="A226:I226"/>
+    <mergeCell ref="A227:A228"/>
+    <mergeCell ref="B227:D227"/>
+    <mergeCell ref="E227:F227"/>
+    <mergeCell ref="G227:I227"/>
+    <mergeCell ref="F238:G238"/>
+    <mergeCell ref="E238:E239"/>
+    <mergeCell ref="G206:I206"/>
+    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="E208:F208"/>
+    <mergeCell ref="G208:I208"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="A258:G258"/>
+    <mergeCell ref="A219:I219"/>
+    <mergeCell ref="E222:F222"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="G196:I196"/>
+    <mergeCell ref="A217:I217"/>
+    <mergeCell ref="B210:D210"/>
+    <mergeCell ref="E210:F210"/>
+    <mergeCell ref="G210:I210"/>
+    <mergeCell ref="B209:D209"/>
+    <mergeCell ref="B206:D206"/>
+    <mergeCell ref="E206:F206"/>
+    <mergeCell ref="A201:I201"/>
+    <mergeCell ref="A203:I203"/>
+    <mergeCell ref="A202:I202"/>
+    <mergeCell ref="E244:G244"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="G114:I114"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="G112:I112"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="G115:I115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="G116:I116"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A97:I97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="G105:I105"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="A71:I71"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:I56"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:G24"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="B32:D32"/>
@@ -13100,288 +13382,6 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="A69:I69"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="A70:I70"/>
-    <mergeCell ref="A71:I71"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="A103:I103"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="G105:I105"/>
-    <mergeCell ref="A82:I82"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A97:I97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="A87:I87"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="A111:I111"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="G114:I114"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="G112:I112"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="G115:I115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="G116:I116"/>
-    <mergeCell ref="G206:I206"/>
-    <mergeCell ref="B208:D208"/>
-    <mergeCell ref="E208:F208"/>
-    <mergeCell ref="G208:I208"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="A258:G258"/>
-    <mergeCell ref="A219:I219"/>
-    <mergeCell ref="E222:F222"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="G196:I196"/>
-    <mergeCell ref="A217:I217"/>
-    <mergeCell ref="B210:D210"/>
-    <mergeCell ref="E210:F210"/>
-    <mergeCell ref="G210:I210"/>
-    <mergeCell ref="B209:D209"/>
-    <mergeCell ref="B206:D206"/>
-    <mergeCell ref="E206:F206"/>
-    <mergeCell ref="A201:I201"/>
-    <mergeCell ref="A203:I203"/>
-    <mergeCell ref="A202:I202"/>
-    <mergeCell ref="E244:G244"/>
-    <mergeCell ref="A234:I234"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:C238"/>
-    <mergeCell ref="E237:G237"/>
-    <mergeCell ref="E220:F220"/>
-    <mergeCell ref="G220:I220"/>
-    <mergeCell ref="E223:F223"/>
-    <mergeCell ref="A226:I226"/>
-    <mergeCell ref="A227:A228"/>
-    <mergeCell ref="B227:D227"/>
-    <mergeCell ref="E227:F227"/>
-    <mergeCell ref="G227:I227"/>
-    <mergeCell ref="F238:G238"/>
-    <mergeCell ref="E238:E239"/>
-    <mergeCell ref="A121:I121"/>
-    <mergeCell ref="A119:I119"/>
-    <mergeCell ref="A120:I120"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="G168:I168"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="A172:I172"/>
-    <mergeCell ref="A129:I129"/>
-    <mergeCell ref="E132:F132"/>
-    <mergeCell ref="G132:I132"/>
-    <mergeCell ref="E133:F133"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="G122:I122"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="G166:I166"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="A127:I127"/>
-    <mergeCell ref="A128:I128"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="E170:F170"/>
-    <mergeCell ref="G170:I170"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="A249:G249"/>
-    <mergeCell ref="A250:A251"/>
-    <mergeCell ref="B250:C250"/>
-    <mergeCell ref="D250:E250"/>
-    <mergeCell ref="F250:G250"/>
-    <mergeCell ref="A244:C244"/>
-    <mergeCell ref="B195:D195"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="E173:F173"/>
-    <mergeCell ref="G173:I173"/>
-    <mergeCell ref="B179:D179"/>
-    <mergeCell ref="E179:F179"/>
-    <mergeCell ref="G179:I179"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="E191:F191"/>
-    <mergeCell ref="G191:I191"/>
-    <mergeCell ref="A204:A205"/>
-    <mergeCell ref="B204:D204"/>
-    <mergeCell ref="E204:F204"/>
-    <mergeCell ref="G204:I204"/>
-    <mergeCell ref="B192:D192"/>
-    <mergeCell ref="E192:F192"/>
-    <mergeCell ref="G192:I192"/>
-    <mergeCell ref="G117:I117"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="G118:I118"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="G130:I130"/>
-    <mergeCell ref="B146:D146"/>
-    <mergeCell ref="E146:F146"/>
-    <mergeCell ref="G146:I146"/>
-    <mergeCell ref="B154:D154"/>
-    <mergeCell ref="E154:F154"/>
-    <mergeCell ref="G154:I154"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="E152:F152"/>
-    <mergeCell ref="G152:I152"/>
-    <mergeCell ref="E136:F136"/>
-    <mergeCell ref="A142:I142"/>
-    <mergeCell ref="A145:I145"/>
-    <mergeCell ref="A144:I144"/>
-    <mergeCell ref="B153:D153"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="B189:D189"/>
-    <mergeCell ref="E189:F189"/>
-    <mergeCell ref="G189:I189"/>
-    <mergeCell ref="A187:I187"/>
-    <mergeCell ref="E183:F183"/>
-    <mergeCell ref="G183:I183"/>
-    <mergeCell ref="B181:D181"/>
-    <mergeCell ref="E181:F181"/>
-    <mergeCell ref="G181:I181"/>
-    <mergeCell ref="A185:I185"/>
-    <mergeCell ref="A173:A174"/>
-    <mergeCell ref="A188:I188"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="B160:D160"/>
-    <mergeCell ref="E160:F160"/>
-    <mergeCell ref="G160:I160"/>
-    <mergeCell ref="E157:F157"/>
-    <mergeCell ref="G157:I157"/>
-    <mergeCell ref="A159:I159"/>
-    <mergeCell ref="A186:I186"/>
-    <mergeCell ref="B180:D180"/>
-    <mergeCell ref="A199:I199"/>
-    <mergeCell ref="B193:D193"/>
-    <mergeCell ref="E193:F193"/>
-    <mergeCell ref="G193:I193"/>
-    <mergeCell ref="B194:D194"/>
-    <mergeCell ref="E194:F194"/>
-    <mergeCell ref="G194:I194"/>
-    <mergeCell ref="E195:F195"/>
-    <mergeCell ref="G195:I195"/>
-    <mergeCell ref="B197:D197"/>
-    <mergeCell ref="G197:I197"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="E198:F198"/>
-    <mergeCell ref="G198:I198"/>
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="G207:I207"/>
-    <mergeCell ref="A211:I211"/>
-    <mergeCell ref="A214:A215"/>
-    <mergeCell ref="B214:D214"/>
-    <mergeCell ref="E214:F214"/>
-    <mergeCell ref="G214:I214"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="G209:I209"/>
-    <mergeCell ref="A213:I213"/>
-    <mergeCell ref="B207:D207"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13392,7 +13392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E82" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -13404,7 +13404,7 @@
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="64.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="76.85546875" customWidth="1"/>
     <col min="8" max="8" width="57" customWidth="1"/>
     <col min="9" max="9" width="130.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -30994,7 +30994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A61" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>